<commit_message>
Fri 26 Aug 2016 23:28 commit by king
Documentation :
- Updated README
- Updated Packet Format

Code : 
- Updated Packet size & delimiter variable
- Added Controller Packet class (wrapper for sending UDP packet to controller)

Functionality : Send actuator switch on/off packet once schedule starts.

Issues Fix :
- New Special Schedule prefilled name is Schedule 1
- User is allowed to create day schedule rule with invalid time
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Meaning</t>
   </si>
@@ -107,13 +107,16 @@
     <t xml:space="preserve">Misc </t>
   </si>
   <si>
-    <t>Separate for Data : |</t>
-  </si>
-  <si>
     <t>GWT to Server Packet Format (SSL)</t>
   </si>
   <si>
     <t>Server to GWT Packet Format (SSL)</t>
+  </si>
+  <si>
+    <t>My I'm alive packet timeout has been changed</t>
+  </si>
+  <si>
+    <t>Separate for Data : Semicolon</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -510,7 +513,7 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -521,7 +524,7 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -538,7 +541,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -547,158 +550,172 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
         <v>0</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sat 26 Aug 2016 12:57 commit by king
Functionality :
- Sensor reading storage is working now
- Actuator status reporting can be interpreted
- Sensor status reporting can be interpreted

Code :
- Added on controller report event trigger
- Added on actuator report event trigger
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>Meaning</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>Separate for Data : Semicolon</t>
+  </si>
+  <si>
+    <t>Implementation Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>To be done</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>Implemented/Planned Version</t>
   </si>
 </sst>
 </file>
@@ -456,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,14 +485,16 @@
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="5" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +510,14 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -507,8 +533,14 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -518,8 +550,14 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -535,8 +573,14 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -549,8 +593,14 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -563,13 +613,19 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -596,8 +652,14 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -613,8 +675,14 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -627,8 +695,14 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -641,13 +715,19 @@
       <c r="D14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -674,13 +754,19 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -707,13 +793,19 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Mon 29 Aug 2016 21:38 commit by king
Functionality : Added GWT Server & User checking support.

Issue Fix : Edit Regular/Special Schedule not working without changing the name
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
   <si>
     <t>Meaning</t>
   </si>
@@ -92,18 +92,6 @@
     <t>Hi, I am alive</t>
   </si>
   <si>
-    <t>SQL Statement</t>
-  </si>
-  <si>
-    <t>SQL Query Result</t>
-  </si>
-  <si>
-    <t>ArrayList&lt;Serializable []&gt;</t>
-  </si>
-  <si>
-    <t>SQL Query (CREATE, INSERT, DELETE)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Misc </t>
   </si>
   <si>
@@ -135,6 +123,27 @@
   </si>
   <si>
     <t>Implemented/Planned Version</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>UserCheckNameExists</t>
+  </si>
+  <si>
+    <t>UserCheckCredentialOK</t>
+  </si>
+  <si>
+    <t>UserRegister</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>FAILCHECK/ACTIVE/PENDING APPROVAL/DEACTIVATED</t>
+  </si>
+  <si>
+    <t>SHA-1(Password)</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +520,10 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -534,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -551,10 +560,10 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -574,10 +583,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -594,15 +603,15 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -614,10 +623,10 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,10 +662,10 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,10 +685,10 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -696,10 +705,10 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,15 +725,15 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -746,68 +755,103 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
         <v>3</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="H22" t="s">
-        <v>35</v>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue 30 Aug 2016 00:23 commit by king
Added some packet formats for GWT server
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>Meaning</t>
   </si>
@@ -140,10 +140,67 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>FAILCHECK/ACTIVE/PENDING APPROVAL/DEACTIVATED</t>
-  </si>
-  <si>
     <t>SHA-1(Password)</t>
+  </si>
+  <si>
+    <t>INVALID/ACTIVE/PENDING APPROVAL/DEACTIVATED</t>
+  </si>
+  <si>
+    <t>SiteGetList</t>
+  </si>
+  <si>
+    <t>SiteGetControllers</t>
+  </si>
+  <si>
+    <t>Sitename</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object[]&gt;</t>
+  </si>
+  <si>
+    <t>ControllerGetSensors</t>
+  </si>
+  <si>
+    <t>ControllerName</t>
+  </si>
+  <si>
+    <t>ControllerGetActuators</t>
+  </si>
+  <si>
+    <t>Object[] returned is in same sequence with the CreateTableSQL</t>
+  </si>
+  <si>
+    <t>DayScheduleRuleGet</t>
+  </si>
+  <si>
+    <t>RuleName</t>
+  </si>
+  <si>
+    <t>DayScheduleRuleGetList (Return all rule names)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String[]&gt;</t>
+  </si>
+  <si>
+    <t>DayScheduleRuleSetTime</t>
+  </si>
+  <si>
+    <t>StartHour</t>
+  </si>
+  <si>
+    <t>StartMinute</t>
+  </si>
+  <si>
+    <t>Data 5</t>
+  </si>
+  <si>
+    <t>Data 6</t>
+  </si>
+  <si>
+    <t>EndHour</t>
+  </si>
+  <si>
+    <t>EndMinute</t>
   </si>
 </sst>
 </file>
@@ -483,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,106 +809,260 @@
       <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thu 1 Sep 2016 12:12 commit by king
PacketFormat : Added more formats

Files : Restored Reading

Functionality : Added scheduling related packet formats
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="124">
   <si>
     <t>Meaning</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Priority (int)</t>
   </si>
   <si>
-    <t>To be Done</t>
-  </si>
-  <si>
     <t>ArrayList&lt;Object []&gt;</t>
   </si>
   <si>
@@ -342,6 +339,63 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/ACTUATOR_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/ACTUATOR_NOT_EXISTS/ERROR/OK</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/INVALID_DAY/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RegularScheduleUpdateDayScheduleRule</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>SpecialScheduleUpdateDayScheduleRule</t>
+  </si>
+  <si>
+    <t>SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/INVALID_DAY/RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>SensorGetReadingLatest100</t>
+  </si>
+  <si>
+    <t>SensorGetReadingDaily</t>
+  </si>
+  <si>
+    <t>SensorGetReadingMonthly</t>
+  </si>
+  <si>
+    <t>SensorGetReadingYearly</t>
+  </si>
+  <si>
+    <t>SensorGetByName</t>
+  </si>
+  <si>
+    <t>SensorName</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Timestamp, value)</t>
+  </si>
+  <si>
+    <t>OngoingScheduleGetAll</t>
+  </si>
+  <si>
+    <t>OngoingScheduleGetByActuatorName</t>
+  </si>
+  <si>
+    <t>ScheduleServerIsStarted</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, actuator flag, priority, next start time, next end time)</t>
   </si>
 </sst>
 </file>
@@ -452,16 +506,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,15 +797,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q90"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
@@ -766,7 +820,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -905,7 +959,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1007,35 +1061,35 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="11"/>
       <c r="C16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1046,41 +1100,41 @@
       <c r="B21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="M21" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="N21" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1333,7 +1387,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
@@ -1350,7 +1404,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
@@ -1364,10 +1418,13 @@
       <c r="E36" t="s">
         <v>74</v>
       </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
@@ -1382,12 +1439,15 @@
         <v>74</v>
       </c>
       <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
@@ -1407,7 +1467,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
         <v>31</v>
@@ -1427,13 +1487,13 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="D40">
         <v>18</v>
@@ -1442,18 +1502,18 @@
         <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D41">
         <v>19</v>
@@ -1462,18 +1522,18 @@
         <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
         <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D42">
         <v>20</v>
@@ -1482,18 +1542,18 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D43">
         <v>21</v>
@@ -1502,53 +1562,56 @@
         <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G43" t="s">
-        <v>80</v>
-      </c>
-      <c r="H43" t="s">
-        <v>89</v>
-      </c>
-      <c r="I43" t="s">
-        <v>90</v>
-      </c>
-      <c r="J43" t="s">
-        <v>82</v>
-      </c>
-      <c r="K43" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D44">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E44" t="s">
         <v>74</v>
       </c>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" t="s">
+        <v>88</v>
+      </c>
+      <c r="I44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" t="s">
+        <v>82</v>
+      </c>
+      <c r="K44" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D45">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
         <v>74</v>
@@ -1556,120 +1619,122 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D46">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E46" t="s">
         <v>74</v>
       </c>
       <c r="F46" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D47">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E47" t="s">
         <v>74</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
         <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
         <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
         <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D49">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E49" t="s">
         <v>74</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>102</v>
+      </c>
+      <c r="G49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
         <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D50">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E50" t="s">
         <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>82</v>
-      </c>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="P50" s="2"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D51">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E51" t="s">
         <v>74</v>
@@ -1677,80 +1742,125 @@
       <c r="F51" t="s">
         <v>81</v>
       </c>
-      <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D52">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E52" t="s">
         <v>74</v>
       </c>
       <c r="F52" t="s">
+        <v>82</v>
+      </c>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="P52" s="2"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53">
+        <v>31</v>
+      </c>
+      <c r="E53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" t="s">
+        <v>81</v>
+      </c>
+      <c r="P53" s="2"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54">
+        <v>32</v>
+      </c>
+      <c r="E54" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" t="s">
         <v>64</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" t="s">
         <v>103</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I54" t="s">
         <v>104</v>
       </c>
-      <c r="I52" t="s">
-        <v>105</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="J54" t="s">
+        <v>88</v>
+      </c>
+      <c r="K54" t="s">
         <v>89</v>
       </c>
-      <c r="K52" t="s">
-        <v>90</v>
-      </c>
-      <c r="L52" t="s">
+      <c r="L54" t="s">
         <v>82</v>
       </c>
-      <c r="M52" t="s">
-        <v>93</v>
-      </c>
-      <c r="P52" s="2"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P53" s="2"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>92</v>
+      </c>
       <c r="P54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C55" s="9" t="s">
-        <v>24</v>
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55">
+        <v>33</v>
       </c>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56">
+        <v>34</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -1761,436 +1871,710 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" t="s">
-        <v>37</v>
+        <v>117</v>
+      </c>
+      <c r="D57">
+        <v>35</v>
+      </c>
+      <c r="E57" t="s">
+        <v>118</v>
       </c>
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
         <v>31</v>
       </c>
       <c r="C58" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58">
         <v>36</v>
       </c>
-      <c r="D58" t="s">
-        <v>37</v>
+      <c r="E58" t="s">
+        <v>118</v>
       </c>
       <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
-      </c>
-      <c r="D59" t="s">
-        <v>39</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D59">
+        <v>37</v>
+      </c>
+      <c r="E59" t="s">
+        <v>118</v>
+      </c>
+      <c r="F59" t="s">
+        <v>102</v>
+      </c>
+      <c r="G59" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" t="s">
+        <v>104</v>
+      </c>
+      <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" t="s">
-        <v>43</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D60">
+        <v>38</v>
+      </c>
+      <c r="E60" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60" t="s">
+        <v>103</v>
+      </c>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
         <v>31</v>
       </c>
       <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61">
+        <v>39</v>
+      </c>
+      <c r="E61" t="s">
+        <v>118</v>
+      </c>
+      <c r="P61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C63" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" t="s">
+        <v>37</v>
+      </c>
+      <c r="P65" s="2"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" t="s">
+        <v>37</v>
+      </c>
+      <c r="P66" s="2"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" t="s">
         <v>41</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D69" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" t="s">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" t="s">
         <v>44</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D70" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" t="s">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" t="s">
         <v>46</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D71" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>28</v>
-      </c>
-      <c r="B64" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" t="s">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" t="s">
         <v>59</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D72" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" t="s">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" t="s">
         <v>60</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D73" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" t="s">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" t="s">
         <v>58</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D74" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" t="s">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" t="s">
         <v>55</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D75" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" t="s">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>31</v>
+      </c>
+      <c r="C76" t="s">
         <v>62</v>
       </c>
-      <c r="D68" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" t="s">
         <v>63</v>
       </c>
-      <c r="D69" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="D77" t="s">
         <v>83</v>
       </c>
-      <c r="B70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" t="s">
+        <v>31</v>
+      </c>
+      <c r="C78" t="s">
         <v>65</v>
       </c>
-      <c r="D70" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="D78" t="s">
         <v>83</v>
       </c>
-      <c r="B71" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" t="s">
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" t="s">
         <v>66</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D79" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" t="s">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" t="s">
         <v>68</v>
       </c>
-      <c r="D72" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" t="s">
-        <v>31</v>
-      </c>
-      <c r="C73" t="s">
-        <v>72</v>
-      </c>
-      <c r="D73" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" t="s">
-        <v>69</v>
-      </c>
-      <c r="D74" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" t="s">
-        <v>73</v>
-      </c>
-      <c r="D75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" t="s">
-        <v>31</v>
-      </c>
-      <c r="C77" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D78" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79" t="s">
-        <v>31</v>
-      </c>
-      <c r="C79" t="s">
-        <v>94</v>
-      </c>
-      <c r="D79" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" t="s">
-        <v>31</v>
-      </c>
-      <c r="C80" t="s">
-        <v>95</v>
-      </c>
       <c r="D80" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="D81" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B82" t="s">
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="D82" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B83" t="s">
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B84" t="s">
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B85" t="s">
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B86" t="s">
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" t="s">
+        <v>67</v>
+      </c>
+      <c r="D87" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" t="s">
         <v>83</v>
       </c>
-      <c r="B87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" t="s">
-        <v>92</v>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>31</v>
+      </c>
       <c r="C90" t="s">
+        <v>95</v>
+      </c>
+      <c r="D90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" t="s">
+        <v>98</v>
+      </c>
+      <c r="D94" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" t="s">
+        <v>100</v>
+      </c>
+      <c r="D96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" t="s">
+        <v>101</v>
+      </c>
+      <c r="D97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" t="s">
+        <v>122</v>
+      </c>
+      <c r="D98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>28</v>
+      </c>
+      <c r="B101" t="s">
+        <v>31</v>
+      </c>
+      <c r="C101" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" t="s">
+        <v>113</v>
+      </c>
+      <c r="D102" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" t="s">
+        <v>31</v>
+      </c>
+      <c r="C103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" t="s">
+        <v>116</v>
+      </c>
+      <c r="D105" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thu 1 Sep 2016 21:12 commit by king
SQL - Added Reading SQLs, updated Reading table

Functionality - Implemented all planned GWT server packet implementation.
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="124">
   <si>
     <t>Meaning</t>
   </si>
@@ -365,27 +365,15 @@
     <t>SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/INVALID_DAY/RULE_NOT_EXIST/ERROR/OK</t>
   </si>
   <si>
-    <t>SensorGetReadingLatest100</t>
-  </si>
-  <si>
-    <t>SensorGetReadingDaily</t>
-  </si>
-  <si>
     <t>SensorGetReadingMonthly</t>
   </si>
   <si>
-    <t>SensorGetReadingYearly</t>
-  </si>
-  <si>
     <t>SensorGetByName</t>
   </si>
   <si>
     <t>SensorName</t>
   </si>
   <si>
-    <t>ArrayList&lt;Object []&gt; (Timestamp, value)</t>
-  </si>
-  <si>
     <t>OngoingScheduleGetAll</t>
   </si>
   <si>
@@ -396,6 +384,18 @@
   </si>
   <si>
     <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, actuator flag, priority, next start time, next end time)</t>
+  </si>
+  <si>
+    <t>SensorGetReadingLatest</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Timestamp (LocalDateTime class), value)</t>
+  </si>
+  <si>
+    <t>Date formatted using  : yyyy-MM-dd HH:mm:ss</t>
+  </si>
+  <si>
+    <t>SensorGetReadingBetweenTime</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -516,6 +516,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q107"/>
+  <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,8 +815,8 @@
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="14" width="12.28515625" customWidth="1"/>
@@ -1838,7 +1844,7 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D55">
         <v>33</v>
@@ -1853,14 +1859,11 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D56">
         <v>34</v>
       </c>
-      <c r="E56" t="s">
-        <v>64</v>
-      </c>
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -1877,70 +1880,67 @@
         <v>35</v>
       </c>
       <c r="E57" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D58">
         <v>36</v>
       </c>
       <c r="E58" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" t="s">
-        <v>114</v>
-      </c>
-      <c r="D59">
+        <v>28</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="13">
         <v>37</v>
       </c>
-      <c r="E59" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" t="s">
-        <v>102</v>
-      </c>
-      <c r="G59" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" t="s">
-        <v>104</v>
+      <c r="E59" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D60">
         <v>38</v>
       </c>
       <c r="E60" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F60" t="s">
         <v>102</v>
@@ -1951,21 +1951,6 @@
       <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" t="s">
-        <v>116</v>
-      </c>
-      <c r="D61">
-        <v>39</v>
-      </c>
-      <c r="E61" t="s">
-        <v>118</v>
-      </c>
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -2469,7 +2454,7 @@
         <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D98" t="s">
         <v>37</v>
@@ -2483,10 +2468,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D99" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,10 +2482,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D100" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,7 +2496,7 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
         <v>53</v>
@@ -2519,62 +2504,34 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B102" t="s">
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D102" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B103" t="s">
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D103" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>30</v>
-      </c>
-      <c r="B104" t="s">
-        <v>31</v>
-      </c>
-      <c r="C104" t="s">
-        <v>115</v>
-      </c>
-      <c r="D104" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>30</v>
-      </c>
-      <c r="B105" t="s">
-        <v>31</v>
-      </c>
-      <c r="C105" t="s">
-        <v>116</v>
-      </c>
-      <c r="D105" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wed 7 Sep 2016 19:13 commit by king
Functionality : 
- Added normal socket programming for GWT communication
- ConfigUI now appears on the middle of screen

Code : GWT Incoming packet changed to Object instead of String

Issue fix : GWT Server not able to off once it is started.
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="129">
   <si>
     <t>Meaning</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -396,6 +393,24 @@
   </si>
   <si>
     <t>SensorGetReadingBetweenTime</t>
+  </si>
+  <si>
+    <t>Year (int)</t>
+  </si>
+  <si>
+    <t>Month (int)</t>
+  </si>
+  <si>
+    <t>Day (int)</t>
+  </si>
+  <si>
+    <t>Rule (int)</t>
+  </si>
+  <si>
+    <t>I want to get your current reading</t>
+  </si>
+  <si>
+    <t>Sensor</t>
   </si>
 </sst>
 </file>
@@ -511,17 +526,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q106"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="B97" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1026,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1020,21 +1035,18 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1043,7 +1055,10 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1054,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -1063,101 +1078,104 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="L22" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="M21" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1168,17 +1186,14 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="F23" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1188,10 +1203,10 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1208,10 +1223,16 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -1222,13 +1243,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1239,13 +1257,13 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1256,10 +1274,10 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
         <v>45</v>
@@ -1273,10 +1291,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1287,13 +1308,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1304,28 +1322,13 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" t="s">
-        <v>76</v>
-      </c>
-      <c r="H31" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -1336,24 +1339,27 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
         <v>76</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>77</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>78</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1365,13 +1371,25 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>64</v>
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1382,10 +1400,10 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -1399,13 +1417,13 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D35">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1416,17 +1434,14 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
         <v>74</v>
       </c>
-      <c r="F36" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1436,19 +1451,16 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
         <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1459,16 +1471,19 @@
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D38">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" t="s">
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>104</v>
+      </c>
+      <c r="G38" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1479,16 +1494,16 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D39">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
         <v>74</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1499,16 +1514,16 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="D40">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
         <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1519,16 +1534,16 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="D41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
         <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1539,16 +1554,16 @@
         <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E42" t="s">
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1559,16 +1574,16 @@
         <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D43">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
         <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,31 +1594,16 @@
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D44">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44" t="s">
         <v>74</v>
       </c>
       <c r="F44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" t="s">
-        <v>80</v>
-      </c>
-      <c r="H44" t="s">
-        <v>88</v>
-      </c>
-      <c r="I44" t="s">
-        <v>89</v>
-      </c>
-      <c r="J44" t="s">
-        <v>82</v>
-      </c>
-      <c r="K44" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1614,14 +1614,32 @@
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D45">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s">
         <v>74</v>
       </c>
+      <c r="F45" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" t="s">
+        <v>89</v>
+      </c>
+      <c r="J45" t="s">
+        <v>82</v>
+      </c>
+      <c r="K45" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1631,17 +1649,14 @@
         <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
         <v>74</v>
       </c>
-      <c r="F46" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1651,16 +1666,16 @@
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E47" t="s">
         <v>74</v>
       </c>
       <c r="F47" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1671,16 +1686,16 @@
         <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E48" t="s">
         <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -1691,22 +1706,16 @@
         <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D49">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E49" t="s">
         <v>74</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
-      </c>
-      <c r="G49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -1717,16 +1726,22 @@
         <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D50">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E50" t="s">
         <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>123</v>
+      </c>
+      <c r="G50" t="s">
+        <v>124</v>
+      </c>
+      <c r="H50" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -1737,16 +1752,16 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D51">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E51" t="s">
         <v>74</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -1757,21 +1772,17 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E52" t="s">
         <v>74</v>
       </c>
       <c r="F52" t="s">
-        <v>82</v>
-      </c>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="P52" s="2"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -1781,17 +1792,20 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E53" t="s">
         <v>74</v>
       </c>
       <c r="F53" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
       <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -1802,37 +1816,16 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E54" t="s">
         <v>74</v>
       </c>
       <c r="F54" t="s">
-        <v>64</v>
-      </c>
-      <c r="G54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" t="s">
-        <v>103</v>
-      </c>
-      <c r="I54" t="s">
-        <v>104</v>
-      </c>
-      <c r="J54" t="s">
-        <v>88</v>
-      </c>
-      <c r="K54" t="s">
-        <v>89</v>
-      </c>
-      <c r="L54" t="s">
-        <v>82</v>
-      </c>
-      <c r="M54" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="P54" s="2"/>
     </row>
@@ -1844,10 +1837,37 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="D55">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G55" t="s">
+        <v>123</v>
+      </c>
+      <c r="H55" t="s">
+        <v>124</v>
+      </c>
+      <c r="I55" t="s">
+        <v>125</v>
+      </c>
+      <c r="J55" t="s">
+        <v>126</v>
+      </c>
+      <c r="K55" t="s">
+        <v>89</v>
+      </c>
+      <c r="L55" t="s">
+        <v>82</v>
+      </c>
+      <c r="M55" t="s">
+        <v>92</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -1859,10 +1879,10 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D56">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P56" s="2"/>
     </row>
@@ -1874,13 +1894,10 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D57">
-        <v>35</v>
-      </c>
-      <c r="E57" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="P57" s="2"/>
     </row>
@@ -1892,109 +1909,112 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58">
+        <v>35</v>
+      </c>
+      <c r="E58" t="s">
+        <v>64</v>
+      </c>
+      <c r="P58" s="2"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59">
+        <v>36</v>
+      </c>
+      <c r="E59" t="s">
         <v>114</v>
       </c>
-      <c r="D58">
-        <v>36</v>
-      </c>
-      <c r="E58" t="s">
-        <v>115</v>
-      </c>
-      <c r="P58" s="2"/>
-    </row>
-    <row r="59" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D59" s="13">
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" s="11">
         <v>37</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P59" s="2"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>28</v>
-      </c>
-      <c r="B60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60">
+      <c r="E60" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="P60" s="2"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61">
         <v>38</v>
       </c>
-      <c r="E60" t="s">
-        <v>115</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E61" t="s">
+        <v>114</v>
+      </c>
+      <c r="F61" t="s">
         <v>102</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>103</v>
       </c>
-      <c r="P60" s="2"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C63" s="7" t="s">
+      <c r="P63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C64" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P63" s="2"/>
-    </row>
-    <row r="64" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B65" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D65" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="P64" s="2"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" t="s">
-        <v>37</v>
-      </c>
+      <c r="E65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
       <c r="P65" s="2"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -2005,7 +2025,7 @@
         <v>31</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D66" t="s">
         <v>37</v>
@@ -2020,11 +2040,12 @@
         <v>31</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P67" s="2"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -2034,10 +2055,10 @@
         <v>31</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D68" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -2048,7 +2069,7 @@
         <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D69" t="s">
         <v>43</v>
@@ -2062,7 +2083,7 @@
         <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D70" t="s">
         <v>43</v>
@@ -2076,7 +2097,7 @@
         <v>31</v>
       </c>
       <c r="C71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D71" t="s">
         <v>43</v>
@@ -2090,10 +2111,10 @@
         <v>31</v>
       </c>
       <c r="C72" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D72" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -2104,10 +2125,10 @@
         <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D73" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -2118,10 +2139,10 @@
         <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -2132,10 +2153,10 @@
         <v>31</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -2146,10 +2167,10 @@
         <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D76" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -2160,7 +2181,7 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D77" t="s">
         <v>83</v>
@@ -2174,7 +2195,7 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D78" t="s">
         <v>83</v>
@@ -2188,10 +2209,10 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -2202,10 +2223,10 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D80" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2216,10 +2237,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D81" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2230,10 +2251,10 @@
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,10 +2265,10 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="D83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,10 +2279,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="D84" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2272,7 +2293,7 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D85" t="s">
         <v>90</v>
@@ -2286,7 +2307,7 @@
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D86" t="s">
         <v>90</v>
@@ -2300,10 +2321,10 @@
         <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D87" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,10 +2335,10 @@
         <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D88" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,10 +2349,10 @@
         <v>31</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D89" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2342,10 +2363,10 @@
         <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D90" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2356,10 +2377,10 @@
         <v>31</v>
       </c>
       <c r="C91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2370,10 +2391,10 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D92" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2384,10 +2405,10 @@
         <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D93" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2398,10 +2419,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D94" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2412,7 +2433,7 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D95" t="s">
         <v>90</v>
@@ -2426,7 +2447,7 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D96" t="s">
         <v>90</v>
@@ -2440,10 +2461,10 @@
         <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2454,10 +2475,10 @@
         <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="D98" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,10 +2489,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D99" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,10 +2503,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D100" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,10 +2517,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D101" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2510,10 +2531,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D102" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,20 +2545,34 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D103" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>28</v>
+      </c>
+      <c r="B104" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" t="s">
+        <v>112</v>
+      </c>
+      <c r="D104" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Wed 7 Sep 2016 21:49 commit by king
Code : Added on report received & reading received event, premilary support for Notification Server.
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="127">
   <si>
     <t>Meaning</t>
   </si>
@@ -332,12 +332,6 @@
     <t>SpecialScheduleCreate</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -383,15 +377,9 @@
     <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, actuator flag, priority, next start time, next end time)</t>
   </si>
   <si>
-    <t>SensorGetReadingLatest</t>
-  </si>
-  <si>
     <t>ArrayList&lt;Object []&gt; (Timestamp (LocalDateTime class), value)</t>
   </si>
   <si>
-    <t>Date formatted using  : yyyy-MM-dd HH:mm:ss</t>
-  </si>
-  <si>
     <t>SensorGetReadingBetweenTime</t>
   </si>
   <si>
@@ -411,6 +399,12 @@
   </si>
   <si>
     <t>Sensor</t>
+  </si>
+  <si>
+    <t>End Date (LocalDateTime)</t>
+  </si>
+  <si>
+    <t>Start Date (LocalDateTime)</t>
   </si>
 </sst>
 </file>
@@ -820,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B97" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1020,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1035,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1460,7 +1454,7 @@
         <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1480,7 +1474,7 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G38" t="s">
         <v>75</v>
@@ -1534,7 +1528,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D41">
         <v>18</v>
@@ -1675,7 +1669,7 @@
         <v>74</v>
       </c>
       <c r="F47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1735,13 +1729,13 @@
         <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H50" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -1752,7 +1746,7 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D51">
         <v>28</v>
@@ -1849,16 +1843,16 @@
         <v>64</v>
       </c>
       <c r="G55" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I55" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J55" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K55" t="s">
         <v>89</v>
@@ -1879,7 +1873,7 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D56">
         <v>33</v>
@@ -1894,7 +1888,7 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D57">
         <v>34</v>
@@ -1909,7 +1903,7 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D58">
         <v>35</v>
@@ -1927,17 +1921,17 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D59">
         <v>36</v>
       </c>
       <c r="E59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>28</v>
       </c>
@@ -1945,19 +1939,19 @@
         <v>31</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D60" s="11">
         <v>37</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="P60" s="2"/>
     </row>
@@ -1969,19 +1963,19 @@
         <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D61">
         <v>38</v>
       </c>
       <c r="E61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F61" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="G61" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="P61" s="2"/>
     </row>
@@ -2254,7 +2248,7 @@
         <v>72</v>
       </c>
       <c r="D82" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,7 +2262,7 @@
         <v>69</v>
       </c>
       <c r="D83" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2279,10 +2273,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D84" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,7 +2332,7 @@
         <v>67</v>
       </c>
       <c r="D88" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,7 +2388,7 @@
         <v>96</v>
       </c>
       <c r="D92" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2419,10 +2413,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D94" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,7 +2483,7 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D99" t="s">
         <v>37</v>
@@ -2503,10 +2497,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D100" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2517,10 +2511,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" t="s">
         <v>116</v>
-      </c>
-      <c r="D101" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2531,7 +2525,7 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D102" t="s">
         <v>53</v>
@@ -2544,11 +2538,11 @@
       <c r="B103" t="s">
         <v>31</v>
       </c>
-      <c r="C103" t="s">
-        <v>119</v>
+      <c r="C103" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D103" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2559,10 +2553,10 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D104" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sat 10 Sep 2016 02:29 commit by king
Code :
- Removed redundant reading callbacks event
- Added report & reading callback unregister functions

Functionality : 
- Added controller report timeout event logging
- Added sensor report timeout event logging
- Added events GWT API

Issues Fix :
- Cascade update in GUI not working (regression from 9 Sep 2016 22:30 commit)
- Actuator Edit Dialog not prefilling controller
- Sensor Edit Dialog not prefilling controller, min & max threshold
- Sensor Edit Dialog showing Already in use when the name is retyped to be the same with the original name
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="133">
   <si>
     <t>Meaning</t>
   </si>
@@ -405,6 +405,24 @@
   </si>
   <si>
     <t>Start Date (LocalDateTime)</t>
+  </si>
+  <si>
+    <t>SensorEventGetByName</t>
+  </si>
+  <si>
+    <t>SensorEventGetBetweenTime</t>
+  </si>
+  <si>
+    <t>ControllerEventGetByName</t>
+  </si>
+  <si>
+    <t>ControllerEventGetBetweenTime</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Sensor name, Timestamp (LocalDateTime), event type, event details)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Controller name, Timestamp (LocalDateTime), event type, event details)</t>
   </si>
 </sst>
 </file>
@@ -812,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q107"/>
+  <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1949,7 @@
       </c>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>28</v>
       </c>
@@ -1980,94 +1998,102 @@
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62">
+        <v>39</v>
+      </c>
+      <c r="E62" t="s">
+        <v>112</v>
+      </c>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D63">
+        <v>40</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>125</v>
+      </c>
       <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C64" s="7" t="s">
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64">
+        <v>41</v>
+      </c>
+      <c r="E64" t="s">
+        <v>45</v>
+      </c>
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65">
+        <v>42</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="P65" s="2"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P66" s="2"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C68" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P64" s="2"/>
-    </row>
-    <row r="65" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="P65" s="2"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D66" t="s">
-        <v>37</v>
-      </c>
-      <c r="P66" s="2"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" t="s">
-        <v>36</v>
-      </c>
-      <c r="D67" t="s">
-        <v>37</v>
-      </c>
-      <c r="P67" s="2"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" t="s">
-        <v>40</v>
-      </c>
-      <c r="D69" t="s">
-        <v>43</v>
-      </c>
+      <c r="E69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="P69" s="2"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -2077,11 +2103,12 @@
         <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D70" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P70" s="2"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -2091,11 +2118,12 @@
         <v>31</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D71" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P71" s="2"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2105,10 +2133,10 @@
         <v>31</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -2119,10 +2147,10 @@
         <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D73" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -2133,10 +2161,10 @@
         <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D74" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -2147,10 +2175,10 @@
         <v>31</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D75" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -2161,10 +2189,10 @@
         <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D76" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -2175,10 +2203,10 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -2189,10 +2217,10 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D78" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -2203,10 +2231,10 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D79" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -2217,10 +2245,10 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D80" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,10 +2259,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,10 +2273,10 @@
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D82" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,10 +2287,10 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D83" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,10 +2301,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="D84" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,7 +2315,7 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D85" t="s">
         <v>90</v>
@@ -2301,10 +2329,10 @@
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D86" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2315,10 +2343,10 @@
         <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D87" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2329,10 +2357,10 @@
         <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2343,10 +2371,10 @@
         <v>31</v>
       </c>
       <c r="C89" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D89" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,10 +2385,10 @@
         <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D90" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2371,7 +2399,7 @@
         <v>31</v>
       </c>
       <c r="C91" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="D91" t="s">
         <v>90</v>
@@ -2385,10 +2413,10 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D92" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,10 +2427,10 @@
         <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D93" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,10 +2441,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D94" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2427,7 +2455,7 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D95" t="s">
         <v>90</v>
@@ -2441,10 +2469,10 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D96" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,7 +2483,7 @@
         <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D97" t="s">
         <v>90</v>
@@ -2469,10 +2497,10 @@
         <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D98" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,10 +2511,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,10 +2525,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D100" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,10 +2539,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D101" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,10 +2553,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D102" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2538,11 +2566,11 @@
       <c r="B103" t="s">
         <v>31</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>118</v>
+      <c r="C103" t="s">
+        <v>115</v>
       </c>
       <c r="D103" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,14 +2581,114 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
+        <v>113</v>
+      </c>
+      <c r="D104" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>28</v>
+      </c>
+      <c r="B105" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>28</v>
+      </c>
+      <c r="B106" t="s">
+        <v>31</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
+      <c r="D106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>31</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D107" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>28</v>
+      </c>
+      <c r="B108" t="s">
+        <v>31</v>
+      </c>
+      <c r="C108" t="s">
         <v>110</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D108" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" t="s">
+        <v>127</v>
+      </c>
+      <c r="D109" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110" t="s">
+        <v>128</v>
+      </c>
+      <c r="D110" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" t="s">
+        <v>129</v>
+      </c>
+      <c r="D111" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D112" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sat 10 Sep 2016 02:41 commit by king
GWT Server : Packet format fixed (ACTIVE -> ACTIVATED)

Issue fix : Notification center not auto updating
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -143,9 +143,6 @@
     <t>SHA-1(Password)</t>
   </si>
   <si>
-    <t>INVALID/ACTIVE/PENDING APPROVAL/DEACTIVATED</t>
-  </si>
-  <si>
     <t>SiteGetList</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>ControllerGetActuators</t>
   </si>
   <si>
-    <t>Object[] returned is in same sequence with the CreateTableSQL</t>
-  </si>
-  <si>
     <t>RuleName</t>
   </si>
   <si>
@@ -423,6 +417,12 @@
   </si>
   <si>
     <t>ArrayList&lt;Object []&gt; (Controller name, Timestamp (LocalDateTime), event type, event details)</t>
+  </si>
+  <si>
+    <t>INVALID/ACTIVATED/PENDING APPROVAL/DEACTIVATED</t>
+  </si>
+  <si>
+    <t>Object[] returned is in same sequence with the CreateTableSQL unless special specified</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1047,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1</v>
@@ -1172,22 +1172,22 @@
         <v>4</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1255,7 +1255,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1269,13 +1269,13 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1286,13 +1286,13 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1303,13 +1303,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30">
         <v>7</v>
@@ -1334,13 +1334,13 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -1351,28 +1351,28 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32">
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" t="s">
         <v>76</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>77</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1383,25 +1383,25 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" t="s">
+        <v>75</v>
+      </c>
+      <c r="H33" t="s">
         <v>76</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>77</v>
-      </c>
-      <c r="H33" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1412,13 +1412,13 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1429,13 +1429,13 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1446,13 +1446,13 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1463,16 +1463,16 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1483,19 +1483,19 @@
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D38">
         <v>15</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1506,16 +1506,16 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D39">
         <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1526,16 +1526,16 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D40">
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1546,16 +1546,16 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D41">
         <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1566,16 +1566,16 @@
         <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D42">
         <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1586,16 +1586,16 @@
         <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D43">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1606,16 +1606,16 @@
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D44">
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1626,31 +1626,31 @@
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D45">
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G45" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" t="s">
+        <v>86</v>
+      </c>
+      <c r="I45" t="s">
+        <v>87</v>
+      </c>
+      <c r="J45" t="s">
         <v>80</v>
       </c>
-      <c r="H45" t="s">
-        <v>88</v>
-      </c>
-      <c r="I45" t="s">
-        <v>89</v>
-      </c>
-      <c r="J45" t="s">
-        <v>82</v>
-      </c>
       <c r="K45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -1661,13 +1661,13 @@
         <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D46">
         <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1678,16 +1678,16 @@
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47">
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1698,16 +1698,16 @@
         <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D48">
         <v>25</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -1718,16 +1718,16 @@
         <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D49">
         <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -1738,22 +1738,22 @@
         <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D50">
         <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F50" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" t="s">
+        <v>118</v>
+      </c>
+      <c r="H50" t="s">
         <v>119</v>
-      </c>
-      <c r="G50" t="s">
-        <v>120</v>
-      </c>
-      <c r="H50" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -1764,16 +1764,16 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D51">
         <v>28</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -1784,16 +1784,16 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D52">
         <v>29</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -1804,16 +1804,16 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D53">
         <v>30</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
@@ -1828,16 +1828,16 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D54">
         <v>31</v>
       </c>
       <c r="E54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P54" s="2"/>
     </row>
@@ -1849,37 +1849,37 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D55">
         <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G55" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" t="s">
         <v>119</v>
       </c>
-      <c r="H55" t="s">
+      <c r="J55" t="s">
         <v>120</v>
       </c>
-      <c r="I55" t="s">
-        <v>121</v>
-      </c>
-      <c r="J55" t="s">
-        <v>122</v>
-      </c>
       <c r="K55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -1891,7 +1891,7 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D56">
         <v>33</v>
@@ -1906,7 +1906,7 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D57">
         <v>34</v>
@@ -1921,13 +1921,13 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D58">
         <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P58" s="2"/>
     </row>
@@ -1939,13 +1939,13 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D59">
         <v>36</v>
       </c>
       <c r="E59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P59" s="2"/>
     </row>
@@ -1957,19 +1957,19 @@
         <v>31</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D60" s="11">
         <v>37</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P60" s="2"/>
     </row>
@@ -1981,19 +1981,19 @@
         <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D61">
         <v>38</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P61" s="2"/>
     </row>
@@ -2002,13 +2002,13 @@
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D62">
         <v>39</v>
       </c>
       <c r="E62" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P62" s="2"/>
     </row>
@@ -2017,16 +2017,16 @@
         <v>29</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D63">
         <v>40</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P63" s="2"/>
     </row>
@@ -2035,13 +2035,13 @@
         <v>29</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D64">
         <v>41</v>
       </c>
       <c r="E64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P64" s="2"/>
     </row>
@@ -2050,16 +2050,16 @@
         <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D65">
         <v>42</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P65" s="2"/>
     </row>
@@ -2086,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E69" s="2"/>
       <c r="H69" s="2"/>
@@ -2136,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -2147,10 +2147,10 @@
         <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -2161,10 +2161,10 @@
         <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -2175,10 +2175,10 @@
         <v>31</v>
       </c>
       <c r="C75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -2189,10 +2189,10 @@
         <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -2203,10 +2203,10 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D77" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -2217,10 +2217,10 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D78" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -2231,10 +2231,10 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -2245,10 +2245,10 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D80" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,10 +2259,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D81" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,10 +2273,10 @@
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,10 +2287,10 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,10 +2301,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D84" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2315,10 +2315,10 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D85" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2329,10 +2329,10 @@
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2343,10 +2343,10 @@
         <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D87" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,10 +2357,10 @@
         <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D88" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2371,10 +2371,10 @@
         <v>31</v>
       </c>
       <c r="C89" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D89" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2385,10 +2385,10 @@
         <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D90" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,10 +2399,10 @@
         <v>31</v>
       </c>
       <c r="C91" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,10 +2413,10 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D92" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2427,10 +2427,10 @@
         <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D93" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2441,10 +2441,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D94" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,10 +2455,10 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D95" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,10 +2469,10 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D96" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,10 +2483,10 @@
         <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D97" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,10 +2497,10 @@
         <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D98" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,10 +2511,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D99" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,10 +2525,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D100" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2539,10 +2539,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D101" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,10 +2553,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D102" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D103" t="s">
         <v>37</v>
@@ -2581,10 +2581,10 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D104" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2595,10 +2595,10 @@
         <v>31</v>
       </c>
       <c r="C105" t="s">
+        <v>112</v>
+      </c>
+      <c r="D105" t="s">
         <v>114</v>
-      </c>
-      <c r="D105" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2609,10 +2609,10 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D106" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2623,10 +2623,10 @@
         <v>31</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D107" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,10 +2637,10 @@
         <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D108" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,10 +2648,10 @@
         <v>29</v>
       </c>
       <c r="C109" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D109" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2659,10 +2659,10 @@
         <v>29</v>
       </c>
       <c r="C110" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D110" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2670,10 +2670,10 @@
         <v>29</v>
       </c>
       <c r="C111" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D111" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2681,15 +2681,15 @@
         <v>29</v>
       </c>
       <c r="C112" t="s">
+        <v>128</v>
+      </c>
+      <c r="D112" t="s">
         <v>130</v>
-      </c>
-      <c r="D112" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue 27 Sep 2016 22:35 commit by king
Code :
- GWTServer add actuator command
- ControllerPacketActuatorTrigger issues start thread instead of calling
the run method
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\King\EclipseProjects\Chi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="138">
   <si>
     <t>Meaning</t>
   </si>
@@ -423,6 +423,21 @@
   </si>
   <si>
     <t>Object[] returned is in same sequence with the CreateTableSQL unless special specified</t>
+  </si>
+  <si>
+    <t>ActuatorGetByName</t>
+  </si>
+  <si>
+    <t>ActuatorSetStatus</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ActuatorGetAll</t>
+  </si>
+  <si>
+    <t>ACTUATOR_NOT_EXIST/OK</t>
   </si>
 </sst>
 </file>
@@ -830,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q114"/>
+  <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="B109" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,81 +2078,85 @@
       </c>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66">
+        <v>43</v>
+      </c>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67">
+        <v>44</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F67" s="10"/>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C68" s="7" t="s">
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>134</v>
+      </c>
+      <c r="D68">
+        <v>45</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P69" s="2"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P70" s="2"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C71" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P68" s="2"/>
-    </row>
-    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="P71" s="2"/>
+    </row>
+    <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C72" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="P69" s="2"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>28</v>
-      </c>
-      <c r="B70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" t="s">
-        <v>34</v>
-      </c>
-      <c r="D70" t="s">
-        <v>37</v>
-      </c>
-      <c r="P70" s="2"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>28</v>
-      </c>
-      <c r="B71" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" t="s">
-        <v>37</v>
-      </c>
-      <c r="P71" s="2"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>28</v>
-      </c>
-      <c r="B72" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" t="s">
-        <v>35</v>
-      </c>
-      <c r="D72" t="s">
-        <v>131</v>
-      </c>
+      <c r="E72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="P72" s="2"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -2147,11 +2166,12 @@
         <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -2161,11 +2181,12 @@
         <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D74" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P74" s="2"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2175,10 +2196,10 @@
         <v>31</v>
       </c>
       <c r="C75" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D75" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -2189,7 +2210,7 @@
         <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
         <v>42</v>
@@ -2203,10 +2224,10 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D77" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -2217,10 +2238,10 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D78" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -2231,10 +2252,10 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D79" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -2245,10 +2266,10 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D80" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,10 +2280,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D81" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,10 +2294,10 @@
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D82" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,10 +2308,10 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D83" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,10 +2322,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D84" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2315,10 +2336,10 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D85" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2329,10 +2350,10 @@
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D86" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2343,10 +2364,10 @@
         <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D87" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,10 +2378,10 @@
         <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="D88" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2371,10 +2392,10 @@
         <v>31</v>
       </c>
       <c r="C89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D89" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2385,10 +2406,10 @@
         <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D90" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,10 +2420,10 @@
         <v>31</v>
       </c>
       <c r="C91" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D91" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,10 +2434,10 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D92" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2427,10 +2448,10 @@
         <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D93" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2441,10 +2462,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D94" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,10 +2476,10 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="D95" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,10 +2490,10 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D96" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,10 +2504,10 @@
         <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D97" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,10 +2518,10 @@
         <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D98" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,10 +2532,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D99" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,7 +2546,7 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D100" t="s">
         <v>88</v>
@@ -2539,10 +2560,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D101" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,10 +2574,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2567,10 +2588,10 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D103" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2581,10 +2602,10 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D104" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2595,10 +2616,10 @@
         <v>31</v>
       </c>
       <c r="C105" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D105" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2609,10 +2630,10 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D106" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2622,11 +2643,11 @@
       <c r="B107" t="s">
         <v>31</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>116</v>
+      <c r="C107" t="s">
+        <v>111</v>
       </c>
       <c r="D107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,43 +2658,52 @@
         <v>31</v>
       </c>
       <c r="C108" t="s">
+        <v>112</v>
+      </c>
+      <c r="D108" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>28</v>
+      </c>
+      <c r="B109" t="s">
+        <v>31</v>
+      </c>
+      <c r="C109" t="s">
+        <v>109</v>
+      </c>
+      <c r="D109" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>28</v>
+      </c>
+      <c r="B110" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D110" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>28</v>
+      </c>
+      <c r="B111" t="s">
+        <v>31</v>
+      </c>
+      <c r="C111" t="s">
         <v>108</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D111" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>29</v>
-      </c>
-      <c r="C109" t="s">
-        <v>125</v>
-      </c>
-      <c r="D109" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>29</v>
-      </c>
-      <c r="C110" t="s">
-        <v>126</v>
-      </c>
-      <c r="D110" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>29</v>
-      </c>
-      <c r="C111" t="s">
-        <v>127</v>
-      </c>
-      <c r="D111" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2681,14 +2711,80 @@
         <v>29</v>
       </c>
       <c r="C112" t="s">
+        <v>125</v>
+      </c>
+      <c r="D112" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" t="s">
+        <v>127</v>
+      </c>
+      <c r="D114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" t="s">
         <v>128</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D115" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" t="s">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>136</v>
+      </c>
+      <c r="D116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>29</v>
+      </c>
+      <c r="C117" t="s">
+        <v>133</v>
+      </c>
+      <c r="D117" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" t="s">
+        <v>134</v>
+      </c>
+      <c r="D118" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sun 2 Oct 2016 10:13 commit by king
Code :
- Improves microcontroller communication reliability
- Added notification message on open actuator management frame when data server is not on
- Disable actuator status toggle when data server is not on
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\King\EclipseProjects\Chi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="139">
   <si>
     <t>Meaning</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>ACTUATOR_NOT_EXIST/OK</t>
+  </si>
+  <si>
+    <t>TBD (Controller too slow)</t>
   </si>
 </sst>
 </file>
@@ -847,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +974,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -991,7 +994,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1093,7 +1096,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1113,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Mon 10 Oct 2016 22:53 commit by king
Functionality :
- Scheduling now has OnStart and OnEnd action
- Supports cross day time rules
- Close HSQL connection once exit button is clicked
- Scheduling is now under automation feature

Code :
- Primilary support for Sensor Actuator Response

Needs work :
- Add Cache support for sensor actuator response
- Implement the service for sensor actuator response
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\King\EclipseProjects\Chi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="153">
   <si>
     <t>Meaning</t>
   </si>
@@ -239,9 +239,6 @@
     <t>RegularScheduleUpdateActuator</t>
   </si>
   <si>
-    <t>RegularScheduleUpdateActuatorOn</t>
-  </si>
-  <si>
     <t>ScheduleName</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>Rule</t>
   </si>
   <si>
-    <t>ActuatorOn (boolean)</t>
-  </si>
-  <si>
     <t>SCHEDULE_NOT_EXIST/ERROR/OK</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
     <t>SpecialScheduleUpdateDay</t>
   </si>
   <si>
-    <t>SpecialScheduleUpdateActuatorOn</t>
-  </si>
-  <si>
     <t>SpecialScheduleUpdatePriority</t>
   </si>
   <si>
@@ -368,9 +359,6 @@
     <t>ScheduleServerIsStarted</t>
   </si>
   <si>
-    <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, actuator flag, priority, next start time, next end time)</t>
-  </si>
-  <si>
     <t>ArrayList&lt;Object []&gt; (Timestamp (LocalDateTime class), value)</t>
   </si>
   <si>
@@ -441,6 +429,60 @@
   </si>
   <si>
     <t>TBD (Controller too slow)</t>
+  </si>
+  <si>
+    <t>ON/OFF/NOTHING</t>
+  </si>
+  <si>
+    <t>19a</t>
+  </si>
+  <si>
+    <t>19b</t>
+  </si>
+  <si>
+    <t>19c</t>
+  </si>
+  <si>
+    <t>OnStart</t>
+  </si>
+  <si>
+    <t>OnEnd</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>SpecialScheduleUpdateOnStartAction</t>
+  </si>
+  <si>
+    <t>RegularScheduleUpdateOnStartAction</t>
+  </si>
+  <si>
+    <t>RegularScheduleUpdateOnEndAction</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>29a</t>
+  </si>
+  <si>
+    <t>29b</t>
+  </si>
+  <si>
+    <t>29c</t>
+  </si>
+  <si>
+    <t>SpecialScheduleUpdateOnEndAction</t>
+  </si>
+  <si>
+    <t>SpecialScheduleUpdateManualLock</t>
+  </si>
+  <si>
+    <t>RegularScheduleUpdateManualLock</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, start action, end action, lock, priority, next start time, next end time)</t>
   </si>
 </sst>
 </file>
@@ -535,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -566,6 +608,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -848,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q120"/>
+  <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +1019,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -994,7 +1039,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1056,7 +1101,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1065,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1096,7 +1141,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1116,7 +1161,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1196,16 +1241,16 @@
         <v>49</v>
       </c>
       <c r="K22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1381,19 +1426,19 @@
         <v>59</v>
       </c>
       <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" t="s">
         <v>74</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>75</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>76</v>
       </c>
-      <c r="J32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1410,19 +1455,19 @@
         <v>46</v>
       </c>
       <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>75</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>76</v>
       </c>
-      <c r="I33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1439,7 +1484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1456,7 +1501,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1470,10 +1515,10 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1487,13 +1532,13 @@
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -1507,16 +1552,16 @@
         <v>15</v>
       </c>
       <c r="E38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
         <v>72</v>
       </c>
-      <c r="F38" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -1530,13 +1575,13 @@
         <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1550,13 +1595,13 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1564,168 +1609,174 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D41">
         <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C42" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" t="s">
         <v>71</v>
       </c>
-      <c r="D42">
-        <v>19</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
-      </c>
       <c r="F42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E44" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43">
-        <v>20</v>
-      </c>
-      <c r="E43" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
         <v>68</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>21</v>
       </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" t="s">
+        <v>139</v>
+      </c>
+      <c r="J47" t="s">
+        <v>140</v>
+      </c>
+      <c r="K47" t="s">
+        <v>141</v>
+      </c>
+      <c r="L47" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s">
-        <v>72</v>
-      </c>
-      <c r="F45" t="s">
-        <v>62</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" t="s">
-        <v>86</v>
-      </c>
-      <c r="I45" t="s">
-        <v>87</v>
-      </c>
-      <c r="J45" t="s">
-        <v>80</v>
-      </c>
-      <c r="K45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46">
+      <c r="M47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48">
         <v>23</v>
       </c>
-      <c r="E46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47">
-        <v>24</v>
-      </c>
-      <c r="E47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F47" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48">
-        <v>25</v>
-      </c>
       <c r="E48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -1736,16 +1787,16 @@
         <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D49">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F49" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -1756,22 +1807,16 @@
         <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D50">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E50" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" t="s">
         <v>72</v>
-      </c>
-      <c r="F50" t="s">
-        <v>117</v>
-      </c>
-      <c r="G50" t="s">
-        <v>118</v>
-      </c>
-      <c r="H50" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -1782,16 +1827,16 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D51">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -1802,16 +1847,22 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D52">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F52" t="s">
-        <v>79</v>
+        <v>113</v>
+      </c>
+      <c r="G52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H52" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -1822,21 +1873,17 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D53">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F53" t="s">
-        <v>80</v>
-      </c>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="P53" s="2"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -1846,18 +1893,17 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54">
-        <v>31</v>
+        <v>142</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F54" t="s">
-        <v>79</v>
-      </c>
-      <c r="P54" s="2"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -1867,39 +1913,17 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55">
-        <v>32</v>
+        <v>149</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="E55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F55" t="s">
-        <v>62</v>
-      </c>
-      <c r="G55" t="s">
-        <v>117</v>
-      </c>
-      <c r="H55" t="s">
-        <v>118</v>
-      </c>
-      <c r="I55" t="s">
-        <v>119</v>
-      </c>
-      <c r="J55" t="s">
-        <v>120</v>
-      </c>
-      <c r="K55" t="s">
-        <v>87</v>
-      </c>
-      <c r="L55" t="s">
-        <v>80</v>
-      </c>
-      <c r="M55" t="s">
-        <v>90</v>
-      </c>
-      <c r="P55" s="2"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1909,12 +1933,17 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56">
-        <v>33</v>
-      </c>
-      <c r="P56" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E56" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -1924,11 +1953,20 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D57">
-        <v>34</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" t="s">
+        <v>79</v>
+      </c>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -1939,13 +1977,16 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D58">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="F58" t="s">
+        <v>78</v>
       </c>
       <c r="P58" s="2"/>
     </row>
@@ -1957,37 +1998,58 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D59">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E59" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" t="s">
+        <v>62</v>
+      </c>
+      <c r="G59" t="s">
+        <v>113</v>
+      </c>
+      <c r="H59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I59" t="s">
+        <v>115</v>
+      </c>
+      <c r="J59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K59" t="s">
+        <v>139</v>
+      </c>
+      <c r="L59" t="s">
+        <v>140</v>
+      </c>
+      <c r="M59" t="s">
+        <v>141</v>
+      </c>
+      <c r="N59" t="s">
+        <v>79</v>
+      </c>
+      <c r="O59" t="s">
+        <v>88</v>
+      </c>
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
         <v>110</v>
       </c>
-      <c r="P59" s="2"/>
-    </row>
-    <row r="60" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>28</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D60" s="11">
-        <v>37</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>123</v>
+      <c r="D60">
+        <v>33</v>
       </c>
       <c r="P60" s="2"/>
     </row>
@@ -2002,222 +2064,260 @@
         <v>108</v>
       </c>
       <c r="D61">
+        <v>34</v>
+      </c>
+      <c r="P61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62">
+        <v>35</v>
+      </c>
+      <c r="E62" t="s">
+        <v>62</v>
+      </c>
+      <c r="P62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63">
+        <v>36</v>
+      </c>
+      <c r="E63" t="s">
+        <v>107</v>
+      </c>
+      <c r="P63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="11">
+        <v>37</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65">
         <v>38</v>
       </c>
-      <c r="E61" t="s">
-        <v>110</v>
-      </c>
-      <c r="F61" t="s">
-        <v>117</v>
-      </c>
-      <c r="G61" t="s">
-        <v>118</v>
-      </c>
-      <c r="P61" s="2"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C62" t="s">
-        <v>125</v>
-      </c>
-      <c r="D62">
-        <v>39</v>
-      </c>
-      <c r="E62" t="s">
-        <v>110</v>
-      </c>
-      <c r="P62" s="2"/>
-    </row>
-    <row r="63" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" t="s">
-        <v>126</v>
-      </c>
-      <c r="D63">
-        <v>40</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="P63" s="2"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64">
-        <v>41</v>
-      </c>
-      <c r="E64" t="s">
-        <v>44</v>
-      </c>
-      <c r="P64" s="2"/>
-    </row>
-    <row r="65" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" t="s">
-        <v>128</v>
-      </c>
-      <c r="D65">
-        <v>42</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>123</v>
+      <c r="E65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F65" t="s">
+        <v>113</v>
+      </c>
+      <c r="G65" t="s">
+        <v>114</v>
       </c>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
       <c r="B66" t="s">
         <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D66">
-        <v>43</v>
-      </c>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
+        <v>39</v>
+      </c>
+      <c r="E66" t="s">
+        <v>107</v>
+      </c>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
       <c r="B67" t="s">
         <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D67">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F67" s="10"/>
+        <v>120</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>119</v>
+      </c>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
       <c r="B68" t="s">
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D68">
+        <v>41</v>
+      </c>
+      <c r="E68" t="s">
+        <v>44</v>
+      </c>
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69">
+        <v>42</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="P69" s="2"/>
+    </row>
+    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70">
+        <v>43</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="P70" s="2"/>
+    </row>
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71">
+        <v>44</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="10"/>
+      <c r="P71" s="2"/>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72">
         <v>45</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E72" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F68" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="P68" s="2"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P69" s="2"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P70" s="2"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C71" s="7" t="s">
+      <c r="F72" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P72" s="2"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P73" s="2"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P74" s="2"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C75" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P71" s="2"/>
-    </row>
-    <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="P75" s="2"/>
+    </row>
+    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="P72" s="2"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>28</v>
-      </c>
-      <c r="B73" t="s">
-        <v>31</v>
-      </c>
-      <c r="C73" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" t="s">
-        <v>37</v>
-      </c>
-      <c r="P73" s="2"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>28</v>
-      </c>
-      <c r="B74" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" t="s">
-        <v>36</v>
-      </c>
-      <c r="D74" t="s">
-        <v>37</v>
-      </c>
-      <c r="P74" s="2"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>28</v>
-      </c>
-      <c r="B75" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" t="s">
-        <v>35</v>
-      </c>
-      <c r="D75" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>28</v>
-      </c>
-      <c r="B76" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76" t="s">
-        <v>42</v>
-      </c>
+      <c r="E76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -2227,11 +2327,12 @@
         <v>31</v>
       </c>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D77" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P77" s="2"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -2241,11 +2342,12 @@
         <v>31</v>
       </c>
       <c r="C78" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D78" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -2255,10 +2357,10 @@
         <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D79" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -2269,10 +2371,10 @@
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D80" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2283,10 +2385,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D81" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2297,10 +2399,10 @@
         <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D82" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2311,10 +2413,10 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D83" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2325,10 +2427,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D84" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2339,10 +2441,10 @@
         <v>31</v>
       </c>
       <c r="C85" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D85" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2353,10 +2455,10 @@
         <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D86" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2367,10 +2469,10 @@
         <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D87" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2381,10 +2483,10 @@
         <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D88" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2395,10 +2497,10 @@
         <v>31</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2409,10 +2511,10 @@
         <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D90" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2423,10 +2525,10 @@
         <v>31</v>
       </c>
       <c r="C91" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="D91" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2437,10 +2539,10 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2451,10 +2553,10 @@
         <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D93" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,10 +2567,10 @@
         <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D94" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,10 +2581,10 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="D95" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,13 +2592,13 @@
         <v>28</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C96" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="D96" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,13 +2606,13 @@
         <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C97" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,13 +2620,13 @@
         <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C98" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="D98" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,10 +2637,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="D99" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,10 +2651,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D100" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2563,10 +2665,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,10 +2679,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D102" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2591,10 +2693,10 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D103" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2605,10 +2707,10 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D104" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,10 +2721,10 @@
         <v>31</v>
       </c>
       <c r="C105" t="s">
+        <v>92</v>
+      </c>
+      <c r="D105" t="s">
         <v>99</v>
-      </c>
-      <c r="D105" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,10 +2735,10 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D106" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2647,10 +2749,10 @@
         <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D107" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2658,13 +2760,13 @@
         <v>28</v>
       </c>
       <c r="B108" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="D108" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,13 +2774,13 @@
         <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="D109" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,13 +2788,13 @@
         <v>28</v>
       </c>
       <c r="B110" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>116</v>
+        <v>145</v>
+      </c>
+      <c r="C110" t="s">
+        <v>150</v>
       </c>
       <c r="D110" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,92 +2805,225 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
+        <v>94</v>
+      </c>
+      <c r="D111" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>28</v>
+      </c>
+      <c r="B112" t="s">
+        <v>31</v>
+      </c>
+      <c r="C112" t="s">
+        <v>95</v>
+      </c>
+      <c r="D112" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>28</v>
+      </c>
+      <c r="B113" t="s">
+        <v>31</v>
+      </c>
+      <c r="C113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D113" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" t="s">
+        <v>110</v>
+      </c>
+      <c r="D114" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" t="s">
+        <v>31</v>
+      </c>
+      <c r="C115" t="s">
         <v>108</v>
       </c>
-      <c r="D111" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>29</v>
-      </c>
-      <c r="C112" t="s">
-        <v>125</v>
-      </c>
-      <c r="D112" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>29</v>
-      </c>
-      <c r="C113" t="s">
-        <v>126</v>
-      </c>
-      <c r="D113" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>29</v>
-      </c>
-      <c r="C114" t="s">
-        <v>127</v>
-      </c>
-      <c r="D114" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>29</v>
-      </c>
-      <c r="C115" t="s">
-        <v>128</v>
-      </c>
       <c r="D115" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>28</v>
+      </c>
       <c r="B116" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="D116" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>28</v>
+      </c>
       <c r="B117" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D117" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>28</v>
+      </c>
       <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D118" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119" t="s">
+        <v>31</v>
+      </c>
+      <c r="C119" t="s">
+        <v>105</v>
+      </c>
+      <c r="D119" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>28</v>
+      </c>
+      <c r="B120" t="s">
         <v>29</v>
       </c>
-      <c r="C118" t="s">
-        <v>134</v>
-      </c>
-      <c r="D118" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
+        <v>121</v>
+      </c>
+      <c r="D120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>28</v>
+      </c>
+      <c r="B121" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" t="s">
+        <v>122</v>
+      </c>
+      <c r="D121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>28</v>
+      </c>
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" t="s">
+        <v>123</v>
+      </c>
+      <c r="D122" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>124</v>
+      </c>
+      <c r="D123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>28</v>
+      </c>
+      <c r="B124" t="s">
+        <v>29</v>
+      </c>
+      <c r="C124" t="s">
         <v>132</v>
+      </c>
+      <c r="D124" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B125" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" t="s">
+        <v>129</v>
+      </c>
+      <c r="D125" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>28</v>
+      </c>
+      <c r="B126" t="s">
+        <v>29</v>
+      </c>
+      <c r="C126" t="s">
+        <v>130</v>
+      </c>
+      <c r="D126" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue 11 Oct 2016 15:50 commit by king
Code :
- Added Control Type field in Actuator
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -488,7 +483,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,13 +599,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -885,7 +880,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -895,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,10 +1172,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="14"/>
       <c r="C17" t="s">
         <v>26</v>
       </c>
@@ -1631,7 +1626,7 @@
       <c r="C42" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="12" t="s">
         <v>136</v>
       </c>
       <c r="E42" t="s">
@@ -1651,7 +1646,7 @@
       <c r="C43" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="12" t="s">
         <v>137</v>
       </c>
       <c r="E43" t="s">
@@ -1671,7 +1666,7 @@
       <c r="C44" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="12" t="s">
         <v>138</v>
       </c>
       <c r="E44" t="s">
@@ -1895,7 +1890,7 @@
       <c r="C54" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="12" t="s">
         <v>146</v>
       </c>
       <c r="E54" t="s">
@@ -1915,7 +1910,7 @@
       <c r="C55" t="s">
         <v>149</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="12" t="s">
         <v>147</v>
       </c>
       <c r="E55" t="s">
@@ -1935,7 +1930,7 @@
       <c r="C56" t="s">
         <v>150</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="12" t="s">
         <v>148</v>
       </c>
       <c r="E56" t="s">

</xml_diff>

<commit_message>
Sun 23 Oct 2016 19:23 commit by king
Functionality :
- Added API for sensor actuator response
- Added Logging options in Config
- Disabled debugging tab

Issue Fix :
- Empty log file is created when no log to file option is enabled
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\King\EclipseProjects\Chi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="173">
   <si>
     <t>Meaning</t>
   </si>
@@ -478,12 +483,72 @@
   </si>
   <si>
     <t>ArrayList&lt;Object []&gt; (Schedule name, actuator name, start action, end action, lock, priority, next start time, next end time)</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseGetAll</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseGetByActuatorName</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseCreate</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseSetOnTriggerAction</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseSetOnNotTriggerAction</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseSetExpression</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseSetEnabled</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseSetTimeout</t>
+  </si>
+  <si>
+    <t>OnTriggerAction</t>
+  </si>
+  <si>
+    <t>OnNotTriggerAction</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>ACTUATOR_ALREADY_USED/EXPRESSION_ERROR/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RESPONSE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RESPONSE_NOT_EXIST/EXPRESSION_ERROR/ERROR/OK</t>
+  </si>
+  <si>
+    <t>Enabled (String)</t>
+  </si>
+  <si>
+    <t>Timeout (int)</t>
+  </si>
+  <si>
+    <t>Id (int)</t>
+  </si>
+  <si>
+    <t>RESPONSE_NOT_EXIST/INVALID_TIME/ERROR/OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -880,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -888,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q128"/>
+  <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,36 +2347,94 @@
       </c>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73">
+        <v>46</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" t="s">
+        <v>154</v>
+      </c>
+      <c r="D74">
+        <v>47</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74" s="10"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C75" s="7" t="s">
-        <v>24</v>
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75">
+        <v>48</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G75" t="s">
+        <v>162</v>
+      </c>
+      <c r="H75" t="s">
+        <v>163</v>
+      </c>
+      <c r="I75" t="s">
+        <v>164</v>
+      </c>
+      <c r="J75" t="s">
+        <v>165</v>
       </c>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76">
+        <v>49</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -2319,13 +2442,19 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C77" t="s">
-        <v>34</v>
-      </c>
-      <c r="D77" t="s">
-        <v>37</v>
+        <v>157</v>
+      </c>
+      <c r="D77">
+        <v>50</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F77" t="s">
+        <v>162</v>
       </c>
       <c r="P77" s="2"/>
     </row>
@@ -2334,13 +2463,19 @@
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C78" t="s">
-        <v>36</v>
-      </c>
-      <c r="D78" t="s">
-        <v>37</v>
+        <v>158</v>
+      </c>
+      <c r="D78">
+        <v>51</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F78" t="s">
+        <v>163</v>
       </c>
       <c r="P78" s="2"/>
     </row>
@@ -2349,251 +2484,232 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C79" t="s">
-        <v>35</v>
-      </c>
-      <c r="D79" t="s">
-        <v>127</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="D79">
+        <v>52</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F79" t="s">
+        <v>169</v>
+      </c>
+      <c r="P79" s="2"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80">
+        <v>53</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F80" t="s">
+        <v>170</v>
+      </c>
+      <c r="P80" s="2"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P81" s="2"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P82" s="2"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P83" s="2"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C84" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P84" s="2"/>
+    </row>
+    <row r="85" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="P85" s="2"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" t="s">
+        <v>34</v>
+      </c>
+      <c r="D86" t="s">
+        <v>37</v>
+      </c>
+      <c r="P86" s="2"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" t="s">
+        <v>37</v>
+      </c>
+      <c r="P87" s="2"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" t="s">
         <v>39</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D89" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>28</v>
-      </c>
-      <c r="B81" t="s">
-        <v>31</v>
-      </c>
-      <c r="C81" t="s">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C90" t="s">
         <v>40</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D90" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" t="s">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" t="s">
         <v>43</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D91" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>28</v>
-      </c>
-      <c r="B83" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" t="s">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
         <v>45</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>28</v>
-      </c>
-      <c r="B84" t="s">
-        <v>31</v>
-      </c>
-      <c r="C84" t="s">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
         <v>57</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D93" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>28</v>
-      </c>
-      <c r="B85" t="s">
-        <v>31</v>
-      </c>
-      <c r="C85" t="s">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" t="s">
         <v>58</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D94" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>28</v>
-      </c>
-      <c r="B86" t="s">
-        <v>31</v>
-      </c>
-      <c r="C86" t="s">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
         <v>56</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D95" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>28</v>
-      </c>
-      <c r="B87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" t="s">
         <v>53</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D96" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>28</v>
-      </c>
-      <c r="B88" t="s">
-        <v>31</v>
-      </c>
-      <c r="C88" t="s">
-        <v>60</v>
-      </c>
-      <c r="D88" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>28</v>
-      </c>
-      <c r="B89" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" t="s">
-        <v>61</v>
-      </c>
-      <c r="D89" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>28</v>
-      </c>
-      <c r="B90" t="s">
-        <v>31</v>
-      </c>
-      <c r="C90" t="s">
-        <v>63</v>
-      </c>
-      <c r="D90" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" t="s">
-        <v>31</v>
-      </c>
-      <c r="C91" t="s">
-        <v>64</v>
-      </c>
-      <c r="D91" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>28</v>
-      </c>
-      <c r="B92" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" t="s">
-        <v>66</v>
-      </c>
-      <c r="D92" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>28</v>
-      </c>
-      <c r="B93" t="s">
-        <v>31</v>
-      </c>
-      <c r="C93" t="s">
-        <v>70</v>
-      </c>
-      <c r="D93" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>28</v>
-      </c>
-      <c r="B94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94" t="s">
-        <v>67</v>
-      </c>
-      <c r="D94" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>28</v>
-      </c>
-      <c r="B95" t="s">
-        <v>31</v>
-      </c>
-      <c r="C95" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>28</v>
-      </c>
-      <c r="B96" t="s">
-        <v>145</v>
-      </c>
-      <c r="C96" t="s">
-        <v>143</v>
-      </c>
-      <c r="D96" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2601,13 +2717,13 @@
         <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="D97" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2615,13 +2731,13 @@
         <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="D98" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,10 +2748,10 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D99" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2646,10 +2762,10 @@
         <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D100" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,10 +2776,10 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D101" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,10 +2790,10 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D102" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,10 +2804,10 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D103" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,10 +2818,10 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D104" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,13 +2829,13 @@
         <v>28</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="D105" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2727,10 +2843,10 @@
         <v>28</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C106" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="D106" t="s">
         <v>86</v>
@@ -2741,13 +2857,13 @@
         <v>28</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C107" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D107" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2755,10 +2871,10 @@
         <v>28</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="D108" t="s">
         <v>86</v>
@@ -2769,10 +2885,10 @@
         <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>149</v>
+        <v>68</v>
       </c>
       <c r="D109" t="s">
         <v>86</v>
@@ -2783,13 +2899,13 @@
         <v>28</v>
       </c>
       <c r="B110" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="D110" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,10 +2916,10 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D111" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,10 +2930,10 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D112" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,10 +2944,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D113" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,10 +2958,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D114" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2856,10 +2972,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D115" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,10 +2986,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D116" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2881,13 +2997,13 @@
         <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C117" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="D117" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2895,13 +3011,13 @@
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>112</v>
+        <v>145</v>
+      </c>
+      <c r="C118" t="s">
+        <v>149</v>
       </c>
       <c r="D118" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,13 +3025,13 @@
         <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="C119" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="D119" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2923,13 +3039,13 @@
         <v>28</v>
       </c>
       <c r="B120" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D120" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2937,13 +3053,13 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="D121" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2951,13 +3067,13 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="D122" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2965,13 +3081,13 @@
         <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D123" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,13 +3095,13 @@
         <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D124" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,13 +3109,13 @@
         <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D125" t="s">
-        <v>51</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,17 +3123,255 @@
         <v>28</v>
       </c>
       <c r="B126" t="s">
+        <v>31</v>
+      </c>
+      <c r="C126" t="s">
+        <v>106</v>
+      </c>
+      <c r="D126" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>28</v>
+      </c>
+      <c r="B127" t="s">
+        <v>31</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D127" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>28</v>
+      </c>
+      <c r="B128" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" t="s">
+        <v>105</v>
+      </c>
+      <c r="D128" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>28</v>
+      </c>
+      <c r="B129" t="s">
         <v>29</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C129" t="s">
+        <v>121</v>
+      </c>
+      <c r="D129" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>28</v>
+      </c>
+      <c r="B130" t="s">
+        <v>29</v>
+      </c>
+      <c r="C130" t="s">
+        <v>122</v>
+      </c>
+      <c r="D130" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>28</v>
+      </c>
+      <c r="B131" t="s">
+        <v>29</v>
+      </c>
+      <c r="C131" t="s">
+        <v>123</v>
+      </c>
+      <c r="D131" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>28</v>
+      </c>
+      <c r="B132" t="s">
+        <v>29</v>
+      </c>
+      <c r="C132" t="s">
+        <v>124</v>
+      </c>
+      <c r="D132" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>28</v>
+      </c>
+      <c r="B133" t="s">
+        <v>29</v>
+      </c>
+      <c r="C133" t="s">
+        <v>132</v>
+      </c>
+      <c r="D133" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>28</v>
+      </c>
+      <c r="B134" t="s">
+        <v>29</v>
+      </c>
+      <c r="C134" t="s">
+        <v>129</v>
+      </c>
+      <c r="D134" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>28</v>
+      </c>
+      <c r="B135" t="s">
+        <v>29</v>
+      </c>
+      <c r="C135" t="s">
         <v>130</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D135" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>28</v>
+      </c>
+      <c r="B136" t="s">
+        <v>145</v>
+      </c>
+      <c r="C136" t="s">
+        <v>153</v>
+      </c>
+      <c r="D136" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>28</v>
+      </c>
+      <c r="B137" t="s">
+        <v>145</v>
+      </c>
+      <c r="C137" t="s">
+        <v>154</v>
+      </c>
+      <c r="D137" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>28</v>
+      </c>
+      <c r="B138" t="s">
+        <v>145</v>
+      </c>
+      <c r="C138" t="s">
+        <v>155</v>
+      </c>
+      <c r="D138" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>28</v>
+      </c>
+      <c r="B139" t="s">
+        <v>145</v>
+      </c>
+      <c r="C139" t="s">
+        <v>156</v>
+      </c>
+      <c r="D139" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>28</v>
+      </c>
+      <c r="B140" t="s">
+        <v>145</v>
+      </c>
+      <c r="C140" t="s">
+        <v>157</v>
+      </c>
+      <c r="D140" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>28</v>
+      </c>
+      <c r="B141" t="s">
+        <v>145</v>
+      </c>
+      <c r="C141" t="s">
+        <v>158</v>
+      </c>
+      <c r="D141" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>28</v>
+      </c>
+      <c r="B142" t="s">
+        <v>145</v>
+      </c>
+      <c r="C142" t="s">
+        <v>159</v>
+      </c>
+      <c r="D142" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" t="s">
+        <v>145</v>
+      </c>
+      <c r="C143" t="s">
+        <v>160</v>
+      </c>
+      <c r="D143" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thu 27 Oct 2016 22:57 commit by king
Code :
- Further package separation

Functionality :
- Actuator toggle menu will be disabled when it is locked under a schedule
- GWT ActuatorSetStatus will return ACTUATOR_LOCKED_BY_SCHEDULE when the actuator is locked
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -425,9 +425,6 @@
     <t>ActuatorGetAll</t>
   </si>
   <si>
-    <t>ACTUATOR_NOT_EXIST/OK</t>
-  </si>
-  <si>
     <t>TBD (Controller too slow)</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>RESPONSE_NOT_EXIST/INVALID_TIME/ERROR/OK</t>
+  </si>
+  <si>
+    <t>ACTUATOR_LOCKED_BY_SCHEDULE/ACTUATOR_NOT_EXIST/FAIL/OK</t>
   </si>
 </sst>
 </file>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1079,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1099,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1201,7 +1201,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1221,7 +1221,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1686,19 +1686,19 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E42" t="s">
         <v>71</v>
       </c>
       <c r="F42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1706,19 +1706,19 @@
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
         <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1729,10 +1729,10 @@
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
         <v>71</v>
@@ -1807,13 +1807,13 @@
         <v>85</v>
       </c>
       <c r="I47" t="s">
+        <v>138</v>
+      </c>
+      <c r="J47" t="s">
         <v>139</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>140</v>
-      </c>
-      <c r="K47" t="s">
-        <v>141</v>
       </c>
       <c r="L47" t="s">
         <v>79</v>
@@ -1953,16 +1953,16 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
         <v>71</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -1973,16 +1973,16 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
         <v>71</v>
       </c>
       <c r="F55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -1993,10 +1993,10 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" t="s">
         <v>71</v>
@@ -2082,13 +2082,13 @@
         <v>116</v>
       </c>
       <c r="K59" t="s">
+        <v>138</v>
+      </c>
+      <c r="L59" t="s">
         <v>139</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>140</v>
-      </c>
-      <c r="M59" t="s">
-        <v>141</v>
       </c>
       <c r="N59" t="s">
         <v>79</v>
@@ -2352,10 +2352,10 @@
         <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D73">
         <v>46</v>
@@ -2369,10 +2369,10 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D74">
         <v>47</v>
@@ -2388,10 +2388,10 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D75">
         <v>48</v>
@@ -2400,19 +2400,19 @@
         <v>62</v>
       </c>
       <c r="F75" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G75" t="s">
         <v>161</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>162</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>163</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>164</v>
-      </c>
-      <c r="J75" t="s">
-        <v>165</v>
       </c>
       <c r="P75" s="2"/>
     </row>
@@ -2421,19 +2421,19 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D76">
         <v>49</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P76" s="2"/>
     </row>
@@ -2442,19 +2442,19 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D77">
         <v>50</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P77" s="2"/>
     </row>
@@ -2463,19 +2463,19 @@
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D78">
         <v>51</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P78" s="2"/>
     </row>
@@ -2484,19 +2484,19 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D79">
         <v>52</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P79" s="2"/>
     </row>
@@ -2505,19 +2505,19 @@
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D80">
         <v>53</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P80" s="2"/>
     </row>
@@ -2829,10 +2829,10 @@
         <v>28</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D105" t="s">
         <v>86</v>
@@ -2843,10 +2843,10 @@
         <v>28</v>
       </c>
       <c r="B106" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C106" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D106" t="s">
         <v>86</v>
@@ -2857,10 +2857,10 @@
         <v>28</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D107" t="s">
         <v>86</v>
@@ -2997,10 +2997,10 @@
         <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C117" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D117" t="s">
         <v>86</v>
@@ -3011,10 +3011,10 @@
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C118" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D118" t="s">
         <v>86</v>
@@ -3025,10 +3025,10 @@
         <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C119" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D119" t="s">
         <v>86</v>
@@ -3101,7 +3101,7 @@
         <v>108</v>
       </c>
       <c r="D124" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3115,7 +3115,7 @@
         <v>109</v>
       </c>
       <c r="D125" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,7 +3255,7 @@
         <v>130</v>
       </c>
       <c r="D135" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3263,10 +3263,10 @@
         <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C136" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D136" t="s">
         <v>80</v>
@@ -3277,10 +3277,10 @@
         <v>28</v>
       </c>
       <c r="B137" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C137" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D137" t="s">
         <v>51</v>
@@ -3291,13 +3291,13 @@
         <v>28</v>
       </c>
       <c r="B138" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C138" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D138" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3305,13 +3305,13 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C139" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D139" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3319,13 +3319,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C140" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D140" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3333,13 +3333,13 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C141" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D141" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3347,13 +3347,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D142" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3361,13 +3361,13 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C143" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D143" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tue 1 Nov 2016 17:56 commit by king
Functionality :
- Actuator actions now programmable
- Added UserSensorNotification table
- Added UserActuatorNotification table
- Added UserControllerNotification table
- Added Packet for UserSensorNotification & UserActuatorNotification
- Added Actuatorevent
- Added Regular & Special Schedule Update fields & Delete
- Actuator toggles now cycles along the possible status list

Improvement :
- Events now deleted when entity gets removed

Issue Fixes :
- Exception thrown on right click actuator when schedule server is not
running
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\King\EclipseProjects\Chi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="211">
   <si>
     <t>Meaning</t>
   </si>
@@ -287,9 +282,6 @@
     <t>SCHEDULE_NOT_EXIST/ERROR/OK</t>
   </si>
   <si>
-    <t>SCHEDULE_ALREADY_EXISTS/ERROR/OK</t>
-  </si>
-  <si>
     <t>Enabled (boolean)</t>
   </si>
   <si>
@@ -543,12 +535,129 @@
   </si>
   <si>
     <t>ACTUATOR_LOCKED_BY_SCHEDULE/ACTUATOR_NOT_EXIST/FAIL/OK</t>
+  </si>
+  <si>
+    <t>UserSubscribeSensorNotification</t>
+  </si>
+  <si>
+    <t>UserUpdateSensorNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>UserUnsubscribeSensorNotification</t>
+  </si>
+  <si>
+    <t>UserGetSensorNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>Time (LocalDateTime)</t>
+  </si>
+  <si>
+    <t>UserSubscribeActuatorNotification</t>
+  </si>
+  <si>
+    <t>UserUpdateActuatorNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>UserUnsubscribeActuatorNotification</t>
+  </si>
+  <si>
+    <t>UserGetActuatorNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>USER_NOT_EXIST/SENSOR_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>LocalDateTime/null</t>
+  </si>
+  <si>
+    <t>UserSubscribeControllerNotification</t>
+  </si>
+  <si>
+    <t>UserUpdateControllerNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>UserUnsubscribeControllerNotification</t>
+  </si>
+  <si>
+    <t>UserGetControllerNotificationLastReadTime</t>
+  </si>
+  <si>
+    <t>USER_NOT_EXIST/CONTROLLER_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>USER_NOT_EXIST/ACTUATOR_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RegularScheduleDelete</t>
+  </si>
+  <si>
+    <t>RegularScheduleUpdateFields</t>
+  </si>
+  <si>
+    <t>22a</t>
+  </si>
+  <si>
+    <t>22b</t>
+  </si>
+  <si>
+    <t>39a</t>
+  </si>
+  <si>
+    <t>39b</t>
+  </si>
+  <si>
+    <t>40a</t>
+  </si>
+  <si>
+    <t>40b</t>
+  </si>
+  <si>
+    <t>ActuatorEventGetByName</t>
+  </si>
+  <si>
+    <t>ActuatorEventGetBetweenTime</t>
+  </si>
+  <si>
+    <t>41a</t>
+  </si>
+  <si>
+    <t>41b</t>
+  </si>
+  <si>
+    <t>NewScheduleName</t>
+  </si>
+  <si>
+    <t>22c</t>
+  </si>
+  <si>
+    <t>SpecialScheduleDelete</t>
+  </si>
+  <si>
+    <t>SpecialScheduleUpdateFields</t>
+  </si>
+  <si>
+    <t>SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>32a</t>
+  </si>
+  <si>
+    <t>32b</t>
+  </si>
+  <si>
+    <t>32c</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>SCHEDULE_NOT_EXIST/SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/INVALID_DAY/RULE_NOT_EXIST/ERROR/OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -945,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -953,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q145"/>
+  <dimension ref="A1:Q177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1188,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1099,7 +1208,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1161,7 +1270,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1170,7 +1279,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1201,7 +1310,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1221,7 +1330,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1595,7 +1704,7 @@
         <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1615,7 +1724,7 @@
         <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
         <v>72</v>
@@ -1669,7 +1778,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41">
         <v>18</v>
@@ -1686,19 +1795,19 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" t="s">
         <v>71</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1706,19 +1815,19 @@
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
         <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1729,10 +1838,10 @@
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44" t="s">
         <v>71</v>
@@ -1791,8 +1900,8 @@
       <c r="C47" t="s">
         <v>65</v>
       </c>
-      <c r="D47">
-        <v>22</v>
+      <c r="D47" t="s">
+        <v>191</v>
       </c>
       <c r="E47" t="s">
         <v>71</v>
@@ -1807,19 +1916,19 @@
         <v>85</v>
       </c>
       <c r="I47" t="s">
+        <v>137</v>
+      </c>
+      <c r="J47" t="s">
         <v>138</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>139</v>
-      </c>
-      <c r="K47" t="s">
-        <v>140</v>
       </c>
       <c r="L47" t="s">
         <v>79</v>
       </c>
       <c r="M47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -1827,13 +1936,13 @@
         <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48">
-        <v>23</v>
+        <v>189</v>
+      </c>
+      <c r="D48" t="s">
+        <v>192</v>
       </c>
       <c r="E48" t="s">
         <v>71</v>
@@ -1844,19 +1953,43 @@
         <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49">
-        <v>24</v>
+        <v>190</v>
+      </c>
+      <c r="D49" t="s">
+        <v>202</v>
       </c>
       <c r="E49" t="s">
         <v>71</v>
       </c>
       <c r="F49" t="s">
-        <v>97</v>
+        <v>201</v>
+      </c>
+      <c r="G49" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I49" t="s">
+        <v>85</v>
+      </c>
+      <c r="J49" t="s">
+        <v>137</v>
+      </c>
+      <c r="K49" t="s">
+        <v>138</v>
+      </c>
+      <c r="L49" t="s">
+        <v>139</v>
+      </c>
+      <c r="M49" t="s">
+        <v>79</v>
+      </c>
+      <c r="N49" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -1867,17 +2000,14 @@
         <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D50">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E50" t="s">
         <v>71</v>
       </c>
-      <c r="F50" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1887,16 +2017,16 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D51">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E51" t="s">
         <v>71</v>
       </c>
       <c r="F51" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -1907,22 +2037,16 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D52">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E52" t="s">
         <v>71</v>
       </c>
       <c r="F52" t="s">
-        <v>113</v>
-      </c>
-      <c r="G52" t="s">
-        <v>114</v>
-      </c>
-      <c r="H52" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -1933,16 +2057,16 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D53">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E53" t="s">
         <v>71</v>
       </c>
       <c r="F53" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -1953,16 +2077,22 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>145</v>
+        <v>92</v>
+      </c>
+      <c r="D54">
+        <v>27</v>
       </c>
       <c r="E54" t="s">
         <v>71</v>
       </c>
       <c r="F54" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="G54" t="s">
+        <v>113</v>
+      </c>
+      <c r="H54" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -1973,16 +2103,16 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>146</v>
+        <v>102</v>
+      </c>
+      <c r="D55">
+        <v>28</v>
       </c>
       <c r="E55" t="s">
         <v>71</v>
       </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -1993,16 +2123,16 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E56" t="s">
         <v>71</v>
       </c>
       <c r="F56" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -2013,21 +2143,17 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57">
-        <v>30</v>
+        <v>147</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="E57" t="s">
         <v>71</v>
       </c>
       <c r="F57" t="s">
-        <v>79</v>
-      </c>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="P57" s="2"/>
+        <v>133</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2037,10 +2163,10 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58">
-        <v>31</v>
+        <v>148</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="E58" t="s">
         <v>71</v>
@@ -2048,7 +2174,6 @@
       <c r="F58" t="s">
         <v>78</v>
       </c>
-      <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2058,44 +2183,20 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D59">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E59" t="s">
         <v>71</v>
       </c>
       <c r="F59" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" t="s">
-        <v>113</v>
-      </c>
-      <c r="H59" t="s">
-        <v>114</v>
-      </c>
-      <c r="I59" t="s">
-        <v>115</v>
-      </c>
-      <c r="J59" t="s">
-        <v>116</v>
-      </c>
-      <c r="K59" t="s">
-        <v>138</v>
-      </c>
-      <c r="L59" t="s">
-        <v>139</v>
-      </c>
-      <c r="M59" t="s">
-        <v>140</v>
-      </c>
-      <c r="N59" t="s">
         <v>79</v>
       </c>
-      <c r="O59" t="s">
-        <v>88</v>
-      </c>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
       <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -2106,10 +2207,16 @@
         <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D60">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="E60" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" t="s">
+        <v>78</v>
       </c>
       <c r="P60" s="2"/>
     </row>
@@ -2121,10 +2228,43 @@
         <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
-      </c>
-      <c r="D61">
-        <v>34</v>
+        <v>95</v>
+      </c>
+      <c r="D61" t="s">
+        <v>206</v>
+      </c>
+      <c r="E61" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61" t="s">
+        <v>113</v>
+      </c>
+      <c r="I61" t="s">
+        <v>114</v>
+      </c>
+      <c r="J61" t="s">
+        <v>115</v>
+      </c>
+      <c r="K61" t="s">
+        <v>137</v>
+      </c>
+      <c r="L61" t="s">
+        <v>138</v>
+      </c>
+      <c r="M61" t="s">
+        <v>139</v>
+      </c>
+      <c r="N61" t="s">
+        <v>79</v>
+      </c>
+      <c r="O61" t="s">
+        <v>87</v>
       </c>
       <c r="P61" s="2"/>
     </row>
@@ -2133,16 +2273,16 @@
         <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C62" t="s">
-        <v>109</v>
-      </c>
-      <c r="D62">
-        <v>35</v>
+        <v>189</v>
+      </c>
+      <c r="D62" t="s">
+        <v>207</v>
       </c>
       <c r="E62" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="P62" s="2"/>
     </row>
@@ -2151,40 +2291,63 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
-      </c>
-      <c r="D63">
-        <v>36</v>
+        <v>204</v>
+      </c>
+      <c r="D63" t="s">
+        <v>208</v>
       </c>
       <c r="E63" t="s">
-        <v>107</v>
-      </c>
-      <c r="P63" s="2"/>
-    </row>
-    <row r="64" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F63" t="s">
+        <v>201</v>
+      </c>
+      <c r="G63" t="s">
+        <v>62</v>
+      </c>
+      <c r="H63" t="s">
+        <v>112</v>
+      </c>
+      <c r="I63" t="s">
+        <v>113</v>
+      </c>
+      <c r="J63" t="s">
+        <v>114</v>
+      </c>
+      <c r="K63" t="s">
+        <v>115</v>
+      </c>
+      <c r="L63" t="s">
+        <v>137</v>
+      </c>
+      <c r="M63" t="s">
+        <v>138</v>
+      </c>
+      <c r="N63" t="s">
+        <v>139</v>
+      </c>
+      <c r="O63" t="s">
+        <v>79</v>
+      </c>
+      <c r="P63" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D64" s="11">
-        <v>37</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>119</v>
+      <c r="B64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64">
+        <v>33</v>
       </c>
       <c r="P64" s="2"/>
     </row>
@@ -2196,19 +2359,10 @@
         <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D65">
-        <v>38</v>
-      </c>
-      <c r="E65" t="s">
-        <v>107</v>
-      </c>
-      <c r="F65" t="s">
-        <v>113</v>
-      </c>
-      <c r="G65" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="P65" s="2"/>
     </row>
@@ -2217,80 +2371,86 @@
         <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C66" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D66">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C67" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="D67">
-        <v>40</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F67" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" t="s">
+        <v>106</v>
+      </c>
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" s="11">
+        <v>37</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F68" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="P67" s="2"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" t="s">
-        <v>123</v>
-      </c>
-      <c r="D68">
-        <v>41</v>
-      </c>
-      <c r="E68" t="s">
-        <v>44</v>
+      <c r="G68" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="P68" s="2"/>
     </row>
-    <row r="69" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D69">
-        <v>42</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>119</v>
+        <v>38</v>
+      </c>
+      <c r="E69" t="s">
+        <v>106</v>
+      </c>
+      <c r="F69" t="s">
+        <v>112</v>
+      </c>
+      <c r="G69" t="s">
+        <v>113</v>
       </c>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -2298,16 +2458,17 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
-      </c>
-      <c r="D70">
-        <v>43</v>
-      </c>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
+        <v>122</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E70" t="s">
+        <v>44</v>
+      </c>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -2315,18 +2476,20 @@
         <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
-      </c>
-      <c r="D71">
-        <v>44</v>
+        <v>123</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F71" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -2334,226 +2497,285 @@
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72">
-        <v>45</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>131</v>
+        <v>120</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" t="s">
+        <v>106</v>
       </c>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
-      </c>
-      <c r="D73">
-        <v>46</v>
-      </c>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
+        <v>121</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74">
-        <v>47</v>
-      </c>
-      <c r="E74" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" t="s">
         <v>62</v>
       </c>
       <c r="F74" s="10"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="P75" s="2"/>
+    </row>
+    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" t="s">
+        <v>131</v>
+      </c>
+      <c r="D76">
+        <v>43</v>
+      </c>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="P76" s="2"/>
+    </row>
+    <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77">
+        <v>44</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F77" s="10"/>
+      <c r="P77" s="2"/>
+    </row>
+    <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78">
+        <v>45</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="P78" s="2"/>
+    </row>
+    <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79">
+        <v>46</v>
+      </c>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="P79" s="2"/>
+    </row>
+    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>143</v>
+      </c>
+      <c r="C80" t="s">
+        <v>152</v>
+      </c>
+      <c r="D80">
+        <v>47</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="10"/>
+      <c r="P80" s="2"/>
+    </row>
+    <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" t="s">
+        <v>153</v>
+      </c>
+      <c r="D81">
+        <v>48</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G81" t="s">
+        <v>160</v>
+      </c>
+      <c r="H81" t="s">
+        <v>161</v>
+      </c>
+      <c r="I81" t="s">
+        <v>162</v>
+      </c>
+      <c r="J81" t="s">
+        <v>163</v>
+      </c>
+      <c r="P81" s="2"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" t="s">
         <v>154</v>
       </c>
-      <c r="D75">
-        <v>48</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F75" s="10" t="s">
+      <c r="D82">
+        <v>49</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="P82" s="2"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" t="s">
+        <v>155</v>
+      </c>
+      <c r="D83">
+        <v>50</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F83" t="s">
         <v>160</v>
       </c>
-      <c r="G75" t="s">
+      <c r="P83" s="2"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84" t="s">
+        <v>143</v>
+      </c>
+      <c r="C84" t="s">
+        <v>156</v>
+      </c>
+      <c r="D84">
+        <v>51</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F84" t="s">
         <v>161</v>
       </c>
-      <c r="H75" t="s">
-        <v>162</v>
-      </c>
-      <c r="I75" t="s">
-        <v>163</v>
-      </c>
-      <c r="J75" t="s">
-        <v>164</v>
-      </c>
-      <c r="P75" s="2"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>28</v>
-      </c>
-      <c r="B76" t="s">
-        <v>144</v>
-      </c>
-      <c r="C76" t="s">
-        <v>155</v>
-      </c>
-      <c r="D76">
-        <v>49</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="P76" s="2"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>28</v>
-      </c>
-      <c r="B77" t="s">
-        <v>144</v>
-      </c>
-      <c r="C77" t="s">
-        <v>156</v>
-      </c>
-      <c r="D77">
-        <v>50</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F77" t="s">
-        <v>161</v>
-      </c>
-      <c r="P77" s="2"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>28</v>
-      </c>
-      <c r="B78" t="s">
-        <v>144</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="P84" s="2"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85" t="s">
+        <v>143</v>
+      </c>
+      <c r="C85" t="s">
         <v>157</v>
       </c>
-      <c r="D78">
-        <v>51</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F78" t="s">
-        <v>162</v>
-      </c>
-      <c r="P78" s="2"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>28</v>
-      </c>
-      <c r="B79" t="s">
-        <v>144</v>
-      </c>
-      <c r="C79" t="s">
-        <v>158</v>
-      </c>
-      <c r="D79">
+      <c r="D85">
         <v>52</v>
       </c>
-      <c r="E79" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F79" t="s">
-        <v>168</v>
-      </c>
-      <c r="P79" s="2"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>28</v>
-      </c>
-      <c r="B80" t="s">
-        <v>144</v>
-      </c>
-      <c r="C80" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80">
-        <v>53</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E85" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="P80" s="2"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P81" s="2"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P82" s="2"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P83" s="2"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C84" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P84" s="2"/>
-    </row>
-    <row r="85" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
+      <c r="F85" t="s">
+        <v>167</v>
+      </c>
       <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -2561,13 +2783,19 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C86" t="s">
-        <v>34</v>
-      </c>
-      <c r="D86" t="s">
-        <v>37</v>
+        <v>158</v>
+      </c>
+      <c r="D86">
+        <v>53</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F86" t="s">
+        <v>168</v>
       </c>
       <c r="P86" s="2"/>
     </row>
@@ -2576,13 +2804,19 @@
         <v>28</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C87" t="s">
-        <v>36</v>
-      </c>
-      <c r="D87" t="s">
-        <v>37</v>
+        <v>183</v>
+      </c>
+      <c r="D87">
+        <v>54</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F87" t="s">
+        <v>44</v>
       </c>
       <c r="P87" s="2"/>
     </row>
@@ -2591,349 +2825,424 @@
         <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
-      </c>
-      <c r="D88" t="s">
-        <v>127</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="D88">
+        <v>55</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F88" t="s">
+        <v>44</v>
+      </c>
+      <c r="G88" t="s">
+        <v>176</v>
+      </c>
+      <c r="P88" s="2"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C89" t="s">
-        <v>39</v>
-      </c>
-      <c r="D89" t="s">
-        <v>42</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D89">
+        <v>56</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F89" t="s">
+        <v>44</v>
+      </c>
+      <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C90" t="s">
-        <v>40</v>
-      </c>
-      <c r="D90" t="s">
-        <v>42</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D90">
+        <v>57</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F90" t="s">
+        <v>44</v>
+      </c>
+      <c r="P90" s="2"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C91" t="s">
-        <v>43</v>
-      </c>
-      <c r="D91" t="s">
-        <v>42</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D91">
+        <v>58</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F91" t="s">
+        <v>106</v>
+      </c>
+      <c r="P91" s="2"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>28</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C92" t="s">
-        <v>45</v>
-      </c>
-      <c r="D92" t="s">
-        <v>42</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D92">
+        <v>59</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F92" t="s">
+        <v>106</v>
+      </c>
+      <c r="G92" t="s">
+        <v>176</v>
+      </c>
+      <c r="P92" s="2"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
-      </c>
-      <c r="D93" t="s">
-        <v>47</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D93">
+        <v>60</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F93" t="s">
+        <v>106</v>
+      </c>
+      <c r="P93" s="2"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C94" t="s">
-        <v>58</v>
-      </c>
-      <c r="D94" t="s">
-        <v>51</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D94">
+        <v>61</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F94" t="s">
+        <v>106</v>
+      </c>
+      <c r="P94" s="2"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
       <c r="B95" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C95" t="s">
-        <v>56</v>
-      </c>
-      <c r="D95" t="s">
-        <v>52</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="D95">
+        <v>62</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F95" t="s">
+        <v>62</v>
+      </c>
+      <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C96" t="s">
+        <v>178</v>
+      </c>
+      <c r="D96">
+        <v>63</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G96" t="s">
+        <v>176</v>
+      </c>
+      <c r="P96" s="2"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>143</v>
+      </c>
+      <c r="C97" t="s">
+        <v>179</v>
+      </c>
+      <c r="D97">
+        <v>64</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F97" t="s">
+        <v>62</v>
+      </c>
+      <c r="P97" s="2"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
+        <v>143</v>
+      </c>
+      <c r="C98" t="s">
+        <v>180</v>
+      </c>
+      <c r="D98">
+        <v>65</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F98" t="s">
+        <v>62</v>
+      </c>
+      <c r="P98" s="2"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P99" s="2"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C100" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P100" s="2"/>
+    </row>
+    <row r="101" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="P101" s="2"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>28</v>
+      </c>
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" t="s">
+        <v>34</v>
+      </c>
+      <c r="D102" t="s">
+        <v>37</v>
+      </c>
+      <c r="P102" s="2"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>28</v>
+      </c>
+      <c r="B103" t="s">
+        <v>31</v>
+      </c>
+      <c r="C103" t="s">
+        <v>36</v>
+      </c>
+      <c r="D103" t="s">
+        <v>37</v>
+      </c>
+      <c r="P103" s="2"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>28</v>
+      </c>
+      <c r="B104" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>28</v>
+      </c>
+      <c r="B105" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>28</v>
+      </c>
+      <c r="B106" t="s">
+        <v>31</v>
+      </c>
+      <c r="C106" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>31</v>
+      </c>
+      <c r="C107" t="s">
+        <v>43</v>
+      </c>
+      <c r="D107" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>28</v>
+      </c>
+      <c r="B108" t="s">
+        <v>31</v>
+      </c>
+      <c r="C108" t="s">
+        <v>45</v>
+      </c>
+      <c r="D108" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>28</v>
+      </c>
+      <c r="B109" t="s">
+        <v>31</v>
+      </c>
+      <c r="C109" t="s">
+        <v>57</v>
+      </c>
+      <c r="D109" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>28</v>
+      </c>
+      <c r="B110" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" t="s">
+        <v>58</v>
+      </c>
+      <c r="D110" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>28</v>
+      </c>
+      <c r="B111" t="s">
+        <v>31</v>
+      </c>
+      <c r="C111" t="s">
+        <v>56</v>
+      </c>
+      <c r="D111" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>28</v>
+      </c>
+      <c r="B112" t="s">
+        <v>31</v>
+      </c>
+      <c r="C112" t="s">
         <v>53</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D112" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>28</v>
-      </c>
-      <c r="B97" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" t="s">
-        <v>60</v>
-      </c>
-      <c r="D97" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>28</v>
-      </c>
-      <c r="B98" t="s">
-        <v>31</v>
-      </c>
-      <c r="C98" t="s">
-        <v>61</v>
-      </c>
-      <c r="D98" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>28</v>
-      </c>
-      <c r="B99" t="s">
-        <v>31</v>
-      </c>
-      <c r="C99" t="s">
-        <v>63</v>
-      </c>
-      <c r="D99" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>28</v>
-      </c>
-      <c r="B100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C100" t="s">
-        <v>64</v>
-      </c>
-      <c r="D100" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>28</v>
-      </c>
-      <c r="B101" t="s">
-        <v>31</v>
-      </c>
-      <c r="C101" t="s">
-        <v>66</v>
-      </c>
-      <c r="D101" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" t="s">
-        <v>31</v>
-      </c>
-      <c r="C102" t="s">
-        <v>70</v>
-      </c>
-      <c r="D102" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>28</v>
-      </c>
-      <c r="B103" t="s">
-        <v>31</v>
-      </c>
-      <c r="C103" t="s">
-        <v>67</v>
-      </c>
-      <c r="D103" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>28</v>
-      </c>
-      <c r="B104" t="s">
-        <v>31</v>
-      </c>
-      <c r="C104" t="s">
-        <v>101</v>
-      </c>
-      <c r="D104" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>28</v>
-      </c>
-      <c r="B105" t="s">
-        <v>144</v>
-      </c>
-      <c r="C105" t="s">
-        <v>142</v>
-      </c>
-      <c r="D105" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>28</v>
-      </c>
-      <c r="B106" t="s">
-        <v>144</v>
-      </c>
-      <c r="C106" t="s">
-        <v>143</v>
-      </c>
-      <c r="D106" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" t="s">
-        <v>144</v>
-      </c>
-      <c r="C107" t="s">
-        <v>150</v>
-      </c>
-      <c r="D107" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" t="s">
-        <v>69</v>
-      </c>
-      <c r="D108" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>28</v>
-      </c>
-      <c r="B109" t="s">
-        <v>31</v>
-      </c>
-      <c r="C109" t="s">
-        <v>68</v>
-      </c>
-      <c r="D109" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>28</v>
-      </c>
-      <c r="B110" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" t="s">
-        <v>65</v>
-      </c>
-      <c r="D110" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" t="s">
-        <v>31</v>
-      </c>
-      <c r="C111" t="s">
-        <v>89</v>
-      </c>
-      <c r="D111" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" t="s">
-        <v>31</v>
-      </c>
-      <c r="C112" t="s">
-        <v>90</v>
-      </c>
-      <c r="D112" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2944,10 +3253,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="D113" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2958,10 +3267,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="D114" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2972,10 +3281,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D115" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2986,10 +3295,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="D116" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2997,10 +3306,10 @@
         <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="D117" t="s">
         <v>86</v>
@@ -3011,13 +3320,13 @@
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="D118" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3025,13 +3334,13 @@
         <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C119" t="s">
-        <v>149</v>
+        <v>67</v>
       </c>
       <c r="D119" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3042,10 +3351,10 @@
         <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D120" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3053,10 +3362,10 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C121" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="D121" t="s">
         <v>86</v>
@@ -3067,13 +3376,13 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C122" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="D122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3081,13 +3390,13 @@
         <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C123" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="D123" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3098,10 +3407,10 @@
         <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="D124" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3112,10 +3421,10 @@
         <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="D125" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3126,10 +3435,10 @@
         <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="D126" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3137,13 +3446,13 @@
         <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>31</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>112</v>
+        <v>143</v>
+      </c>
+      <c r="C127" t="s">
+        <v>189</v>
       </c>
       <c r="D127" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3151,13 +3460,13 @@
         <v>28</v>
       </c>
       <c r="B128" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="D128" t="s">
-        <v>111</v>
+        <v>210</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3165,13 +3474,13 @@
         <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D129" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3179,13 +3488,13 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="D130" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3193,13 +3502,13 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D131" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3207,13 +3516,13 @@
         <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="D132" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3221,13 +3530,13 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="D133" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3235,13 +3544,13 @@
         <v>28</v>
       </c>
       <c r="B134" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="D134" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3249,13 +3558,13 @@
         <v>28</v>
       </c>
       <c r="B135" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="C135" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D135" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3263,13 +3572,13 @@
         <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C136" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D136" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3277,13 +3586,13 @@
         <v>28</v>
       </c>
       <c r="B137" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C137" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D137" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3291,13 +3600,13 @@
         <v>28</v>
       </c>
       <c r="B138" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="D138" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3305,13 +3614,13 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
       <c r="D139" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3319,13 +3628,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="D140" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3333,13 +3642,13 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="D141" t="s">
-        <v>167</v>
+        <v>86</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3347,13 +3656,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C142" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="D142" t="s">
-        <v>166</v>
+        <v>209</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3361,18 +3670,466 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="C143" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="D143" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>28</v>
+      </c>
+      <c r="B144" t="s">
+        <v>31</v>
+      </c>
+      <c r="C144" t="s">
+        <v>107</v>
+      </c>
+      <c r="D144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>28</v>
+      </c>
+      <c r="B145" t="s">
+        <v>31</v>
+      </c>
+      <c r="C145" t="s">
+        <v>108</v>
+      </c>
+      <c r="D145" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>28</v>
+      </c>
+      <c r="B146" t="s">
+        <v>31</v>
+      </c>
+      <c r="C146" t="s">
+        <v>105</v>
+      </c>
+      <c r="D146" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>28</v>
+      </c>
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D147" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>28</v>
+      </c>
+      <c r="B148" t="s">
+        <v>31</v>
+      </c>
+      <c r="C148" t="s">
+        <v>104</v>
+      </c>
+      <c r="D148" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>28</v>
+      </c>
+      <c r="B149" t="s">
+        <v>29</v>
+      </c>
+      <c r="C149" t="s">
+        <v>120</v>
+      </c>
+      <c r="D149" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>28</v>
+      </c>
+      <c r="B150" t="s">
+        <v>29</v>
+      </c>
+      <c r="C150" t="s">
+        <v>121</v>
+      </c>
+      <c r="D150" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>28</v>
+      </c>
+      <c r="B151" t="s">
+        <v>29</v>
+      </c>
+      <c r="C151" t="s">
+        <v>122</v>
+      </c>
+      <c r="D151" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>28</v>
+      </c>
+      <c r="B152" t="s">
+        <v>29</v>
+      </c>
+      <c r="C152" t="s">
+        <v>123</v>
+      </c>
+      <c r="D152" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>28</v>
+      </c>
+      <c r="B153" t="s">
+        <v>29</v>
+      </c>
+      <c r="C153" t="s">
+        <v>131</v>
+      </c>
+      <c r="D153" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>28</v>
+      </c>
+      <c r="B154" t="s">
+        <v>29</v>
+      </c>
+      <c r="C154" t="s">
+        <v>128</v>
+      </c>
+      <c r="D154" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>28</v>
+      </c>
+      <c r="B155" t="s">
+        <v>29</v>
+      </c>
+      <c r="C155" t="s">
+        <v>129</v>
+      </c>
+      <c r="D155" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" t="s">
-        <v>128</v>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" t="s">
+        <v>143</v>
+      </c>
+      <c r="C156" t="s">
+        <v>151</v>
+      </c>
+      <c r="D156" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>28</v>
+      </c>
+      <c r="B157" t="s">
+        <v>143</v>
+      </c>
+      <c r="C157" t="s">
+        <v>152</v>
+      </c>
+      <c r="D157" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>28</v>
+      </c>
+      <c r="B158" t="s">
+        <v>143</v>
+      </c>
+      <c r="C158" t="s">
+        <v>153</v>
+      </c>
+      <c r="D158" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>28</v>
+      </c>
+      <c r="B159" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159" t="s">
+        <v>154</v>
+      </c>
+      <c r="D159" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>28</v>
+      </c>
+      <c r="B160" t="s">
+        <v>143</v>
+      </c>
+      <c r="C160" t="s">
+        <v>155</v>
+      </c>
+      <c r="D160" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>28</v>
+      </c>
+      <c r="B161" t="s">
+        <v>143</v>
+      </c>
+      <c r="C161" t="s">
+        <v>156</v>
+      </c>
+      <c r="D161" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>28</v>
+      </c>
+      <c r="B162" t="s">
+        <v>143</v>
+      </c>
+      <c r="C162" t="s">
+        <v>157</v>
+      </c>
+      <c r="D162" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>28</v>
+      </c>
+      <c r="B163" t="s">
+        <v>143</v>
+      </c>
+      <c r="C163" t="s">
+        <v>158</v>
+      </c>
+      <c r="D163" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>28</v>
+      </c>
+      <c r="B164" t="s">
+        <v>143</v>
+      </c>
+      <c r="C164" t="s">
+        <v>183</v>
+      </c>
+      <c r="D164" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>28</v>
+      </c>
+      <c r="B165" t="s">
+        <v>143</v>
+      </c>
+      <c r="C165" t="s">
+        <v>184</v>
+      </c>
+      <c r="D165" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>28</v>
+      </c>
+      <c r="B166" t="s">
+        <v>143</v>
+      </c>
+      <c r="C166" t="s">
+        <v>185</v>
+      </c>
+      <c r="D166" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>28</v>
+      </c>
+      <c r="B167" t="s">
+        <v>143</v>
+      </c>
+      <c r="C167" t="s">
+        <v>186</v>
+      </c>
+      <c r="D167" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>28</v>
+      </c>
+      <c r="B168" t="s">
+        <v>143</v>
+      </c>
+      <c r="C168" t="s">
+        <v>172</v>
+      </c>
+      <c r="D168" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>28</v>
+      </c>
+      <c r="B169" t="s">
+        <v>143</v>
+      </c>
+      <c r="C169" t="s">
+        <v>173</v>
+      </c>
+      <c r="D169" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>28</v>
+      </c>
+      <c r="B170" t="s">
+        <v>143</v>
+      </c>
+      <c r="C170" t="s">
+        <v>174</v>
+      </c>
+      <c r="D170" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>28</v>
+      </c>
+      <c r="B171" t="s">
+        <v>143</v>
+      </c>
+      <c r="C171" t="s">
+        <v>175</v>
+      </c>
+      <c r="D171" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>28</v>
+      </c>
+      <c r="B172" t="s">
+        <v>143</v>
+      </c>
+      <c r="C172" t="s">
+        <v>177</v>
+      </c>
+      <c r="D172" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>28</v>
+      </c>
+      <c r="B173" t="s">
+        <v>143</v>
+      </c>
+      <c r="C173" t="s">
+        <v>178</v>
+      </c>
+      <c r="D173" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>28</v>
+      </c>
+      <c r="B174" t="s">
+        <v>143</v>
+      </c>
+      <c r="C174" t="s">
+        <v>179</v>
+      </c>
+      <c r="D174" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>28</v>
+      </c>
+      <c r="B175" t="s">
+        <v>143</v>
+      </c>
+      <c r="C175" t="s">
+        <v>180</v>
+      </c>
+      <c r="D175" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wed 2 Nov 2016 18:00 commit by king
Functionality :
- Adds DayScheduleRule delete packet

Issue Fixes :
- GWT Server fails to update/delete Regular & SpecialSchedules
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="215">
   <si>
     <t>Meaning</t>
   </si>
@@ -177,9 +177,6 @@
     <t>ArrayList&lt;Object&gt;</t>
   </si>
   <si>
-    <t>RULE_NOT_EXIST/INVALID_TIME/ERROR/OK</t>
-  </si>
-  <si>
     <t>DayScheduleRuleCreate</t>
   </si>
   <si>
@@ -652,6 +649,21 @@
   </si>
   <si>
     <t>SCHEDULE_NOT_EXIST/SCHEDULE_ALREADY_EXISTS/ACTUATOR_NOT_EXIST/INVALID_DAY/RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RULE_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>RULE_NOT_EXIST/RULE_ALREADY_EXISTS/INVALID_TIME/ERROR/OK</t>
+  </si>
+  <si>
+    <t>DayScheduleRuleDelete</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>9b</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q177"/>
+  <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1208,7 +1220,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1270,7 +1282,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1279,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1310,7 +1322,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1330,7 +1342,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1410,16 +1422,16 @@
         <v>49</v>
       </c>
       <c r="K22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1552,7 +1564,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>7</v>
@@ -1566,7 +1578,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>8</v>
@@ -1583,28 +1595,28 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>213</v>
       </c>
       <c r="E32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" t="s">
         <v>73</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>74</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>75</v>
-      </c>
-      <c r="J32" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1612,29 +1624,17 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33">
-        <v>10</v>
+        <v>212</v>
+      </c>
+      <c r="D33" t="s">
+        <v>214</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
       </c>
-      <c r="F33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
-      </c>
-      <c r="H33" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1644,13 +1644,25 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D34">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1661,13 +1673,13 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
         <v>61</v>
-      </c>
-      <c r="D35">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -1678,13 +1690,13 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D36">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1695,16 +1707,13 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1715,19 +1724,16 @@
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D38">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1738,16 +1744,19 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
         <v>70</v>
       </c>
-      <c r="D39">
-        <v>16</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" t="s">
         <v>71</v>
-      </c>
-      <c r="F39" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -1758,16 +1767,16 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D40">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -1778,16 +1787,16 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D41">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F41" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -1795,19 +1804,19 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>134</v>
+        <v>99</v>
+      </c>
+      <c r="D42">
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F42" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1815,19 +1824,19 @@
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1835,19 +1844,19 @@
         <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -1858,16 +1867,16 @@
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45">
-        <v>20</v>
+        <v>148</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -1881,10 +1890,10 @@
         <v>68</v>
       </c>
       <c r="D46">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F46" t="s">
         <v>78</v>
@@ -1898,37 +1907,16 @@
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" t="s">
-        <v>191</v>
+        <v>67</v>
+      </c>
+      <c r="D47">
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" t="s">
-        <v>62</v>
-      </c>
-      <c r="G47" t="s">
         <v>77</v>
-      </c>
-      <c r="H47" t="s">
-        <v>85</v>
-      </c>
-      <c r="I47" t="s">
-        <v>137</v>
-      </c>
-      <c r="J47" t="s">
-        <v>138</v>
-      </c>
-      <c r="K47" t="s">
-        <v>139</v>
-      </c>
-      <c r="L47" t="s">
-        <v>79</v>
-      </c>
-      <c r="M47" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -1936,16 +1924,40 @@
         <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="F48" t="s">
+        <v>61</v>
+      </c>
+      <c r="G48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48" t="s">
+        <v>136</v>
+      </c>
+      <c r="J48" t="s">
+        <v>137</v>
+      </c>
+      <c r="K48" t="s">
+        <v>138</v>
+      </c>
+      <c r="L48" t="s">
+        <v>78</v>
+      </c>
+      <c r="M48" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -1953,43 +1965,16 @@
         <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49" t="s">
-        <v>201</v>
-      </c>
-      <c r="G49" t="s">
-        <v>62</v>
-      </c>
-      <c r="H49" t="s">
-        <v>77</v>
-      </c>
-      <c r="I49" t="s">
-        <v>85</v>
-      </c>
-      <c r="J49" t="s">
-        <v>137</v>
-      </c>
-      <c r="K49" t="s">
-        <v>138</v>
-      </c>
-      <c r="L49" t="s">
-        <v>139</v>
-      </c>
-      <c r="M49" t="s">
-        <v>79</v>
-      </c>
-      <c r="N49" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -1997,16 +1982,43 @@
         <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50">
-        <v>23</v>
+        <v>189</v>
+      </c>
+      <c r="D50" t="s">
+        <v>201</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="F50" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>76</v>
+      </c>
+      <c r="I50" t="s">
+        <v>84</v>
+      </c>
+      <c r="J50" t="s">
+        <v>136</v>
+      </c>
+      <c r="K50" t="s">
+        <v>137</v>
+      </c>
+      <c r="L50" t="s">
+        <v>138</v>
+      </c>
+      <c r="M50" t="s">
+        <v>78</v>
+      </c>
+      <c r="N50" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -2017,16 +2029,13 @@
         <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
-      </c>
-      <c r="F51" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -2037,16 +2046,16 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D52">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -2057,16 +2066,16 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D53">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E53" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" t="s">
         <v>71</v>
-      </c>
-      <c r="F53" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -2077,22 +2086,16 @@
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D54">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F54" t="s">
-        <v>112</v>
-      </c>
-      <c r="G54" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -2103,16 +2106,22 @@
         <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D55">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F55" t="s">
-        <v>46</v>
+        <v>111</v>
+      </c>
+      <c r="G55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H55" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -2123,16 +2132,16 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>144</v>
+        <v>101</v>
+      </c>
+      <c r="D56">
+        <v>28</v>
       </c>
       <c r="E56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -2143,16 +2152,16 @@
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -2163,16 +2172,16 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F58" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -2183,21 +2192,17 @@
         <v>31</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59">
-        <v>30</v>
+        <v>147</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F59" t="s">
-        <v>79</v>
-      </c>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="P59" s="2"/>
+        <v>77</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -2207,17 +2212,20 @@
         <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D60">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" t="s">
         <v>78</v>
       </c>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
       <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -2228,43 +2236,16 @@
         <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" t="s">
-        <v>206</v>
+        <v>93</v>
+      </c>
+      <c r="D61">
+        <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" t="s">
-        <v>62</v>
-      </c>
-      <c r="G61" t="s">
-        <v>112</v>
-      </c>
-      <c r="H61" t="s">
-        <v>113</v>
-      </c>
-      <c r="I61" t="s">
-        <v>114</v>
-      </c>
-      <c r="J61" t="s">
-        <v>115</v>
-      </c>
-      <c r="K61" t="s">
-        <v>137</v>
-      </c>
-      <c r="L61" t="s">
-        <v>138</v>
-      </c>
-      <c r="M61" t="s">
-        <v>139</v>
-      </c>
-      <c r="N61" t="s">
-        <v>79</v>
-      </c>
-      <c r="O61" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="P61" s="2"/>
     </row>
@@ -2273,16 +2254,46 @@
         <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E62" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="F62" t="s">
+        <v>61</v>
+      </c>
+      <c r="G62" t="s">
+        <v>111</v>
+      </c>
+      <c r="H62" t="s">
+        <v>112</v>
+      </c>
+      <c r="I62" t="s">
+        <v>113</v>
+      </c>
+      <c r="J62" t="s">
+        <v>114</v>
+      </c>
+      <c r="K62" t="s">
+        <v>136</v>
+      </c>
+      <c r="L62" t="s">
+        <v>137</v>
+      </c>
+      <c r="M62" t="s">
+        <v>138</v>
+      </c>
+      <c r="N62" t="s">
+        <v>78</v>
+      </c>
+      <c r="O62" t="s">
+        <v>86</v>
       </c>
       <c r="P62" s="2"/>
     </row>
@@ -2291,65 +2302,68 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E63" t="s">
-        <v>71</v>
-      </c>
-      <c r="F63" t="s">
-        <v>201</v>
-      </c>
-      <c r="G63" t="s">
-        <v>62</v>
-      </c>
-      <c r="H63" t="s">
-        <v>112</v>
-      </c>
-      <c r="I63" t="s">
-        <v>113</v>
-      </c>
-      <c r="J63" t="s">
-        <v>114</v>
-      </c>
-      <c r="K63" t="s">
-        <v>115</v>
-      </c>
-      <c r="L63" t="s">
-        <v>137</v>
-      </c>
-      <c r="M63" t="s">
-        <v>138</v>
-      </c>
-      <c r="N63" t="s">
-        <v>139</v>
-      </c>
-      <c r="O63" t="s">
-        <v>79</v>
-      </c>
-      <c r="P63" t="s">
-        <v>87</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C64" t="s">
-        <v>109</v>
-      </c>
-      <c r="D64">
-        <v>33</v>
-      </c>
-      <c r="P64" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="D64" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s">
+        <v>200</v>
+      </c>
+      <c r="G64" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" t="s">
+        <v>112</v>
+      </c>
+      <c r="J64" t="s">
+        <v>113</v>
+      </c>
+      <c r="K64" t="s">
+        <v>114</v>
+      </c>
+      <c r="L64" t="s">
+        <v>136</v>
+      </c>
+      <c r="M64" t="s">
+        <v>137</v>
+      </c>
+      <c r="N64" t="s">
+        <v>138</v>
+      </c>
+      <c r="O64" t="s">
+        <v>78</v>
+      </c>
+      <c r="P64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -2359,10 +2373,10 @@
         <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D65">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P65" s="2"/>
     </row>
@@ -2374,13 +2388,10 @@
         <v>31</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D66">
-        <v>35</v>
-      </c>
-      <c r="E66" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="P66" s="2"/>
     </row>
@@ -2392,61 +2403,55 @@
         <v>31</v>
       </c>
       <c r="C67" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67">
+        <v>35</v>
+      </c>
+      <c r="E67" t="s">
+        <v>61</v>
+      </c>
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68">
+        <v>36</v>
+      </c>
+      <c r="E68" t="s">
         <v>105</v>
       </c>
-      <c r="D67">
-        <v>36</v>
-      </c>
-      <c r="E67" t="s">
-        <v>106</v>
-      </c>
-      <c r="P67" s="2"/>
-    </row>
-    <row r="68" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D68" s="11">
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="11">
         <v>37</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="G68" s="10" t="s">
+      <c r="E69" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F69" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="P68" s="2"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" t="s">
-        <v>104</v>
-      </c>
-      <c r="D69">
-        <v>38</v>
-      </c>
-      <c r="E69" t="s">
-        <v>106</v>
-      </c>
-      <c r="F69" t="s">
-        <v>112</v>
-      </c>
-      <c r="G69" t="s">
-        <v>113</v>
+      <c r="G69" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="P69" s="2"/>
     </row>
@@ -2455,20 +2460,26 @@
         <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>122</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>193</v>
+        <v>103</v>
+      </c>
+      <c r="D70">
+        <v>38</v>
       </c>
       <c r="E70" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+      <c r="F70" t="s">
+        <v>111</v>
+      </c>
+      <c r="G70" t="s">
+        <v>112</v>
       </c>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -2476,20 +2487,17 @@
         <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>118</v>
+        <v>192</v>
+      </c>
+      <c r="E71" t="s">
+        <v>44</v>
       </c>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -2497,17 +2505,20 @@
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E72" t="s">
-        <v>106</v>
+        <v>193</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -2515,16 +2526,13 @@
         <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>118</v>
+        <v>194</v>
+      </c>
+      <c r="E73" t="s">
+        <v>105</v>
       </c>
       <c r="P73" s="2"/>
     </row>
@@ -2533,18 +2541,20 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>120</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="E74" t="s">
-        <v>62</v>
-      </c>
-      <c r="F74" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="P74" s="2"/>
     </row>
     <row r="75" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2552,40 +2562,42 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C75" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D75" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F75" s="10" t="s">
+      <c r="E75" t="s">
+        <v>61</v>
+      </c>
+      <c r="F75" s="10"/>
+      <c r="P75" s="2"/>
+    </row>
+    <row r="76" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E76" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="P75" s="2"/>
-    </row>
-    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>28</v>
-      </c>
-      <c r="B76" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" t="s">
-        <v>131</v>
-      </c>
-      <c r="D76">
-        <v>43</v>
-      </c>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
+      <c r="F76" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -2593,14 +2605,12 @@
         <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D77">
-        <v>44</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>62</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E77" s="10"/>
       <c r="F77" s="10"/>
       <c r="P77" s="2"/>
     </row>
@@ -2612,17 +2622,15 @@
         <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D78">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F78" s="10" t="s">
-        <v>130</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F78" s="10"/>
       <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2630,16 +2638,20 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D79">
-        <v>46</v>
-      </c>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
+        <v>45</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="P79" s="2"/>
     </row>
     <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2647,17 +2659,15 @@
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D80">
-        <v>47</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>62</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="P80" s="2"/>
     </row>
@@ -2666,52 +2676,50 @@
         <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D81">
+        <v>47</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81" s="10"/>
+      <c r="P81" s="2"/>
+    </row>
+    <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" t="s">
+        <v>152</v>
+      </c>
+      <c r="D82">
         <v>48</v>
       </c>
-      <c r="E81" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F81" s="10" t="s">
+      <c r="E82" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G82" t="s">
         <v>159</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H82" t="s">
         <v>160</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I82" t="s">
         <v>161</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J82" t="s">
         <v>162</v>
-      </c>
-      <c r="J81" t="s">
-        <v>163</v>
-      </c>
-      <c r="P81" s="2"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" t="s">
-        <v>143</v>
-      </c>
-      <c r="C82" t="s">
-        <v>154</v>
-      </c>
-      <c r="D82">
-        <v>49</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F82" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="P82" s="2"/>
     </row>
@@ -2720,19 +2728,19 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D83">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F83" t="s">
-        <v>160</v>
+        <v>168</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="P83" s="2"/>
     </row>
@@ -2741,19 +2749,19 @@
         <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D84">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F84" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P84" s="2"/>
     </row>
@@ -2762,19 +2770,19 @@
         <v>28</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C85" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D85">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F85" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="P85" s="2"/>
     </row>
@@ -2783,19 +2791,19 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D86">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P86" s="2"/>
     </row>
@@ -2804,19 +2812,19 @@
         <v>28</v>
       </c>
       <c r="B87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="D87">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="P87" s="2"/>
     </row>
@@ -2825,13 +2833,13 @@
         <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D88">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>33</v>
@@ -2839,9 +2847,6 @@
       <c r="F88" t="s">
         <v>44</v>
       </c>
-      <c r="G88" t="s">
-        <v>176</v>
-      </c>
       <c r="P88" s="2"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -2849,13 +2854,13 @@
         <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D89">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>33</v>
@@ -2863,6 +2868,9 @@
       <c r="F89" t="s">
         <v>44</v>
       </c>
+      <c r="G89" t="s">
+        <v>175</v>
+      </c>
       <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -2870,13 +2878,13 @@
         <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D90">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>33</v>
@@ -2891,19 +2899,19 @@
         <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D91">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F91" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="P91" s="2"/>
     </row>
@@ -2912,22 +2920,19 @@
         <v>28</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D92">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F92" t="s">
-        <v>106</v>
-      </c>
-      <c r="G92" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="P92" s="2"/>
     </row>
@@ -2936,19 +2941,22 @@
         <v>28</v>
       </c>
       <c r="B93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D93">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F93" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="G93" t="s">
+        <v>175</v>
       </c>
       <c r="P93" s="2"/>
     </row>
@@ -2957,19 +2965,19 @@
         <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D94">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P94" s="2"/>
     </row>
@@ -2978,19 +2986,19 @@
         <v>28</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D95">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F95" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="P95" s="2"/>
     </row>
@@ -2999,22 +3007,19 @@
         <v>28</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D96">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F96" t="s">
-        <v>62</v>
-      </c>
-      <c r="G96" t="s">
-        <v>176</v>
+        <v>61</v>
       </c>
       <c r="P96" s="2"/>
     </row>
@@ -3023,19 +3028,22 @@
         <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D97">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F97" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="G97" t="s">
+        <v>175</v>
       </c>
       <c r="P97" s="2"/>
     </row>
@@ -3044,64 +3052,70 @@
         <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D98">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P98" s="2"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99" t="s">
+        <v>179</v>
+      </c>
+      <c r="D99">
+        <v>65</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F99" t="s">
+        <v>61</v>
+      </c>
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C100" s="7" t="s">
+      <c r="P100" s="2"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C101" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P100" s="2"/>
-    </row>
-    <row r="101" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="P101" s="2"/>
+    </row>
+    <row r="102" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B102" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C102" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D101" s="9" t="s">
+      <c r="D102" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="P101" s="2"/>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" t="s">
-        <v>31</v>
-      </c>
-      <c r="C102" t="s">
-        <v>34</v>
-      </c>
-      <c r="D102" t="s">
-        <v>37</v>
-      </c>
+      <c r="E102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -3112,7 +3126,7 @@
         <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D103" t="s">
         <v>37</v>
@@ -3127,11 +3141,12 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D104" t="s">
-        <v>126</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P104" s="2"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -3141,10 +3156,10 @@
         <v>31</v>
       </c>
       <c r="C105" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D105" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -3155,7 +3170,7 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D106" t="s">
         <v>42</v>
@@ -3169,7 +3184,7 @@
         <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D107" t="s">
         <v>42</v>
@@ -3183,7 +3198,7 @@
         <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D108" t="s">
         <v>42</v>
@@ -3197,10 +3212,10 @@
         <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D109" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -3211,10 +3226,10 @@
         <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D110" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -3225,10 +3240,10 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D111" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -3239,10 +3254,10 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D112" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3253,10 +3268,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>60</v>
+        <v>212</v>
       </c>
       <c r="D113" t="s">
-        <v>80</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3267,10 +3282,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D114" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3281,10 +3296,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D115" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3295,10 +3310,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D116" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3309,10 +3324,10 @@
         <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D117" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3323,10 +3338,10 @@
         <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D118" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3337,10 +3352,10 @@
         <v>31</v>
       </c>
       <c r="C119" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D119" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3351,10 +3366,10 @@
         <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D120" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3362,13 +3377,13 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="D121" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,13 +3391,13 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="D122" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,13 +3405,13 @@
         <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C123" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D123" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,13 +3419,13 @@
         <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C124" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="D124" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,13 +3433,13 @@
         <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C125" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="D125" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3435,10 +3450,10 @@
         <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D126" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3446,13 +3461,13 @@
         <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C127" t="s">
-        <v>189</v>
+        <v>67</v>
       </c>
       <c r="D127" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3460,13 +3475,13 @@
         <v>28</v>
       </c>
       <c r="B128" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C128" t="s">
-        <v>190</v>
+        <v>64</v>
       </c>
       <c r="D128" t="s">
-        <v>210</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,13 +3489,13 @@
         <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C129" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="D129" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3488,13 +3503,13 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C130" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="D130" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3505,10 +3520,10 @@
         <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D131" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,10 +3534,10 @@
         <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D132" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3533,10 +3548,10 @@
         <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D133" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3547,10 +3562,10 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D134" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3558,13 +3573,13 @@
         <v>28</v>
       </c>
       <c r="B135" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="D135" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,13 +3587,13 @@
         <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="D136" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,13 +3601,13 @@
         <v>28</v>
       </c>
       <c r="B137" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C137" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D137" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,13 +3615,13 @@
         <v>28</v>
       </c>
       <c r="B138" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C138" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D138" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,13 +3629,13 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C139" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="D139" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3631,10 +3646,10 @@
         <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D140" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3642,13 +3657,13 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C141" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="D141" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,13 +3671,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C142" t="s">
+        <v>94</v>
+      </c>
+      <c r="D142" t="s">
         <v>204</v>
-      </c>
-      <c r="D142" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,13 +3685,13 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="D143" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,13 +3699,13 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="D144" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3704,7 +3719,7 @@
         <v>108</v>
       </c>
       <c r="D145" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3715,10 +3730,10 @@
         <v>31</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D146" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3728,11 +3743,11 @@
       <c r="B147" t="s">
         <v>31</v>
       </c>
-      <c r="C147" s="5" t="s">
-        <v>111</v>
+      <c r="C147" t="s">
+        <v>107</v>
       </c>
       <c r="D147" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,7 +3761,7 @@
         <v>104</v>
       </c>
       <c r="D148" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,13 +3769,13 @@
         <v>28</v>
       </c>
       <c r="B149" t="s">
-        <v>29</v>
-      </c>
-      <c r="C149" t="s">
-        <v>120</v>
+        <v>31</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D149" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,13 +3783,13 @@
         <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D150" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,10 +3800,10 @@
         <v>29</v>
       </c>
       <c r="C151" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D151" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,10 +3814,10 @@
         <v>29</v>
       </c>
       <c r="C152" t="s">
+        <v>120</v>
+      </c>
+      <c r="D152" t="s">
         <v>123</v>
-      </c>
-      <c r="D152" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3813,10 +3828,10 @@
         <v>29</v>
       </c>
       <c r="C153" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D153" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,10 +3842,10 @@
         <v>29</v>
       </c>
       <c r="C154" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D154" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3841,10 +3856,10 @@
         <v>29</v>
       </c>
       <c r="C155" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D155" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3852,13 +3867,13 @@
         <v>28</v>
       </c>
       <c r="B156" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C156" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D156" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,13 +3881,13 @@
         <v>28</v>
       </c>
       <c r="B157" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C157" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D157" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,13 +3895,13 @@
         <v>28</v>
       </c>
       <c r="B158" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C158" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D158" t="s">
-        <v>164</v>
+        <v>79</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,13 +3909,13 @@
         <v>28</v>
       </c>
       <c r="B159" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C159" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D159" t="s">
-        <v>165</v>
+        <v>51</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,13 +3923,13 @@
         <v>28</v>
       </c>
       <c r="B160" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C160" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D160" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3922,13 +3937,13 @@
         <v>28</v>
       </c>
       <c r="B161" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C161" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D161" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3936,13 +3951,13 @@
         <v>28</v>
       </c>
       <c r="B162" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C162" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D162" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,13 +3965,13 @@
         <v>28</v>
       </c>
       <c r="B163" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C163" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D163" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,13 +3979,13 @@
         <v>28</v>
       </c>
       <c r="B164" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C164" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D164" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3978,13 +3993,13 @@
         <v>28</v>
       </c>
       <c r="B165" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C165" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D165" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -3992,13 +4007,13 @@
         <v>28</v>
       </c>
       <c r="B166" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C166" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4006,13 +4021,13 @@
         <v>28</v>
       </c>
       <c r="B167" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C167" t="s">
+        <v>183</v>
+      </c>
+      <c r="D167" t="s">
         <v>186</v>
-      </c>
-      <c r="D167" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,13 +4035,13 @@
         <v>28</v>
       </c>
       <c r="B168" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C168" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="D168" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4034,10 +4049,10 @@
         <v>28</v>
       </c>
       <c r="B169" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="D169" t="s">
         <v>181</v>
@@ -4048,13 +4063,13 @@
         <v>28</v>
       </c>
       <c r="B170" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D170" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,13 +4077,13 @@
         <v>28</v>
       </c>
       <c r="B171" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D171" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,13 +4091,13 @@
         <v>28</v>
       </c>
       <c r="B172" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D172" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,13 +4105,13 @@
         <v>28</v>
       </c>
       <c r="B173" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D173" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4104,13 +4119,13 @@
         <v>28</v>
       </c>
       <c r="B174" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4118,18 +4133,46 @@
         <v>28</v>
       </c>
       <c r="B175" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D175" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>28</v>
+      </c>
+      <c r="B176" t="s">
+        <v>142</v>
+      </c>
+      <c r="C176" t="s">
+        <v>178</v>
+      </c>
+      <c r="D176" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>28</v>
+      </c>
+      <c r="B177" t="s">
+        <v>142</v>
+      </c>
       <c r="C177" t="s">
-        <v>127</v>
+        <v>179</v>
+      </c>
+      <c r="D177" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mon 7 Nov 2016 18:19 commit by king
Issue Fix :
- Remove Hashset usage in entities
- PacketFormat correction
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="214">
   <si>
     <t>Meaning</t>
   </si>
@@ -502,9 +502,6 @@
   </si>
   <si>
     <t>Expression</t>
-  </si>
-  <si>
-    <t>Enabled</t>
   </si>
   <si>
     <t>Timeout</t>
@@ -1066,7 +1063,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1076,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="C73" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1595,7 @@
         <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E32" t="s">
         <v>54</v>
@@ -1627,10 +1624,10 @@
         <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
@@ -1930,7 +1927,7 @@
         <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s">
         <v>70</v>
@@ -1968,10 +1965,10 @@
         <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E49" t="s">
         <v>70</v>
@@ -1985,16 +1982,16 @@
         <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E50" t="s">
         <v>70</v>
       </c>
       <c r="F50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G50" t="s">
         <v>61</v>
@@ -2260,7 +2257,7 @@
         <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E62" t="s">
         <v>70</v>
@@ -2305,10 +2302,10 @@
         <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E63" t="s">
         <v>70</v>
@@ -2323,16 +2320,16 @@
         <v>142</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
         <v>70</v>
       </c>
       <c r="F64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G64" t="s">
         <v>61</v>
@@ -2490,7 +2487,7 @@
         <v>121</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E71" t="s">
         <v>44</v>
@@ -2508,7 +2505,7 @@
         <v>122</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>118</v>
@@ -2529,7 +2526,7 @@
         <v>119</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E73" t="s">
         <v>105</v>
@@ -2547,7 +2544,7 @@
         <v>120</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>118</v>
@@ -2565,10 +2562,10 @@
         <v>142</v>
       </c>
       <c r="C75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E75" t="s">
         <v>61</v>
@@ -2584,10 +2581,10 @@
         <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>118</v>
@@ -2716,10 +2713,10 @@
         <v>160</v>
       </c>
       <c r="I82" t="s">
+        <v>86</v>
+      </c>
+      <c r="J82" t="s">
         <v>161</v>
-      </c>
-      <c r="J82" t="s">
-        <v>162</v>
       </c>
       <c r="P82" s="2"/>
     </row>
@@ -2737,7 +2734,7 @@
         <v>49</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>158</v>
@@ -2758,7 +2755,7 @@
         <v>50</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F84" t="s">
         <v>159</v>
@@ -2779,7 +2776,7 @@
         <v>51</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F85" t="s">
         <v>160</v>
@@ -2800,10 +2797,10 @@
         <v>52</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P86" s="2"/>
     </row>
@@ -2821,10 +2818,10 @@
         <v>53</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P87" s="2"/>
     </row>
@@ -2836,7 +2833,7 @@
         <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D88">
         <v>54</v>
@@ -2857,7 +2854,7 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D89">
         <v>55</v>
@@ -2869,7 +2866,7 @@
         <v>44</v>
       </c>
       <c r="G89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P89" s="2"/>
     </row>
@@ -2881,7 +2878,7 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D90">
         <v>56</v>
@@ -2902,7 +2899,7 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D91">
         <v>57</v>
@@ -2923,7 +2920,7 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D92">
         <v>58</v>
@@ -2944,7 +2941,7 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D93">
         <v>59</v>
@@ -2956,7 +2953,7 @@
         <v>105</v>
       </c>
       <c r="G93" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P93" s="2"/>
     </row>
@@ -2968,7 +2965,7 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D94">
         <v>60</v>
@@ -2989,7 +2986,7 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D95">
         <v>61</v>
@@ -3010,7 +3007,7 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D96">
         <v>62</v>
@@ -3031,7 +3028,7 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D97">
         <v>63</v>
@@ -3043,7 +3040,7 @@
         <v>61</v>
       </c>
       <c r="G97" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P97" s="2"/>
     </row>
@@ -3055,7 +3052,7 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D98">
         <v>64</v>
@@ -3076,7 +3073,7 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D99">
         <v>65</v>
@@ -3257,7 +3254,7 @@
         <v>55</v>
       </c>
       <c r="D112" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,10 +3265,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D113" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3492,7 +3489,7 @@
         <v>142</v>
       </c>
       <c r="C129" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D129" t="s">
         <v>85</v>
@@ -3506,10 +3503,10 @@
         <v>142</v>
       </c>
       <c r="C130" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D130" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,7 +3674,7 @@
         <v>94</v>
       </c>
       <c r="D142" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3688,7 +3685,7 @@
         <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3702,10 +3699,10 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D144" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,7 +3884,7 @@
         <v>128</v>
       </c>
       <c r="D157" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,7 +3926,7 @@
         <v>152</v>
       </c>
       <c r="D160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,7 +3940,7 @@
         <v>153</v>
       </c>
       <c r="D161" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,7 +3954,7 @@
         <v>154</v>
       </c>
       <c r="D162" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,7 +3968,7 @@
         <v>155</v>
       </c>
       <c r="D163" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,7 +3982,7 @@
         <v>156</v>
       </c>
       <c r="D164" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,7 +3996,7 @@
         <v>157</v>
       </c>
       <c r="D165" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,10 +4007,10 @@
         <v>142</v>
       </c>
       <c r="C166" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D166" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,10 +4021,10 @@
         <v>142</v>
       </c>
       <c r="C167" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D167" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,10 +4035,10 @@
         <v>142</v>
       </c>
       <c r="C168" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D168" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,10 +4049,10 @@
         <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D169" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,10 +4063,10 @@
         <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D170" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4080,10 +4077,10 @@
         <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D171" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4094,10 +4091,10 @@
         <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D172" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4108,10 +4105,10 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D173" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,10 +4119,10 @@
         <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D174" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4136,10 +4133,10 @@
         <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D175" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4150,10 +4147,10 @@
         <v>142</v>
       </c>
       <c r="C176" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D176" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4164,10 +4161,10 @@
         <v>142</v>
       </c>
       <c r="C177" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D177" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mon 7 Nov 2016 19:09 commit by king
Functionality :
- Adds SensorActuatorResponse Update&Delete packet format

Issue Fix :
- SensorActuatorResponse expression without sensor can be accepted. Now
no longer able.
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="219">
   <si>
     <t>Meaning</t>
   </si>
@@ -661,6 +661,21 @@
   </si>
   <si>
     <t>9b</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseUpdate</t>
+  </si>
+  <si>
+    <t>48b</t>
+  </si>
+  <si>
+    <t>48c</t>
+  </si>
+  <si>
+    <t>SensorActuatorResponseDelete</t>
+  </si>
+  <si>
+    <t>48a</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1078,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1071,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q179"/>
+  <dimension ref="A1:Q181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,8 +2712,8 @@
       <c r="C82" t="s">
         <v>152</v>
       </c>
-      <c r="D82">
-        <v>48</v>
+      <c r="D82" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>61</v>
@@ -2720,7 +2735,7 @@
       </c>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>28</v>
       </c>
@@ -2728,20 +2743,35 @@
         <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>153</v>
-      </c>
-      <c r="D83">
-        <v>49</v>
+        <v>214</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F83" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>158</v>
       </c>
+      <c r="H83" t="s">
+        <v>159</v>
+      </c>
+      <c r="I83" t="s">
+        <v>160</v>
+      </c>
+      <c r="J83" t="s">
+        <v>86</v>
+      </c>
+      <c r="K83" t="s">
+        <v>161</v>
+      </c>
       <c r="P83" s="2"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -2749,17 +2779,16 @@
         <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>154</v>
-      </c>
-      <c r="D84">
-        <v>50</v>
+        <v>217</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F84" t="s">
-        <v>159</v>
-      </c>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
       <c r="P84" s="2"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -2770,16 +2799,16 @@
         <v>142</v>
       </c>
       <c r="C85" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D85">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F85" t="s">
-        <v>160</v>
+      <c r="F85" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="P85" s="2"/>
     </row>
@@ -2791,16 +2820,16 @@
         <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D86">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F86" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="P86" s="2"/>
     </row>
@@ -2812,16 +2841,16 @@
         <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D87">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F87" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="P87" s="2"/>
     </row>
@@ -2833,16 +2862,16 @@
         <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D88">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F88" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="P88" s="2"/>
     </row>
@@ -2854,19 +2883,16 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D89">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F89" t="s">
-        <v>44</v>
-      </c>
-      <c r="G89" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="P89" s="2"/>
     </row>
@@ -2878,10 +2904,10 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D90">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>33</v>
@@ -2899,10 +2925,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D91">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>33</v>
@@ -2910,6 +2936,9 @@
       <c r="F91" t="s">
         <v>44</v>
       </c>
+      <c r="G91" t="s">
+        <v>174</v>
+      </c>
       <c r="P91" s="2"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -2920,16 +2949,16 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="D92">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F92" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="P92" s="2"/>
     </row>
@@ -2941,19 +2970,16 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="D93">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F93" t="s">
-        <v>105</v>
-      </c>
-      <c r="G93" t="s">
-        <v>174</v>
+        <v>44</v>
       </c>
       <c r="P93" s="2"/>
     </row>
@@ -2965,10 +2991,10 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D94">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>33</v>
@@ -2986,10 +3012,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D95">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>33</v>
@@ -2997,6 +3023,9 @@
       <c r="F95" t="s">
         <v>105</v>
       </c>
+      <c r="G95" t="s">
+        <v>174</v>
+      </c>
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -3007,16 +3036,16 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D96">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F96" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="P96" s="2"/>
     </row>
@@ -3028,19 +3057,16 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D97">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F97" t="s">
-        <v>61</v>
-      </c>
-      <c r="G97" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
       <c r="P97" s="2"/>
     </row>
@@ -3052,10 +3078,10 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D98">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
@@ -3073,10 +3099,10 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D99">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
@@ -3084,65 +3110,80 @@
       <c r="F99" t="s">
         <v>61</v>
       </c>
+      <c r="G99" t="s">
+        <v>174</v>
+      </c>
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" t="s">
+        <v>142</v>
+      </c>
+      <c r="C100" t="s">
+        <v>177</v>
+      </c>
+      <c r="D100">
+        <v>64</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F100" t="s">
+        <v>61</v>
+      </c>
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C101" s="7" t="s">
+      <c r="A101" t="s">
+        <v>28</v>
+      </c>
+      <c r="B101" t="s">
+        <v>142</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
+      </c>
+      <c r="D101">
+        <v>65</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F101" t="s">
+        <v>61</v>
+      </c>
+      <c r="P101" s="2"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P102" s="2"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C103" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P101" s="2"/>
-    </row>
-    <row r="102" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="P103" s="2"/>
+    </row>
+    <row r="104" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B104" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C104" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D102" s="9" t="s">
+      <c r="D104" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="P102" s="2"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>28</v>
-      </c>
-      <c r="B103" t="s">
-        <v>31</v>
-      </c>
-      <c r="C103" t="s">
-        <v>34</v>
-      </c>
-      <c r="D103" t="s">
-        <v>37</v>
-      </c>
-      <c r="P103" s="2"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>28</v>
-      </c>
-      <c r="B104" t="s">
-        <v>31</v>
-      </c>
-      <c r="C104" t="s">
-        <v>36</v>
-      </c>
-      <c r="D104" t="s">
-        <v>37</v>
-      </c>
+      <c r="E104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
       <c r="P104" s="2"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -3153,11 +3194,12 @@
         <v>31</v>
       </c>
       <c r="C105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D105" t="s">
-        <v>125</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P105" s="2"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -3167,11 +3209,12 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D106" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P106" s="2"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -3181,10 +3224,10 @@
         <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D107" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -3195,7 +3238,7 @@
         <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D108" t="s">
         <v>42</v>
@@ -3209,7 +3252,7 @@
         <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D109" t="s">
         <v>42</v>
@@ -3223,10 +3266,10 @@
         <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D110" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -3237,10 +3280,10 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D111" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -3251,10 +3294,10 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D112" t="s">
-        <v>210</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3265,10 +3308,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="D113" t="s">
-        <v>209</v>
+        <v>51</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3279,10 +3322,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D114" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3293,10 +3336,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="D115" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3307,10 +3350,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D116" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,7 +3364,7 @@
         <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D117" t="s">
         <v>79</v>
@@ -3335,10 +3378,10 @@
         <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D118" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3349,10 +3392,10 @@
         <v>31</v>
       </c>
       <c r="C119" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D119" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3363,10 +3406,10 @@
         <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D120" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3377,10 +3420,10 @@
         <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D121" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3391,10 +3434,10 @@
         <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="D122" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,13 +3445,13 @@
         <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="D123" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3416,13 +3459,13 @@
         <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="D124" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3433,7 +3476,7 @@
         <v>142</v>
       </c>
       <c r="C125" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D125" t="s">
         <v>85</v>
@@ -3444,10 +3487,10 @@
         <v>28</v>
       </c>
       <c r="B126" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C126" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="D126" t="s">
         <v>85</v>
@@ -3458,10 +3501,10 @@
         <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C127" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="D127" t="s">
         <v>85</v>
@@ -3475,10 +3518,10 @@
         <v>31</v>
       </c>
       <c r="C128" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D128" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3486,10 +3529,10 @@
         <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>187</v>
+        <v>67</v>
       </c>
       <c r="D129" t="s">
         <v>85</v>
@@ -3500,13 +3543,13 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>188</v>
+        <v>64</v>
       </c>
       <c r="D130" t="s">
-        <v>208</v>
+        <v>102</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3514,13 +3557,13 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C131" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="D131" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3528,13 +3571,13 @@
         <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C132" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="D132" t="s">
-        <v>51</v>
+        <v>208</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3545,10 +3588,10 @@
         <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D133" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3559,10 +3602,10 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D134" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3573,7 +3616,7 @@
         <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D135" t="s">
         <v>85</v>
@@ -3587,10 +3630,10 @@
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D136" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,10 +3641,10 @@
         <v>28</v>
       </c>
       <c r="B137" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="D137" t="s">
         <v>85</v>
@@ -3612,13 +3655,13 @@
         <v>28</v>
       </c>
       <c r="B138" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="D138" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3629,7 +3672,7 @@
         <v>142</v>
       </c>
       <c r="C139" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D139" t="s">
         <v>85</v>
@@ -3640,10 +3683,10 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="D140" t="s">
         <v>85</v>
@@ -3654,10 +3697,10 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C141" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="D141" t="s">
         <v>85</v>
@@ -3671,10 +3714,10 @@
         <v>31</v>
       </c>
       <c r="C142" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D142" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3682,10 +3725,10 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C143" t="s">
-        <v>201</v>
+        <v>93</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3696,13 +3739,13 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C144" t="s">
-        <v>202</v>
+        <v>94</v>
       </c>
       <c r="D144" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3710,13 +3753,13 @@
         <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C145" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="D145" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,13 +3767,13 @@
         <v>28</v>
       </c>
       <c r="B146" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="D146" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3741,10 +3784,10 @@
         <v>31</v>
       </c>
       <c r="C147" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D147" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,10 +3798,10 @@
         <v>31</v>
       </c>
       <c r="C148" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D148" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,11 +3811,11 @@
       <c r="B149" t="s">
         <v>31</v>
       </c>
-      <c r="C149" s="5" t="s">
-        <v>110</v>
+      <c r="C149" t="s">
+        <v>107</v>
       </c>
       <c r="D149" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,10 +3826,10 @@
         <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D150" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3794,13 +3837,13 @@
         <v>28</v>
       </c>
       <c r="B151" t="s">
-        <v>29</v>
-      </c>
-      <c r="C151" t="s">
-        <v>119</v>
+        <v>31</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D151" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3808,13 +3851,13 @@
         <v>28</v>
       </c>
       <c r="B152" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C152" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="D152" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3825,10 +3868,10 @@
         <v>29</v>
       </c>
       <c r="C153" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D153" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3839,10 +3882,10 @@
         <v>29</v>
       </c>
       <c r="C154" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3853,10 +3896,10 @@
         <v>29</v>
       </c>
       <c r="C155" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D155" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3867,10 +3910,10 @@
         <v>29</v>
       </c>
       <c r="C156" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D156" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3881,10 +3924,10 @@
         <v>29</v>
       </c>
       <c r="C157" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D157" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3892,13 +3935,13 @@
         <v>28</v>
       </c>
       <c r="B158" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C158" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D158" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3906,13 +3949,13 @@
         <v>28</v>
       </c>
       <c r="B159" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C159" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D159" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3923,10 +3966,10 @@
         <v>142</v>
       </c>
       <c r="C160" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D160" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3937,10 +3980,10 @@
         <v>142</v>
       </c>
       <c r="C161" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D161" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3951,10 +3994,10 @@
         <v>142</v>
       </c>
       <c r="C162" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D162" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3965,10 +4008,10 @@
         <v>142</v>
       </c>
       <c r="C163" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D163" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3979,7 +4022,7 @@
         <v>142</v>
       </c>
       <c r="C164" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D164" t="s">
         <v>163</v>
@@ -3993,10 +4036,10 @@
         <v>142</v>
       </c>
       <c r="C165" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D165" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,10 +4050,10 @@
         <v>142</v>
       </c>
       <c r="C166" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D166" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,10 +4064,10 @@
         <v>142</v>
       </c>
       <c r="C167" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D167" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,7 +4078,7 @@
         <v>142</v>
       </c>
       <c r="C168" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D168" t="s">
         <v>185</v>
@@ -4049,10 +4092,10 @@
         <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D169" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4063,10 +4106,10 @@
         <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="D170" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,10 +4120,10 @@
         <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="D171" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,7 +4134,7 @@
         <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D172" t="s">
         <v>179</v>
@@ -4105,10 +4148,10 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D173" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4119,10 +4162,10 @@
         <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D174" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,10 +4176,10 @@
         <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D175" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,7 +4190,7 @@
         <v>142</v>
       </c>
       <c r="C176" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D176" t="s">
         <v>186</v>
@@ -4161,14 +4204,42 @@
         <v>142</v>
       </c>
       <c r="C177" t="s">
+        <v>176</v>
+      </c>
+      <c r="D177" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>28</v>
+      </c>
+      <c r="B178" t="s">
+        <v>142</v>
+      </c>
+      <c r="C178" t="s">
+        <v>177</v>
+      </c>
+      <c r="D178" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>28</v>
+      </c>
+      <c r="B179" t="s">
+        <v>142</v>
+      </c>
+      <c r="C179" t="s">
         <v>178</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D179" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C179" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tue 8 Nov 2016 17:58 commit by king
Issue Fix :
- Sensor actuator response time not updating

Functionality :
- GWTServer added ActuatorSetControlType
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="225">
   <si>
     <t>Meaning</t>
   </si>
@@ -676,6 +676,24 @@
   </si>
   <si>
     <t>48a</t>
+  </si>
+  <si>
+    <t>RESPONSE_NOT_EXIST/ACTUATOR_ALREADY_USED/EXPRESSION_ERROR/ERROR/OK</t>
+  </si>
+  <si>
+    <t>ActuatorSetControlType</t>
+  </si>
+  <si>
+    <t>45b</t>
+  </si>
+  <si>
+    <t>45a</t>
+  </si>
+  <si>
+    <t>ControlType</t>
+  </si>
+  <si>
+    <t>ACTUATOR_NOT_EXIST/ERROR/OK</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q181"/>
+  <dimension ref="A1:Q185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,8 +2673,8 @@
       <c r="C79" t="s">
         <v>128</v>
       </c>
-      <c r="D79">
-        <v>45</v>
+      <c r="D79" s="12" t="s">
+        <v>222</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>61</v>
@@ -2674,13 +2692,17 @@
         <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>150</v>
-      </c>
-      <c r="D80">
-        <v>46</v>
-      </c>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
+        <v>220</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="P80" s="2"/>
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2691,14 +2713,12 @@
         <v>142</v>
       </c>
       <c r="C81" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D81">
-        <v>47</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>61</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E81" s="10"/>
       <c r="F81" s="10"/>
       <c r="P81" s="2"/>
     </row>
@@ -2710,29 +2730,15 @@
         <v>142</v>
       </c>
       <c r="C82" t="s">
-        <v>152</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>218</v>
+        <v>151</v>
+      </c>
+      <c r="D82">
+        <v>47</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F82" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="G82" t="s">
-        <v>159</v>
-      </c>
-      <c r="H82" t="s">
-        <v>160</v>
-      </c>
-      <c r="I82" t="s">
-        <v>86</v>
-      </c>
-      <c r="J82" t="s">
-        <v>161</v>
-      </c>
+      <c r="F82" s="10"/>
       <c r="P82" s="2"/>
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,30 +2749,27 @@
         <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>167</v>
+        <v>61</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G83" s="10" t="s">
         <v>158</v>
       </c>
+      <c r="G83" t="s">
+        <v>159</v>
+      </c>
       <c r="H83" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I83" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="J83" t="s">
-        <v>86</v>
-      </c>
-      <c r="K83" t="s">
         <v>161</v>
       </c>
       <c r="P83" s="2"/>
@@ -2779,19 +2782,35 @@
         <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
+      <c r="F84" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H84" t="s">
+        <v>159</v>
+      </c>
+      <c r="I84" t="s">
+        <v>160</v>
+      </c>
+      <c r="J84" t="s">
+        <v>86</v>
+      </c>
+      <c r="K84" t="s">
+        <v>161</v>
+      </c>
       <c r="P84" s="2"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
@@ -2799,17 +2818,16 @@
         <v>142</v>
       </c>
       <c r="C85" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85">
-        <v>49</v>
+        <v>217</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F85" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
       <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -2820,16 +2838,16 @@
         <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D86">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F86" t="s">
-        <v>159</v>
+      <c r="F86" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="P86" s="2"/>
     </row>
@@ -2841,16 +2859,16 @@
         <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D87">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P87" s="2"/>
     </row>
@@ -2862,16 +2880,16 @@
         <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D88">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F88" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="P88" s="2"/>
     </row>
@@ -2883,16 +2901,16 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D89">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F89" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P89" s="2"/>
     </row>
@@ -2904,16 +2922,16 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D90">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F90" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="P90" s="2"/>
     </row>
@@ -2925,10 +2943,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D91">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>33</v>
@@ -2936,9 +2954,6 @@
       <c r="F91" t="s">
         <v>44</v>
       </c>
-      <c r="G91" t="s">
-        <v>174</v>
-      </c>
       <c r="P91" s="2"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -2949,10 +2964,10 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D92">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>33</v>
@@ -2960,6 +2975,9 @@
       <c r="F92" t="s">
         <v>44</v>
       </c>
+      <c r="G92" t="s">
+        <v>174</v>
+      </c>
       <c r="P92" s="2"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -2970,10 +2988,10 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D93">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>33</v>
@@ -2991,16 +3009,16 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D94">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F94" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="P94" s="2"/>
     </row>
@@ -3012,10 +3030,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D95">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>33</v>
@@ -3023,9 +3041,6 @@
       <c r="F95" t="s">
         <v>105</v>
       </c>
-      <c r="G95" t="s">
-        <v>174</v>
-      </c>
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -3036,10 +3051,10 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D96">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
@@ -3047,6 +3062,9 @@
       <c r="F96" t="s">
         <v>105</v>
       </c>
+      <c r="G96" t="s">
+        <v>174</v>
+      </c>
       <c r="P96" s="2"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -3057,10 +3075,10 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D97">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
@@ -3078,16 +3096,16 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D98">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="P98" s="2"/>
     </row>
@@ -3099,10 +3117,10 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D99">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
@@ -3110,9 +3128,6 @@
       <c r="F99" t="s">
         <v>61</v>
       </c>
-      <c r="G99" t="s">
-        <v>174</v>
-      </c>
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -3123,10 +3138,10 @@
         <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D100">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>33</v>
@@ -3134,6 +3149,9 @@
       <c r="F100" t="s">
         <v>61</v>
       </c>
+      <c r="G100" t="s">
+        <v>174</v>
+      </c>
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -3144,10 +3162,10 @@
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D101">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>33</v>
@@ -3158,47 +3176,53 @@
       <c r="P101" s="2"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>28</v>
+      </c>
+      <c r="B102" t="s">
+        <v>142</v>
+      </c>
+      <c r="C102" t="s">
+        <v>178</v>
+      </c>
+      <c r="D102">
+        <v>65</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F102" t="s">
+        <v>61</v>
+      </c>
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C103" s="7" t="s">
+      <c r="P103" s="2"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C104" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P103" s="2"/>
-    </row>
-    <row r="104" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="P104" s="2"/>
+    </row>
+    <row r="105" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B105" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C105" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D104" s="9" t="s">
+      <c r="D105" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="P104" s="2"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>28</v>
-      </c>
-      <c r="B105" t="s">
-        <v>31</v>
-      </c>
-      <c r="C105" t="s">
-        <v>34</v>
-      </c>
-      <c r="D105" t="s">
-        <v>37</v>
-      </c>
+      <c r="E105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
       <c r="P105" s="2"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -3209,7 +3233,7 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D106" t="s">
         <v>37</v>
@@ -3224,11 +3248,12 @@
         <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D107" t="s">
-        <v>125</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P107" s="2"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
@@ -3238,10 +3263,10 @@
         <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D108" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -3252,7 +3277,7 @@
         <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D109" t="s">
         <v>42</v>
@@ -3266,7 +3291,7 @@
         <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D110" t="s">
         <v>42</v>
@@ -3280,7 +3305,7 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D111" t="s">
         <v>42</v>
@@ -3294,10 +3319,10 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D112" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,10 +3333,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D113" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3322,10 +3347,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D114" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3336,10 +3361,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="D115" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,10 +3375,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>52</v>
+        <v>211</v>
       </c>
       <c r="D116" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3364,10 +3389,10 @@
         <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D117" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,7 +3403,7 @@
         <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D118" t="s">
         <v>79</v>
@@ -3392,7 +3417,7 @@
         <v>31</v>
       </c>
       <c r="C119" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D119" t="s">
         <v>79</v>
@@ -3406,10 +3431,10 @@
         <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D120" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3420,10 +3445,10 @@
         <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D121" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3434,10 +3459,10 @@
         <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D122" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,10 +3473,10 @@
         <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D123" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,10 +3487,10 @@
         <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="D124" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3473,13 +3498,13 @@
         <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="D125" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3490,7 +3515,7 @@
         <v>142</v>
       </c>
       <c r="C126" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D126" t="s">
         <v>85</v>
@@ -3504,7 +3529,7 @@
         <v>142</v>
       </c>
       <c r="C127" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D127" t="s">
         <v>85</v>
@@ -3515,10 +3540,10 @@
         <v>28</v>
       </c>
       <c r="B128" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C128" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="D128" t="s">
         <v>85</v>
@@ -3532,7 +3557,7 @@
         <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D129" t="s">
         <v>85</v>
@@ -3546,10 +3571,10 @@
         <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D130" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,13 +3582,13 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>187</v>
+        <v>64</v>
       </c>
       <c r="D131" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,10 +3599,10 @@
         <v>142</v>
       </c>
       <c r="C132" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D132" t="s">
-        <v>208</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,13 +3610,13 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C133" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
       <c r="D133" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3602,10 +3627,10 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D134" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,10 +3641,10 @@
         <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D135" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,10 +3655,10 @@
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D136" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3644,10 +3669,10 @@
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D137" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,10 +3683,10 @@
         <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D138" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3669,13 +3694,13 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="D139" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3686,7 +3711,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D140" t="s">
         <v>85</v>
@@ -3700,7 +3725,7 @@
         <v>142</v>
       </c>
       <c r="C141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D141" t="s">
         <v>85</v>
@@ -3711,10 +3736,10 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C142" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="D142" t="s">
         <v>85</v>
@@ -3728,7 +3753,7 @@
         <v>31</v>
       </c>
       <c r="C143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3742,10 +3767,10 @@
         <v>31</v>
       </c>
       <c r="C144" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D144" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3753,13 +3778,13 @@
         <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C145" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="D145" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3770,10 +3795,10 @@
         <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D146" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3781,13 +3806,13 @@
         <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C147" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="D147" t="s">
-        <v>37</v>
+        <v>207</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,10 +3823,10 @@
         <v>31</v>
       </c>
       <c r="C148" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D148" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,7 +3837,7 @@
         <v>31</v>
       </c>
       <c r="C149" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D149" t="s">
         <v>149</v>
@@ -3826,10 +3851,10 @@
         <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D150" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3839,11 +3864,11 @@
       <c r="B151" t="s">
         <v>31</v>
       </c>
-      <c r="C151" s="5" t="s">
-        <v>110</v>
+      <c r="C151" t="s">
+        <v>104</v>
       </c>
       <c r="D151" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3853,8 +3878,8 @@
       <c r="B152" t="s">
         <v>31</v>
       </c>
-      <c r="C152" t="s">
-        <v>103</v>
+      <c r="C152" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D152" t="s">
         <v>109</v>
@@ -3865,13 +3890,13 @@
         <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D153" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,7 +3907,7 @@
         <v>29</v>
       </c>
       <c r="C154" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D154" t="s">
         <v>123</v>
@@ -3896,10 +3921,10 @@
         <v>29</v>
       </c>
       <c r="C155" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D155" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3910,7 +3935,7 @@
         <v>29</v>
       </c>
       <c r="C156" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D156" t="s">
         <v>124</v>
@@ -3924,10 +3949,10 @@
         <v>29</v>
       </c>
       <c r="C157" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D157" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3938,10 +3963,10 @@
         <v>29</v>
       </c>
       <c r="C158" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D158" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3952,10 +3977,10 @@
         <v>29</v>
       </c>
       <c r="C159" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D159" t="s">
-        <v>169</v>
+        <v>51</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,13 +3988,13 @@
         <v>28</v>
       </c>
       <c r="B160" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C160" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D160" t="s">
-        <v>79</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,13 +4002,13 @@
         <v>28</v>
       </c>
       <c r="B161" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C161" t="s">
-        <v>151</v>
+        <v>220</v>
       </c>
       <c r="D161" t="s">
-        <v>51</v>
+        <v>224</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3994,10 +4019,10 @@
         <v>142</v>
       </c>
       <c r="C162" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D162" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,10 +4033,10 @@
         <v>142</v>
       </c>
       <c r="C163" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D163" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,10 +4047,10 @@
         <v>142</v>
       </c>
       <c r="C164" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D164" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4036,10 +4061,10 @@
         <v>142</v>
       </c>
       <c r="C165" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="D165" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4050,7 +4075,7 @@
         <v>142</v>
       </c>
       <c r="C166" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="D166" t="s">
         <v>163</v>
@@ -4064,10 +4089,10 @@
         <v>142</v>
       </c>
       <c r="C167" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D167" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4078,10 +4103,10 @@
         <v>142</v>
       </c>
       <c r="C168" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="D168" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4092,10 +4117,10 @@
         <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D169" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4106,10 +4131,10 @@
         <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D170" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4120,10 +4145,10 @@
         <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D171" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4134,10 +4159,10 @@
         <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D172" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4148,10 +4173,10 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="D173" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4162,10 +4187,10 @@
         <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D174" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4176,7 +4201,7 @@
         <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="D175" t="s">
         <v>180</v>
@@ -4190,10 +4215,10 @@
         <v>142</v>
       </c>
       <c r="C176" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D176" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4204,10 +4229,10 @@
         <v>142</v>
       </c>
       <c r="C177" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D177" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,10 +4243,10 @@
         <v>142</v>
       </c>
       <c r="C178" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D178" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,14 +4257,70 @@
         <v>142</v>
       </c>
       <c r="C179" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D179" t="s">
         <v>180</v>
       </c>
     </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>28</v>
+      </c>
+      <c r="B180" t="s">
+        <v>142</v>
+      </c>
+      <c r="C180" t="s">
+        <v>175</v>
+      </c>
+      <c r="D180" t="s">
+        <v>186</v>
+      </c>
+    </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>28</v>
+      </c>
+      <c r="B181" t="s">
+        <v>142</v>
+      </c>
       <c r="C181" t="s">
+        <v>176</v>
+      </c>
+      <c r="D181" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>28</v>
+      </c>
+      <c r="B182" t="s">
+        <v>142</v>
+      </c>
+      <c r="C182" t="s">
+        <v>177</v>
+      </c>
+      <c r="D182" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>28</v>
+      </c>
+      <c r="B183" t="s">
+        <v>142</v>
+      </c>
+      <c r="C183" t="s">
+        <v>178</v>
+      </c>
+      <c r="D183" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tue 8 Nov 2016 23:27 commit by king
Functionality :
- Added GetController/Actuator/SensorSubscription packet in GWTServer
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="229">
   <si>
     <t>Meaning</t>
   </si>
@@ -694,12 +699,24 @@
   </si>
   <si>
     <t>ACTUATOR_NOT_EXIST/ERROR/OK</t>
+  </si>
+  <si>
+    <t>UserGetSubscribedControllers</t>
+  </si>
+  <si>
+    <t>UserGetSubscribedSensors</t>
+  </si>
+  <si>
+    <t>UserGetSubscribedActuators</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1096,7 +1113,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1104,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q185"/>
+  <dimension ref="A1:Q191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3030,7 +3047,7 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>225</v>
       </c>
       <c r="D95">
         <v>58</v>
@@ -3038,9 +3055,6 @@
       <c r="E95" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F95" t="s">
-        <v>105</v>
-      </c>
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -3051,10 +3065,10 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D96">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
@@ -3062,9 +3076,6 @@
       <c r="F96" t="s">
         <v>105</v>
       </c>
-      <c r="G96" t="s">
-        <v>174</v>
-      </c>
       <c r="P96" s="2"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -3075,10 +3086,10 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D97">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
@@ -3086,6 +3097,9 @@
       <c r="F97" t="s">
         <v>105</v>
       </c>
+      <c r="G97" t="s">
+        <v>174</v>
+      </c>
       <c r="P97" s="2"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -3096,10 +3110,10 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D98">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
@@ -3117,16 +3131,16 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D99">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F99" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="P99" s="2"/>
     </row>
@@ -3138,20 +3152,14 @@
         <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D100">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F100" t="s">
-        <v>61</v>
-      </c>
-      <c r="G100" t="s">
-        <v>174</v>
-      </c>
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -3162,10 +3170,10 @@
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D101">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>33</v>
@@ -3183,10 +3191,10 @@
         <v>142</v>
       </c>
       <c r="C102" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D102">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>33</v>
@@ -3194,80 +3202,99 @@
       <c r="F102" t="s">
         <v>61</v>
       </c>
+      <c r="G102" t="s">
+        <v>174</v>
+      </c>
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>28</v>
+      </c>
+      <c r="B103" t="s">
+        <v>142</v>
+      </c>
+      <c r="C103" t="s">
+        <v>177</v>
+      </c>
+      <c r="D103">
+        <v>65</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F103" t="s">
+        <v>61</v>
+      </c>
       <c r="P103" s="2"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C104" s="7" t="s">
+      <c r="A104" t="s">
+        <v>28</v>
+      </c>
+      <c r="B104" t="s">
+        <v>142</v>
+      </c>
+      <c r="C104" t="s">
+        <v>178</v>
+      </c>
+      <c r="D104">
+        <v>67</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F104" t="s">
+        <v>61</v>
+      </c>
+      <c r="P104" s="2"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>28</v>
+      </c>
+      <c r="B105" t="s">
+        <v>142</v>
+      </c>
+      <c r="C105" t="s">
+        <v>227</v>
+      </c>
+      <c r="D105">
+        <v>68</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P105" s="2"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P106" s="2"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C107" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P104" s="2"/>
-    </row>
-    <row r="105" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+      <c r="P107" s="2"/>
+    </row>
+    <row r="108" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B108" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C108" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D105" s="9" t="s">
+      <c r="D108" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-      <c r="P105" s="2"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>28</v>
-      </c>
-      <c r="B106" t="s">
-        <v>31</v>
-      </c>
-      <c r="C106" t="s">
-        <v>34</v>
-      </c>
-      <c r="D106" t="s">
-        <v>37</v>
-      </c>
-      <c r="P106" s="2"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" t="s">
-        <v>31</v>
-      </c>
-      <c r="C107" t="s">
-        <v>36</v>
-      </c>
-      <c r="D107" t="s">
-        <v>37</v>
-      </c>
-      <c r="P107" s="2"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" t="s">
-        <v>35</v>
-      </c>
-      <c r="D108" t="s">
-        <v>125</v>
-      </c>
+      <c r="E108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="P108" s="2"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -3277,11 +3304,12 @@
         <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D109" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P109" s="2"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
@@ -3291,11 +3319,12 @@
         <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D110" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P110" s="2"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
@@ -3305,10 +3334,10 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D111" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -3319,7 +3348,7 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D112" t="s">
         <v>42</v>
@@ -3333,10 +3362,10 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D113" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3347,10 +3376,10 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D114" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3361,10 +3390,10 @@
         <v>31</v>
       </c>
       <c r="C115" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D115" t="s">
-        <v>210</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3375,10 +3404,10 @@
         <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>211</v>
+        <v>56</v>
       </c>
       <c r="D116" t="s">
-        <v>209</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3389,10 +3418,10 @@
         <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D117" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3403,10 +3432,10 @@
         <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D118" t="s">
-        <v>79</v>
+        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3417,10 +3446,10 @@
         <v>31</v>
       </c>
       <c r="C119" t="s">
-        <v>60</v>
+        <v>211</v>
       </c>
       <c r="D119" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3431,10 +3460,10 @@
         <v>31</v>
       </c>
       <c r="C120" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D120" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3445,10 +3474,10 @@
         <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D121" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3459,10 +3488,10 @@
         <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D122" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3473,10 +3502,10 @@
         <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D123" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3487,10 +3516,10 @@
         <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D124" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3501,10 +3530,10 @@
         <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="D125" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,13 +3541,13 @@
         <v>28</v>
       </c>
       <c r="B126" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="D126" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3526,13 +3555,13 @@
         <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C127" t="s">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="D127" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,13 +3569,13 @@
         <v>28</v>
       </c>
       <c r="B128" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C128" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="D128" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,10 +3583,10 @@
         <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C129" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="D129" t="s">
         <v>85</v>
@@ -3568,10 +3597,10 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C130" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="D130" t="s">
         <v>85</v>
@@ -3582,13 +3611,13 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C131" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="D131" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,10 +3625,10 @@
         <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>187</v>
+        <v>68</v>
       </c>
       <c r="D132" t="s">
         <v>85</v>
@@ -3610,13 +3639,13 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D133" t="s">
-        <v>208</v>
+        <v>85</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,10 +3656,10 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D134" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,13 +3667,13 @@
         <v>28</v>
       </c>
       <c r="B135" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C135" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="D135" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,13 +3681,13 @@
         <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C136" t="s">
-        <v>89</v>
+        <v>188</v>
       </c>
       <c r="D136" t="s">
-        <v>85</v>
+        <v>208</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3669,10 +3698,10 @@
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D137" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3683,10 +3712,10 @@
         <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D138" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3697,10 +3726,10 @@
         <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D139" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3708,13 +3737,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="D140" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,10 +3751,10 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C141" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="D141" t="s">
         <v>85</v>
@@ -3736,13 +3765,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C142" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="D142" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,10 +3779,10 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3764,10 +3793,10 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D144" t="s">
         <v>85</v>
@@ -3778,13 +3807,13 @@
         <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C145" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="D145" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3792,10 +3821,10 @@
         <v>28</v>
       </c>
       <c r="B146" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C146" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="D146" t="s">
         <v>85</v>
@@ -3806,13 +3835,13 @@
         <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C147" t="s">
-        <v>202</v>
+        <v>93</v>
       </c>
       <c r="D147" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,10 +3852,10 @@
         <v>31</v>
       </c>
       <c r="C148" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D148" t="s">
-        <v>37</v>
+        <v>203</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3834,13 +3863,13 @@
         <v>28</v>
       </c>
       <c r="B149" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C149" t="s">
-        <v>106</v>
+        <v>201</v>
       </c>
       <c r="D149" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3848,13 +3877,13 @@
         <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C150" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D150" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3865,10 +3894,10 @@
         <v>31</v>
       </c>
       <c r="C151" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D151" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3878,11 +3907,11 @@
       <c r="B152" t="s">
         <v>31</v>
       </c>
-      <c r="C152" s="5" t="s">
-        <v>110</v>
+      <c r="C152" t="s">
+        <v>106</v>
       </c>
       <c r="D152" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3893,10 +3922,10 @@
         <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D153" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3904,13 +3933,13 @@
         <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D154" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3918,13 +3947,13 @@
         <v>28</v>
       </c>
       <c r="B155" t="s">
-        <v>29</v>
-      </c>
-      <c r="C155" t="s">
-        <v>120</v>
+        <v>31</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D155" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3932,13 +3961,13 @@
         <v>28</v>
       </c>
       <c r="B156" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C156" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D156" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,10 +3978,10 @@
         <v>29</v>
       </c>
       <c r="C157" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D157" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,10 +3992,10 @@
         <v>29</v>
       </c>
       <c r="C158" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D158" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,10 +4006,10 @@
         <v>29</v>
       </c>
       <c r="C159" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D159" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3991,10 +4020,10 @@
         <v>29</v>
       </c>
       <c r="C160" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D160" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4005,10 +4034,10 @@
         <v>29</v>
       </c>
       <c r="C161" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="D161" t="s">
-        <v>224</v>
+        <v>79</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4016,13 +4045,13 @@
         <v>28</v>
       </c>
       <c r="B162" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C162" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D162" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4030,13 +4059,13 @@
         <v>28</v>
       </c>
       <c r="B163" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C163" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D163" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4044,13 +4073,13 @@
         <v>28</v>
       </c>
       <c r="B164" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C164" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="D164" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4061,10 +4090,10 @@
         <v>142</v>
       </c>
       <c r="C165" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="D165" t="s">
-        <v>219</v>
+        <v>79</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4075,10 +4104,10 @@
         <v>142</v>
       </c>
       <c r="C166" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="D166" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4089,10 +4118,10 @@
         <v>142</v>
       </c>
       <c r="C167" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4103,10 +4132,10 @@
         <v>142</v>
       </c>
       <c r="C168" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="D168" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4117,10 +4146,10 @@
         <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="D169" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4131,7 +4160,7 @@
         <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D170" t="s">
         <v>163</v>
@@ -4145,10 +4174,10 @@
         <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D171" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4159,10 +4188,10 @@
         <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D172" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,10 +4202,10 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="D173" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4187,10 +4216,10 @@
         <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="D174" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4201,10 +4230,10 @@
         <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D175" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4215,10 +4244,10 @@
         <v>142</v>
       </c>
       <c r="C176" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="D176" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4229,10 +4258,10 @@
         <v>142</v>
       </c>
       <c r="C177" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="D177" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4243,10 +4272,10 @@
         <v>142</v>
       </c>
       <c r="C178" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="D178" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4257,10 +4286,10 @@
         <v>142</v>
       </c>
       <c r="C179" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="D179" t="s">
-        <v>180</v>
+        <v>228</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,10 +4300,10 @@
         <v>142</v>
       </c>
       <c r="C180" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D180" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4285,10 +4314,10 @@
         <v>142</v>
       </c>
       <c r="C181" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D181" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4299,10 +4328,10 @@
         <v>142</v>
       </c>
       <c r="C182" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D182" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4313,14 +4342,98 @@
         <v>142</v>
       </c>
       <c r="C183" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D183" t="s">
         <v>180</v>
       </c>
     </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>28</v>
+      </c>
+      <c r="B184" t="s">
+        <v>142</v>
+      </c>
+      <c r="C184" t="s">
+        <v>226</v>
+      </c>
+      <c r="D184" t="s">
+        <v>228</v>
+      </c>
+    </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>28</v>
+      </c>
+      <c r="B185" t="s">
+        <v>142</v>
+      </c>
       <c r="C185" t="s">
+        <v>175</v>
+      </c>
+      <c r="D185" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>28</v>
+      </c>
+      <c r="B186" t="s">
+        <v>142</v>
+      </c>
+      <c r="C186" t="s">
+        <v>176</v>
+      </c>
+      <c r="D186" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>28</v>
+      </c>
+      <c r="B187" t="s">
+        <v>142</v>
+      </c>
+      <c r="C187" t="s">
+        <v>177</v>
+      </c>
+      <c r="D187" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>28</v>
+      </c>
+      <c r="B188" t="s">
+        <v>142</v>
+      </c>
+      <c r="C188" t="s">
+        <v>178</v>
+      </c>
+      <c r="D188" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>28</v>
+      </c>
+      <c r="B189" t="s">
+        <v>142</v>
+      </c>
+      <c r="C189" t="s">
+        <v>227</v>
+      </c>
+      <c r="D189" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wed 9 Nov 2016 14:33 commit by king
Code :
Update PacketFormat.xlsx
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -716,7 +711,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1113,7 +1108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1123,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,7 +3063,7 @@
         <v>170</v>
       </c>
       <c r="D96">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
@@ -3089,7 +3084,7 @@
         <v>171</v>
       </c>
       <c r="D97">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
@@ -3113,7 +3108,7 @@
         <v>172</v>
       </c>
       <c r="D98">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
@@ -3134,7 +3129,7 @@
         <v>173</v>
       </c>
       <c r="D99">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
@@ -3155,7 +3150,7 @@
         <v>226</v>
       </c>
       <c r="D100">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>33</v>
@@ -3173,7 +3168,7 @@
         <v>175</v>
       </c>
       <c r="D101">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>33</v>
@@ -3194,7 +3189,7 @@
         <v>176</v>
       </c>
       <c r="D102">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>33</v>
@@ -3218,7 +3213,7 @@
         <v>177</v>
       </c>
       <c r="D103">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Thu 10 Nov 2016 19:50 commit by king
Functionality :
- Adds event get between time with names in PacketFormat

Issue Fixes :
- Logger still shows INFO even with WARNING or ERROR set

Maintenance :
- Actuator, Controller & Sensor notifications
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="235">
   <si>
     <t>Meaning</t>
   </si>
@@ -705,7 +705,25 @@
     <t>UserGetSubscribedActuators</t>
   </si>
   <si>
-    <t>ArrayList&lt;String&gt;</t>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>ControllerNames (ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t>SensorNames (ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t>ActuatorNames (ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t>40c</t>
+  </si>
+  <si>
+    <t>39c</t>
+  </si>
+  <si>
+    <t>41c</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q191"/>
+  <dimension ref="A1:Q195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,7 +2578,7 @@
       </c>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -2568,17 +2586,23 @@
         <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="E73" t="s">
-        <v>105</v>
+        <v>229</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2586,16 +2610,13 @@
         <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>117</v>
+        <v>193</v>
+      </c>
+      <c r="E74" t="s">
+        <v>105</v>
       </c>
       <c r="P74" s="2"/>
     </row>
@@ -2604,18 +2625,20 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" t="s">
-        <v>61</v>
-      </c>
-      <c r="F75" s="10"/>
+        <v>194</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="P75" s="2"/>
     </row>
     <row r="76" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,59 +2646,66 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C76" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E76" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E76" t="s">
+        <v>230</v>
+      </c>
+      <c r="F76" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="G76" s="10" t="s">
         <v>117</v>
       </c>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
-      </c>
-      <c r="D77">
-        <v>43</v>
-      </c>
-      <c r="E77" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E77" t="s">
+        <v>61</v>
+      </c>
       <c r="F77" s="10"/>
       <c r="P77" s="2"/>
     </row>
-    <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>127</v>
-      </c>
-      <c r="D78">
-        <v>44</v>
+        <v>196</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>198</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F78" s="10"/>
+        <v>118</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="P78" s="2"/>
     </row>
-    <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -2683,20 +2713,23 @@
         <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>61</v>
+        <v>234</v>
+      </c>
+      <c r="E79" t="s">
+        <v>231</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>129</v>
+        <v>118</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -2704,31 +2737,27 @@
         <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>220</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>223</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="D80" s="12">
+        <v>42</v>
+      </c>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D81">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
@@ -2739,13 +2768,13 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D82">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>61</v>
@@ -2758,31 +2787,19 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>61</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="G83" t="s">
-        <v>159</v>
-      </c>
-      <c r="H83" t="s">
-        <v>160</v>
-      </c>
-      <c r="I83" t="s">
-        <v>86</v>
-      </c>
-      <c r="J83" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="P83" s="2"/>
     </row>
@@ -2794,31 +2811,16 @@
         <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>167</v>
+        <v>61</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="H84" t="s">
-        <v>159</v>
-      </c>
-      <c r="I84" t="s">
-        <v>160</v>
-      </c>
-      <c r="J84" t="s">
-        <v>86</v>
-      </c>
-      <c r="K84" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
       <c r="P84" s="2"/>
     </row>
@@ -2830,19 +2832,16 @@
         <v>142</v>
       </c>
       <c r="C85" t="s">
-        <v>217</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>167</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D85">
+        <v>46</v>
+      </c>
+      <c r="E85" s="10"/>
       <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
       <c r="P85" s="2"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -2850,41 +2849,51 @@
         <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D86">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F86" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F86" s="10"/>
+      <c r="P86" s="2"/>
+    </row>
+    <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F87" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="P86" s="2"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>28</v>
-      </c>
-      <c r="B87" t="s">
-        <v>142</v>
-      </c>
-      <c r="C87" t="s">
-        <v>154</v>
-      </c>
-      <c r="D87">
-        <v>50</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>159</v>
       </c>
+      <c r="H87" t="s">
+        <v>160</v>
+      </c>
+      <c r="I87" t="s">
+        <v>86</v>
+      </c>
+      <c r="J87" t="s">
+        <v>161</v>
+      </c>
       <c r="P87" s="2"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>28</v>
       </c>
@@ -2892,20 +2901,35 @@
         <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
-      </c>
-      <c r="D88">
-        <v>51</v>
+        <v>214</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H88" t="s">
+        <v>159</v>
+      </c>
+      <c r="I88" t="s">
         <v>160</v>
       </c>
+      <c r="J88" t="s">
+        <v>86</v>
+      </c>
+      <c r="K88" t="s">
+        <v>161</v>
+      </c>
       <c r="P88" s="2"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -2913,17 +2937,16 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
-      </c>
-      <c r="D89">
-        <v>52</v>
+        <v>217</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F89" t="s">
-        <v>165</v>
-      </c>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
       <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -2934,16 +2957,16 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D90">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F90" t="s">
-        <v>166</v>
+      <c r="F90" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="P90" s="2"/>
     </row>
@@ -2955,16 +2978,16 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="D91">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F91" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="P91" s="2"/>
     </row>
@@ -2976,19 +2999,16 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D92">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F92" t="s">
-        <v>44</v>
-      </c>
-      <c r="G92" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="P92" s="2"/>
     </row>
@@ -3000,16 +3020,16 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D93">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F93" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="P93" s="2"/>
     </row>
@@ -3021,16 +3041,16 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D94">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F94" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="P94" s="2"/>
     </row>
@@ -3042,14 +3062,17 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="D95">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F95" t="s">
+        <v>44</v>
+      </c>
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -3060,16 +3083,19 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="D96">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F96" t="s">
-        <v>105</v>
+        <v>44</v>
+      </c>
+      <c r="G96" t="s">
+        <v>174</v>
       </c>
       <c r="P96" s="2"/>
     </row>
@@ -3081,19 +3107,16 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="D97">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F97" t="s">
-        <v>105</v>
-      </c>
-      <c r="G97" t="s">
-        <v>174</v>
+        <v>44</v>
       </c>
       <c r="P97" s="2"/>
     </row>
@@ -3105,16 +3128,16 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="D98">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="P98" s="2"/>
     </row>
@@ -3126,17 +3149,14 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="D99">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F99" t="s">
-        <v>105</v>
-      </c>
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -3147,14 +3167,17 @@
         <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="D100">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F100" t="s">
+        <v>105</v>
+      </c>
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -3165,16 +3188,19 @@
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D101">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F101" t="s">
-        <v>61</v>
+        <v>105</v>
+      </c>
+      <c r="G101" t="s">
+        <v>174</v>
       </c>
       <c r="P101" s="2"/>
     </row>
@@ -3186,19 +3212,16 @@
         <v>142</v>
       </c>
       <c r="C102" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D102">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F102" t="s">
-        <v>61</v>
-      </c>
-      <c r="G102" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
       <c r="P102" s="2"/>
     </row>
@@ -3210,16 +3233,16 @@
         <v>142</v>
       </c>
       <c r="C103" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D103">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F103" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="P103" s="2"/>
     </row>
@@ -3231,17 +3254,14 @@
         <v>142</v>
       </c>
       <c r="C104" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="D104">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F104" t="s">
-        <v>61</v>
-      </c>
       <c r="P104" s="2"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -3252,43 +3272,83 @@
         <v>142</v>
       </c>
       <c r="C105" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="D105">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E105" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F105" t="s">
+        <v>61</v>
+      </c>
       <c r="P105" s="2"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>28</v>
+      </c>
+      <c r="B106" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106" t="s">
+        <v>176</v>
+      </c>
+      <c r="D106">
+        <v>65</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F106" t="s">
+        <v>61</v>
+      </c>
+      <c r="G106" t="s">
+        <v>174</v>
+      </c>
       <c r="P106" s="2"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C107" s="7" t="s">
-        <v>24</v>
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" t="s">
+        <v>177</v>
+      </c>
+      <c r="D107">
+        <v>66</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F107" t="s">
+        <v>61</v>
       </c>
       <c r="P107" s="2"/>
     </row>
-    <row r="108" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>28</v>
+      </c>
+      <c r="B108" t="s">
+        <v>142</v>
+      </c>
+      <c r="C108" t="s">
+        <v>178</v>
+      </c>
+      <c r="D108">
+        <v>67</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F108" t="s">
+        <v>61</v>
+      </c>
       <c r="P108" s="2"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -3296,281 +3356,272 @@
         <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C109" t="s">
+        <v>227</v>
+      </c>
+      <c r="D109">
+        <v>68</v>
+      </c>
+      <c r="E109" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P109" s="2"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P110" s="2"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C111" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P111" s="2"/>
+    </row>
+    <row r="112" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="P112" s="2"/>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>28</v>
+      </c>
+      <c r="B113" t="s">
+        <v>31</v>
+      </c>
+      <c r="C113" t="s">
         <v>34</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D113" t="s">
         <v>37</v>
       </c>
-      <c r="P109" s="2"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>28</v>
-      </c>
-      <c r="B110" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="P113" s="2"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" t="s">
         <v>36</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D114" t="s">
         <v>37</v>
       </c>
-      <c r="P110" s="2"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" t="s">
-        <v>31</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="P114" s="2"/>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" t="s">
+        <v>31</v>
+      </c>
+      <c r="C115" t="s">
         <v>35</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D115" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" t="s">
-        <v>31</v>
-      </c>
-      <c r="C112" t="s">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" t="s">
+        <v>31</v>
+      </c>
+      <c r="C116" t="s">
         <v>39</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D116" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>28</v>
-      </c>
-      <c r="B113" t="s">
-        <v>31</v>
-      </c>
-      <c r="C113" t="s">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" t="s">
+        <v>31</v>
+      </c>
+      <c r="C117" t="s">
         <v>40</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D117" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>28</v>
-      </c>
-      <c r="B114" t="s">
-        <v>31</v>
-      </c>
-      <c r="C114" t="s">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" t="s">
         <v>43</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D118" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>28</v>
-      </c>
-      <c r="B115" t="s">
-        <v>31</v>
-      </c>
-      <c r="C115" t="s">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119" t="s">
+        <v>31</v>
+      </c>
+      <c r="C119" t="s">
         <v>45</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D119" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>28</v>
-      </c>
-      <c r="B116" t="s">
-        <v>31</v>
-      </c>
-      <c r="C116" t="s">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>28</v>
+      </c>
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" t="s">
         <v>56</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D120" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>28</v>
-      </c>
-      <c r="B117" t="s">
-        <v>31</v>
-      </c>
-      <c r="C117" t="s">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>28</v>
+      </c>
+      <c r="B121" t="s">
+        <v>31</v>
+      </c>
+      <c r="C121" t="s">
         <v>57</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D121" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>28</v>
-      </c>
-      <c r="B118" t="s">
-        <v>31</v>
-      </c>
-      <c r="C118" t="s">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>28</v>
+      </c>
+      <c r="B122" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" t="s">
         <v>55</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D122" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" t="s">
-        <v>31</v>
-      </c>
-      <c r="C119" t="s">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" t="s">
         <v>211</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D123" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>28</v>
-      </c>
-      <c r="B120" t="s">
-        <v>31</v>
-      </c>
-      <c r="C120" t="s">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>28</v>
+      </c>
+      <c r="B124" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" t="s">
         <v>52</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D124" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" t="s">
-        <v>31</v>
-      </c>
-      <c r="C121" t="s">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B125" t="s">
+        <v>31</v>
+      </c>
+      <c r="C125" t="s">
         <v>59</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D125" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>28</v>
-      </c>
-      <c r="B122" t="s">
-        <v>31</v>
-      </c>
-      <c r="C122" t="s">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>28</v>
+      </c>
+      <c r="B126" t="s">
+        <v>31</v>
+      </c>
+      <c r="C126" t="s">
         <v>60</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D126" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>28</v>
-      </c>
-      <c r="B123" t="s">
-        <v>31</v>
-      </c>
-      <c r="C123" t="s">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>28</v>
+      </c>
+      <c r="B127" t="s">
+        <v>31</v>
+      </c>
+      <c r="C127" t="s">
         <v>62</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D127" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>28</v>
-      </c>
-      <c r="B124" t="s">
-        <v>31</v>
-      </c>
-      <c r="C124" t="s">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>28</v>
+      </c>
+      <c r="B128" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" t="s">
         <v>63</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D128" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>28</v>
-      </c>
-      <c r="B125" t="s">
-        <v>31</v>
-      </c>
-      <c r="C125" t="s">
-        <v>65</v>
-      </c>
-      <c r="D125" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>28</v>
-      </c>
-      <c r="B126" t="s">
-        <v>31</v>
-      </c>
-      <c r="C126" t="s">
-        <v>69</v>
-      </c>
-      <c r="D126" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>28</v>
-      </c>
-      <c r="B127" t="s">
-        <v>31</v>
-      </c>
-      <c r="C127" t="s">
-        <v>66</v>
-      </c>
-      <c r="D127" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>28</v>
-      </c>
-      <c r="B128" t="s">
-        <v>31</v>
-      </c>
-      <c r="C128" t="s">
-        <v>99</v>
-      </c>
-      <c r="D128" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3578,10 +3629,10 @@
         <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="D129" t="s">
         <v>85</v>
@@ -3592,13 +3643,13 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="D130" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3606,13 +3657,13 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
       <c r="D131" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,10 +3674,10 @@
         <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D132" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3634,10 +3685,10 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C133" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="D133" t="s">
         <v>85</v>
@@ -3648,13 +3699,13 @@
         <v>28</v>
       </c>
       <c r="B134" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C134" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="D134" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3716,7 @@
         <v>142</v>
       </c>
       <c r="C135" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="D135" t="s">
         <v>85</v>
@@ -3676,13 +3727,13 @@
         <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="D136" t="s">
-        <v>208</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3693,10 +3744,10 @@
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D137" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,10 +3758,10 @@
         <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D138" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3718,10 +3769,10 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C139" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="D139" t="s">
         <v>85</v>
@@ -3732,13 +3783,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="D140" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,10 +3800,10 @@
         <v>31</v>
       </c>
       <c r="C141" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D141" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3763,10 +3814,10 @@
         <v>31</v>
       </c>
       <c r="C142" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D142" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3774,10 +3825,10 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C143" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3788,13 +3839,13 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C144" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="D144" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3802,10 +3853,10 @@
         <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C145" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="D145" t="s">
         <v>85</v>
@@ -3819,10 +3870,10 @@
         <v>31</v>
       </c>
       <c r="C146" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D146" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3830,10 +3881,10 @@
         <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C147" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="D147" t="s">
         <v>85</v>
@@ -3844,13 +3895,13 @@
         <v>28</v>
       </c>
       <c r="B148" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C148" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D148" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3861,7 +3912,7 @@
         <v>142</v>
       </c>
       <c r="C149" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="D149" t="s">
         <v>85</v>
@@ -3872,13 +3923,13 @@
         <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="D150" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,10 +3940,10 @@
         <v>31</v>
       </c>
       <c r="C151" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D151" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,10 +3954,10 @@
         <v>31</v>
       </c>
       <c r="C152" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D152" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3914,13 +3965,13 @@
         <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C153" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D153" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3928,13 +3979,13 @@
         <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C154" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="D154" t="s">
-        <v>51</v>
+        <v>207</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3944,11 +3995,11 @@
       <c r="B155" t="s">
         <v>31</v>
       </c>
-      <c r="C155" s="5" t="s">
-        <v>110</v>
+      <c r="C155" t="s">
+        <v>108</v>
       </c>
       <c r="D155" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,10 +4010,10 @@
         <v>31</v>
       </c>
       <c r="C156" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D156" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3970,13 +4021,13 @@
         <v>28</v>
       </c>
       <c r="B157" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C157" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D157" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3984,13 +4035,13 @@
         <v>28</v>
       </c>
       <c r="B158" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C158" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D158" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3998,13 +4049,13 @@
         <v>28</v>
       </c>
       <c r="B159" t="s">
-        <v>29</v>
-      </c>
-      <c r="C159" t="s">
-        <v>121</v>
+        <v>31</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D159" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4012,13 +4063,13 @@
         <v>28</v>
       </c>
       <c r="B160" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C160" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D160" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,10 +4080,10 @@
         <v>29</v>
       </c>
       <c r="C161" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D161" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,10 +4094,10 @@
         <v>29</v>
       </c>
       <c r="C162" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D162" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4057,10 +4108,10 @@
         <v>29</v>
       </c>
       <c r="C163" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D163" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,10 +4122,10 @@
         <v>29</v>
       </c>
       <c r="C164" t="s">
-        <v>220</v>
+        <v>122</v>
       </c>
       <c r="D164" t="s">
-        <v>224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,10 +4133,10 @@
         <v>28</v>
       </c>
       <c r="B165" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C165" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D165" t="s">
         <v>79</v>
@@ -4096,10 +4147,10 @@
         <v>28</v>
       </c>
       <c r="B166" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C166" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D166" t="s">
         <v>51</v>
@@ -4110,13 +4161,13 @@
         <v>28</v>
       </c>
       <c r="B167" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C167" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D167" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4124,13 +4175,13 @@
         <v>28</v>
       </c>
       <c r="B168" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C168" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D168" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4141,10 +4192,10 @@
         <v>142</v>
       </c>
       <c r="C169" t="s">
-        <v>217</v>
+        <v>150</v>
       </c>
       <c r="D169" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4155,10 +4206,10 @@
         <v>142</v>
       </c>
       <c r="C170" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D170" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4169,10 +4220,10 @@
         <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D171" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4183,10 +4234,10 @@
         <v>142</v>
       </c>
       <c r="C172" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="D172" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4197,7 +4248,7 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="D173" t="s">
         <v>163</v>
@@ -4211,10 +4262,10 @@
         <v>142</v>
       </c>
       <c r="C174" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D174" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4225,10 +4276,10 @@
         <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="D175" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,10 +4290,10 @@
         <v>142</v>
       </c>
       <c r="C176" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D176" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4253,10 +4304,10 @@
         <v>142</v>
       </c>
       <c r="C177" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D177" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4267,10 +4318,10 @@
         <v>142</v>
       </c>
       <c r="C178" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D178" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,10 +4332,10 @@
         <v>142</v>
       </c>
       <c r="C179" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="D179" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,10 +4346,10 @@
         <v>142</v>
       </c>
       <c r="C180" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="D180" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,10 +4360,10 @@
         <v>142</v>
       </c>
       <c r="C181" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="D181" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,10 +4374,10 @@
         <v>142</v>
       </c>
       <c r="C182" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="D182" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4337,10 +4388,10 @@
         <v>142</v>
       </c>
       <c r="C183" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="D183" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4351,10 +4402,10 @@
         <v>142</v>
       </c>
       <c r="C184" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="D184" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4365,10 +4416,10 @@
         <v>142</v>
       </c>
       <c r="C185" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D185" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4379,10 +4430,10 @@
         <v>142</v>
       </c>
       <c r="C186" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D186" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4393,10 +4444,10 @@
         <v>142</v>
       </c>
       <c r="C187" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D187" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4407,10 +4458,10 @@
         <v>142</v>
       </c>
       <c r="C188" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="D188" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,14 +4472,70 @@
         <v>142</v>
       </c>
       <c r="C189" t="s">
+        <v>175</v>
+      </c>
+      <c r="D189" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>28</v>
+      </c>
+      <c r="B190" t="s">
+        <v>142</v>
+      </c>
+      <c r="C190" t="s">
+        <v>176</v>
+      </c>
+      <c r="D190" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>28</v>
+      </c>
+      <c r="B191" t="s">
+        <v>142</v>
+      </c>
+      <c r="C191" t="s">
+        <v>177</v>
+      </c>
+      <c r="D191" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>28</v>
+      </c>
+      <c r="B192" t="s">
+        <v>142</v>
+      </c>
+      <c r="C192" t="s">
+        <v>178</v>
+      </c>
+      <c r="D192" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>28</v>
+      </c>
+      <c r="B193" t="s">
+        <v>142</v>
+      </c>
+      <c r="C193" t="s">
         <v>227</v>
       </c>
-      <c r="D189" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C191" t="s">
+      <c r="D193" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C195" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tue 15 Nov 2016 commit by king
Code : 
- Further decomposes classes into packages (Reading, GWTServer)
- Relocated some classes into intended packages
- Removed start transaction on get event methods

Functionality :
- Actuator will log issue when fail to communicate with controller
- Added Sum/Avg/Culmulative value for reading, grouped by day, month or
year format.
- Renamed GWT Server into App Server
- Added Gantt Chart to view Ongoing Schedule

Issue Fixes :
- Controller Packet sends thrice
- Schedule is later by 1 day when cross day time rule is scheduled
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="257">
   <si>
     <t>Meaning</t>
   </si>
@@ -724,6 +724,72 @@
   </si>
   <si>
     <t>41c</t>
+  </si>
+  <si>
+    <t>GetTotalReadingGroupByDay</t>
+  </si>
+  <si>
+    <t>Sensorname</t>
+  </si>
+  <si>
+    <t>GetTotalReadingGroupByMonth</t>
+  </si>
+  <si>
+    <t>GetTotalReadingGroupByYear</t>
+  </si>
+  <si>
+    <t>69a</t>
+  </si>
+  <si>
+    <t>69b</t>
+  </si>
+  <si>
+    <t>69c</t>
+  </si>
+  <si>
+    <t>GetAverageReadingGroupByDay</t>
+  </si>
+  <si>
+    <t>GetAverageReadingGroupByMonth</t>
+  </si>
+  <si>
+    <t>GetAverageReadingGroupByYear</t>
+  </si>
+  <si>
+    <t>70a</t>
+  </si>
+  <si>
+    <t>71b</t>
+  </si>
+  <si>
+    <t>70b</t>
+  </si>
+  <si>
+    <t>70c</t>
+  </si>
+  <si>
+    <t>71a</t>
+  </si>
+  <si>
+    <t>71c</t>
+  </si>
+  <si>
+    <t>GetCulmulativeReadingGroupByDay</t>
+  </si>
+  <si>
+    <t>GetCulmulativeReadingGroupByMonth</t>
+  </si>
+  <si>
+    <t>GetCulmulativeReadingGroupByYear</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; | Year, Month, Day, Reading</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; | Year, Month, Reading</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Object []&gt; | Year, Reading</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1192,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1134,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q195"/>
+  <dimension ref="A1:Q213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3370,32 +3436,57 @@
       <c r="P109" s="2"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>28</v>
+      </c>
+      <c r="B110" t="s">
+        <v>142</v>
+      </c>
+      <c r="C110" t="s">
+        <v>235</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>236</v>
+      </c>
       <c r="P110" s="2"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C111" s="7" t="s">
-        <v>24</v>
+      <c r="A111" t="s">
+        <v>28</v>
+      </c>
+      <c r="B111" t="s">
+        <v>142</v>
+      </c>
+      <c r="C111" t="s">
+        <v>237</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="P111" s="2"/>
     </row>
-    <row r="112" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
-      <c r="K112" s="2"/>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>28</v>
+      </c>
+      <c r="B112" t="s">
+        <v>142</v>
+      </c>
+      <c r="C112" t="s">
+        <v>238</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>236</v>
+      </c>
       <c r="P112" s="2"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
@@ -3403,13 +3494,16 @@
         <v>28</v>
       </c>
       <c r="B113" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C113" t="s">
-        <v>34</v>
-      </c>
-      <c r="D113" t="s">
-        <v>37</v>
+        <v>242</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="P113" s="2"/>
     </row>
@@ -3418,13 +3512,16 @@
         <v>28</v>
       </c>
       <c r="B114" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C114" t="s">
-        <v>36</v>
-      </c>
-      <c r="D114" t="s">
-        <v>37</v>
+        <v>243</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="P114" s="2"/>
     </row>
@@ -3433,98 +3530,95 @@
         <v>28</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C115" t="s">
-        <v>35</v>
-      </c>
-      <c r="D115" t="s">
-        <v>125</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="E115" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="P115" s="2"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>28</v>
       </c>
       <c r="B116" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C116" t="s">
-        <v>39</v>
-      </c>
-      <c r="D116" t="s">
-        <v>42</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="E116" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="P116" s="2"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C117" t="s">
-        <v>40</v>
-      </c>
-      <c r="D117" t="s">
-        <v>42</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E117" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="P117" s="2"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C118" t="s">
-        <v>43</v>
-      </c>
-      <c r="D118" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" t="s">
-        <v>31</v>
-      </c>
-      <c r="C119" t="s">
-        <v>45</v>
-      </c>
-      <c r="D119" t="s">
-        <v>42</v>
+        <v>253</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>28</v>
-      </c>
-      <c r="B120" t="s">
-        <v>31</v>
-      </c>
-      <c r="C120" t="s">
-        <v>56</v>
-      </c>
-      <c r="D120" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" t="s">
-        <v>31</v>
-      </c>
-      <c r="C121" t="s">
-        <v>57</v>
-      </c>
-      <c r="D121" t="s">
-        <v>51</v>
-      </c>
+      <c r="C120" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -3534,10 +3628,10 @@
         <v>31</v>
       </c>
       <c r="C122" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>210</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
@@ -3548,10 +3642,10 @@
         <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>211</v>
+        <v>36</v>
       </c>
       <c r="D123" t="s">
-        <v>209</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -3562,10 +3656,10 @@
         <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D124" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -3576,10 +3670,10 @@
         <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D125" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -3590,10 +3684,10 @@
         <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D126" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -3604,10 +3698,10 @@
         <v>31</v>
       </c>
       <c r="C127" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D127" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -3618,10 +3712,10 @@
         <v>31</v>
       </c>
       <c r="C128" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D128" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,10 +3726,10 @@
         <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D129" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3646,10 +3740,10 @@
         <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D130" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,10 +3754,10 @@
         <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D131" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3674,10 +3768,10 @@
         <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>99</v>
+        <v>211</v>
       </c>
       <c r="D132" t="s">
-        <v>100</v>
+        <v>209</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3685,13 +3779,13 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="D133" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3699,13 +3793,13 @@
         <v>28</v>
       </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>141</v>
+        <v>59</v>
       </c>
       <c r="D134" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3713,13 +3807,13 @@
         <v>28</v>
       </c>
       <c r="B135" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="D135" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,10 +3824,10 @@
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D136" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,10 +3838,10 @@
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D137" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3758,10 +3852,10 @@
         <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D138" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3769,13 +3863,13 @@
         <v>28</v>
       </c>
       <c r="B139" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>187</v>
+        <v>69</v>
       </c>
       <c r="D139" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,13 +3877,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
       <c r="D140" t="s">
-        <v>208</v>
+        <v>98</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3800,10 +3894,10 @@
         <v>31</v>
       </c>
       <c r="C141" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D141" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,13 +3905,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C142" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="D142" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3825,10 +3919,10 @@
         <v>28</v>
       </c>
       <c r="B143" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3839,13 +3933,13 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="D144" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,7 +3950,7 @@
         <v>31</v>
       </c>
       <c r="C145" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D145" t="s">
         <v>85</v>
@@ -3870,10 +3964,10 @@
         <v>31</v>
       </c>
       <c r="C146" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D146" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3881,13 +3975,13 @@
         <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C147" t="s">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="D147" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3898,7 +3992,7 @@
         <v>142</v>
       </c>
       <c r="C148" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="D148" t="s">
         <v>85</v>
@@ -3912,10 +4006,10 @@
         <v>142</v>
       </c>
       <c r="C149" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="D149" t="s">
-        <v>85</v>
+        <v>208</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,10 +4020,10 @@
         <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D150" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3940,10 +4034,10 @@
         <v>31</v>
       </c>
       <c r="C151" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D151" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3954,10 +4048,10 @@
         <v>31</v>
       </c>
       <c r="C152" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D152" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3965,13 +4059,13 @@
         <v>28</v>
       </c>
       <c r="B153" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="D153" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3979,13 +4073,13 @@
         <v>28</v>
       </c>
       <c r="B154" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>202</v>
+        <v>91</v>
       </c>
       <c r="D154" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3996,10 +4090,10 @@
         <v>31</v>
       </c>
       <c r="C155" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D155" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,13 +4101,13 @@
         <v>28</v>
       </c>
       <c r="B156" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C156" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="D156" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,13 +4115,13 @@
         <v>28</v>
       </c>
       <c r="B157" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C157" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="D157" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,13 +4129,13 @@
         <v>28</v>
       </c>
       <c r="B158" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C158" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="D158" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4051,11 +4145,11 @@
       <c r="B159" t="s">
         <v>31</v>
       </c>
-      <c r="C159" s="5" t="s">
-        <v>110</v>
+      <c r="C159" t="s">
+        <v>92</v>
       </c>
       <c r="D159" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,10 +4160,10 @@
         <v>31</v>
       </c>
       <c r="C160" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D160" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,13 +4171,13 @@
         <v>28</v>
       </c>
       <c r="B161" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C161" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D161" t="s">
-        <v>123</v>
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,13 +4185,13 @@
         <v>28</v>
       </c>
       <c r="B162" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C162" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="D162" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4105,13 +4199,13 @@
         <v>28</v>
       </c>
       <c r="B163" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C163" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
       <c r="D163" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4119,13 +4213,13 @@
         <v>28</v>
       </c>
       <c r="B164" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C164" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D164" t="s">
-        <v>124</v>
+        <v>37</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,13 +4227,13 @@
         <v>28</v>
       </c>
       <c r="B165" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C165" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="D165" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,13 +4241,13 @@
         <v>28</v>
       </c>
       <c r="B166" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C166" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="D166" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4161,13 +4255,13 @@
         <v>28</v>
       </c>
       <c r="B167" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C167" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D167" t="s">
-        <v>169</v>
+        <v>51</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4175,13 +4269,13 @@
         <v>28</v>
       </c>
       <c r="B168" t="s">
-        <v>29</v>
-      </c>
-      <c r="C168" t="s">
-        <v>220</v>
+        <v>31</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D168" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4189,13 +4283,13 @@
         <v>28</v>
       </c>
       <c r="B169" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C169" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="D169" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4203,13 +4297,13 @@
         <v>28</v>
       </c>
       <c r="B170" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C170" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="D170" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,13 +4311,13 @@
         <v>28</v>
       </c>
       <c r="B171" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C171" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="D171" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,13 +4325,13 @@
         <v>28</v>
       </c>
       <c r="B172" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C172" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="D172" t="s">
-        <v>219</v>
+        <v>124</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4245,13 +4339,13 @@
         <v>28</v>
       </c>
       <c r="B173" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C173" t="s">
-        <v>217</v>
+        <v>122</v>
       </c>
       <c r="D173" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4259,13 +4353,13 @@
         <v>28</v>
       </c>
       <c r="B174" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C174" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="D174" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,13 +4367,13 @@
         <v>28</v>
       </c>
       <c r="B175" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C175" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="D175" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,13 +4381,13 @@
         <v>28</v>
       </c>
       <c r="B176" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C176" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="D176" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4301,13 +4395,13 @@
         <v>28</v>
       </c>
       <c r="B177" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C177" t="s">
-        <v>156</v>
+        <v>220</v>
       </c>
       <c r="D177" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4318,10 +4412,10 @@
         <v>142</v>
       </c>
       <c r="C178" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D178" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4332,10 +4426,10 @@
         <v>142</v>
       </c>
       <c r="C179" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="D179" t="s">
-        <v>185</v>
+        <v>51</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4346,10 +4440,10 @@
         <v>142</v>
       </c>
       <c r="C180" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D180" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4360,10 +4454,10 @@
         <v>142</v>
       </c>
       <c r="C181" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="D181" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4374,10 +4468,10 @@
         <v>142</v>
       </c>
       <c r="C182" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="D182" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4388,10 +4482,10 @@
         <v>142</v>
       </c>
       <c r="C183" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="D183" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4402,10 +4496,10 @@
         <v>142</v>
       </c>
       <c r="C184" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D184" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,10 +4510,10 @@
         <v>142</v>
       </c>
       <c r="C185" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D185" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,10 +4524,10 @@
         <v>142</v>
       </c>
       <c r="C186" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="D186" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4444,10 +4538,10 @@
         <v>142</v>
       </c>
       <c r="C187" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="D187" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4458,10 +4552,10 @@
         <v>142</v>
       </c>
       <c r="C188" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="D188" t="s">
-        <v>79</v>
+        <v>185</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4472,10 +4566,10 @@
         <v>142</v>
       </c>
       <c r="C189" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D189" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4486,10 +4580,10 @@
         <v>142</v>
       </c>
       <c r="C190" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D190" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,10 +4594,10 @@
         <v>142</v>
       </c>
       <c r="C191" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D191" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4514,28 +4608,289 @@
         <v>142</v>
       </c>
       <c r="C192" t="s">
+        <v>225</v>
+      </c>
+      <c r="D192" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>28</v>
+      </c>
+      <c r="B193" t="s">
+        <v>142</v>
+      </c>
+      <c r="C193" t="s">
+        <v>170</v>
+      </c>
+      <c r="D193" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>28</v>
+      </c>
+      <c r="B194" t="s">
+        <v>142</v>
+      </c>
+      <c r="C194" t="s">
+        <v>171</v>
+      </c>
+      <c r="D194" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>28</v>
+      </c>
+      <c r="B195" t="s">
+        <v>142</v>
+      </c>
+      <c r="C195" t="s">
+        <v>172</v>
+      </c>
+      <c r="D195" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>28</v>
+      </c>
+      <c r="B196" t="s">
+        <v>142</v>
+      </c>
+      <c r="C196" t="s">
+        <v>173</v>
+      </c>
+      <c r="D196" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>28</v>
+      </c>
+      <c r="B197" t="s">
+        <v>142</v>
+      </c>
+      <c r="C197" t="s">
+        <v>226</v>
+      </c>
+      <c r="D197" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>28</v>
+      </c>
+      <c r="B198" t="s">
+        <v>142</v>
+      </c>
+      <c r="C198" t="s">
+        <v>175</v>
+      </c>
+      <c r="D198" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>28</v>
+      </c>
+      <c r="B199" t="s">
+        <v>142</v>
+      </c>
+      <c r="C199" t="s">
+        <v>176</v>
+      </c>
+      <c r="D199" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>28</v>
+      </c>
+      <c r="B200" t="s">
+        <v>142</v>
+      </c>
+      <c r="C200" t="s">
+        <v>177</v>
+      </c>
+      <c r="D200" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>28</v>
+      </c>
+      <c r="B201" t="s">
+        <v>142</v>
+      </c>
+      <c r="C201" t="s">
         <v>178</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D201" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>28</v>
-      </c>
-      <c r="B193" t="s">
-        <v>142</v>
-      </c>
-      <c r="C193" t="s">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>28</v>
+      </c>
+      <c r="B202" t="s">
+        <v>142</v>
+      </c>
+      <c r="C202" t="s">
         <v>227</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D202" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C195" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>28</v>
+      </c>
+      <c r="B203" t="s">
+        <v>142</v>
+      </c>
+      <c r="C203" t="s">
+        <v>235</v>
+      </c>
+      <c r="D203" t="s">
+        <v>254</v>
+      </c>
+      <c r="E203" s="10"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>28</v>
+      </c>
+      <c r="B204" t="s">
+        <v>142</v>
+      </c>
+      <c r="C204" t="s">
+        <v>237</v>
+      </c>
+      <c r="D204" t="s">
+        <v>255</v>
+      </c>
+      <c r="E204" s="10"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>28</v>
+      </c>
+      <c r="B205" t="s">
+        <v>142</v>
+      </c>
+      <c r="C205" t="s">
+        <v>238</v>
+      </c>
+      <c r="D205" t="s">
+        <v>256</v>
+      </c>
+      <c r="E205" s="10"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>28</v>
+      </c>
+      <c r="B206" t="s">
+        <v>142</v>
+      </c>
+      <c r="C206" t="s">
+        <v>242</v>
+      </c>
+      <c r="D206" t="s">
+        <v>254</v>
+      </c>
+      <c r="E206" s="10"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>28</v>
+      </c>
+      <c r="B207" t="s">
+        <v>142</v>
+      </c>
+      <c r="C207" t="s">
+        <v>243</v>
+      </c>
+      <c r="D207" t="s">
+        <v>255</v>
+      </c>
+      <c r="E207" s="10"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>28</v>
+      </c>
+      <c r="B208" t="s">
+        <v>142</v>
+      </c>
+      <c r="C208" t="s">
+        <v>244</v>
+      </c>
+      <c r="D208" t="s">
+        <v>256</v>
+      </c>
+      <c r="E208" s="10"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>28</v>
+      </c>
+      <c r="B209" t="s">
+        <v>142</v>
+      </c>
+      <c r="C209" t="s">
+        <v>251</v>
+      </c>
+      <c r="D209" t="s">
+        <v>254</v>
+      </c>
+      <c r="E209" s="10"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>28</v>
+      </c>
+      <c r="B210" t="s">
+        <v>142</v>
+      </c>
+      <c r="C210" t="s">
+        <v>252</v>
+      </c>
+      <c r="D210" t="s">
+        <v>255</v>
+      </c>
+      <c r="E210" s="10"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>28</v>
+      </c>
+      <c r="B211" t="s">
+        <v>142</v>
+      </c>
+      <c r="C211" t="s">
+        <v>253</v>
+      </c>
+      <c r="D211" t="s">
+        <v>256</v>
+      </c>
+      <c r="E211" s="10"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C213" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sat 19 Nov 2016 14:26 commit by king
Functionality :
- Improves microcontroller connection performance
- Added length limit on fields
- Live reading now shows timestamp on title
- Improves DataServer performance

Code
- Changed map loading fail to warning level instead

Issue Fixes :
- Logging
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -795,7 +800,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1192,7 +1197,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1202,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D204" sqref="D204"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1413,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1417,7 +1422,10 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1428,7 +1436,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1437,10 +1445,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mon 28 Nov 2016 13:48 commit by king
Functionality :
Added GetSensorLatestReading to App Server
</commit_message>
<xml_diff>
--- a/PacketFormats.xlsx
+++ b/PacketFormats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\EclipseProjects\Chi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12915"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="260">
   <si>
     <t>Meaning</t>
   </si>
@@ -795,12 +790,21 @@
   </si>
   <si>
     <t>ArrayList&lt;Object []&gt; | Year, Reading</t>
+  </si>
+  <si>
+    <t>SensorGetLatestReading</t>
+  </si>
+  <si>
+    <t>38b</t>
+  </si>
+  <si>
+    <t>double</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1197,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1205,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q213"/>
+  <dimension ref="A1:Q215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2615,20 +2619,20 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>191</v>
+        <v>258</v>
       </c>
       <c r="E71" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -2636,16 +2640,13 @@
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>117</v>
+        <v>191</v>
+      </c>
+      <c r="E72" t="s">
+        <v>44</v>
       </c>
       <c r="P72" s="2"/>
     </row>
@@ -2660,20 +2661,17 @@
         <v>122</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="E73" t="s">
-        <v>229</v>
+        <v>192</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G73" s="10" t="s">
         <v>117</v>
       </c>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2681,17 +2679,23 @@
         <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="E74" t="s">
-        <v>105</v>
+        <v>229</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -2699,16 +2703,13 @@
         <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F75" s="10" t="s">
-        <v>117</v>
+        <v>193</v>
+      </c>
+      <c r="E75" t="s">
+        <v>105</v>
       </c>
       <c r="P75" s="2"/>
     </row>
@@ -2723,15 +2724,12 @@
         <v>120</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="E76" t="s">
-        <v>230</v>
+        <v>194</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G76" s="10" t="s">
         <v>117</v>
       </c>
       <c r="P76" s="2"/>
@@ -2741,18 +2739,23 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="E77" t="s">
-        <v>61</v>
-      </c>
-      <c r="F77" s="10"/>
+        <v>230</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="P77" s="2"/>
     </row>
     <row r="78" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2763,17 +2766,15 @@
         <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F78" s="10" t="s">
-        <v>117</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="E78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" s="10"/>
       <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,21 +2782,18 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
         <v>196</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="E79" t="s">
-        <v>231</v>
+        <v>198</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G79" s="10" t="s">
         <v>117</v>
       </c>
       <c r="P79" s="2"/>
@@ -2805,36 +2803,43 @@
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" t="s">
+        <v>231</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="P80" s="2"/>
+    </row>
+    <row r="81" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" t="s">
         <v>228</v>
       </c>
-      <c r="D80" s="12">
+      <c r="D81" s="12">
         <v>42</v>
-      </c>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="P80" s="2"/>
-    </row>
-    <row r="81" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>28</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" t="s">
-        <v>130</v>
-      </c>
-      <c r="D81">
-        <v>43</v>
       </c>
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -2842,14 +2847,12 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D82">
-        <v>44</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>61</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E82" s="10"/>
       <c r="F82" s="10"/>
       <c r="P82" s="2"/>
     </row>
@@ -2861,17 +2864,15 @@
         <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>128</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>222</v>
+        <v>127</v>
+      </c>
+      <c r="D83">
+        <v>44</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F83" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="F83" s="10"/>
       <c r="P83" s="2"/>
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2879,19 +2880,19 @@
         <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C84" t="s">
-        <v>220</v>
+        <v>128</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>61</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>223</v>
+        <v>129</v>
       </c>
       <c r="P84" s="2"/>
     </row>
@@ -2903,13 +2904,17 @@
         <v>142</v>
       </c>
       <c r="C85" t="s">
-        <v>150</v>
-      </c>
-      <c r="D85">
-        <v>46</v>
-      </c>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
+        <v>220</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2920,14 +2925,12 @@
         <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D86">
-        <v>47</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>61</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E86" s="10"/>
       <c r="F86" s="10"/>
       <c r="P86" s="2"/>
     </row>
@@ -2939,29 +2942,15 @@
         <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>152</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>218</v>
+        <v>151</v>
+      </c>
+      <c r="D87">
+        <v>47</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F87" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="G87" t="s">
-        <v>159</v>
-      </c>
-      <c r="H87" t="s">
-        <v>160</v>
-      </c>
-      <c r="I87" t="s">
-        <v>86</v>
-      </c>
-      <c r="J87" t="s">
-        <v>161</v>
-      </c>
+      <c r="F87" s="10"/>
       <c r="P87" s="2"/>
     </row>
     <row r="88" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2972,30 +2961,27 @@
         <v>142</v>
       </c>
       <c r="C88" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>167</v>
+        <v>61</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G88" s="10" t="s">
         <v>158</v>
       </c>
+      <c r="G88" t="s">
+        <v>159</v>
+      </c>
       <c r="H88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I88" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="J88" t="s">
-        <v>86</v>
-      </c>
-      <c r="K88" t="s">
         <v>161</v>
       </c>
       <c r="P88" s="2"/>
@@ -3008,19 +2994,35 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
+      <c r="F89" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H89" t="s">
+        <v>159</v>
+      </c>
+      <c r="I89" t="s">
+        <v>160</v>
+      </c>
+      <c r="J89" t="s">
+        <v>86</v>
+      </c>
+      <c r="K89" t="s">
+        <v>161</v>
+      </c>
       <c r="P89" s="2"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -3028,17 +3030,16 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D90">
-        <v>49</v>
+        <v>217</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F90" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
       <c r="P90" s="2"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -3049,16 +3050,16 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D91">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="F91" t="s">
-        <v>159</v>
+      <c r="F91" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="P91" s="2"/>
     </row>
@@ -3070,16 +3071,16 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D92">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P92" s="2"/>
     </row>
@@ -3091,16 +3092,16 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D93">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F93" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="P93" s="2"/>
     </row>
@@ -3112,16 +3113,16 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D94">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>167</v>
       </c>
       <c r="F94" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P94" s="2"/>
     </row>
@@ -3133,16 +3134,16 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D95">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="F95" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="P95" s="2"/>
     </row>
@@ -3154,10 +3155,10 @@
         <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D96">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>33</v>
@@ -3165,9 +3166,6 @@
       <c r="F96" t="s">
         <v>44</v>
       </c>
-      <c r="G96" t="s">
-        <v>174</v>
-      </c>
       <c r="P96" s="2"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -3178,10 +3176,10 @@
         <v>142</v>
       </c>
       <c r="C97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D97">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>33</v>
@@ -3189,6 +3187,9 @@
       <c r="F97" t="s">
         <v>44</v>
       </c>
+      <c r="G97" t="s">
+        <v>174</v>
+      </c>
       <c r="P97" s="2"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -3199,10 +3200,10 @@
         <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D98">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>33</v>
@@ -3220,14 +3221,17 @@
         <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
       <c r="D99">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F99" t="s">
+        <v>44</v>
+      </c>
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -3238,17 +3242,14 @@
         <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>170</v>
+        <v>225</v>
       </c>
       <c r="D100">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F100" t="s">
-        <v>105</v>
-      </c>
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -3259,10 +3260,10 @@
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D101">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>33</v>
@@ -3270,9 +3271,6 @@
       <c r="F101" t="s">
         <v>105</v>
       </c>
-      <c r="G101" t="s">
-        <v>174</v>
-      </c>
       <c r="P101" s="2"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
@@ -3283,10 +3281,10 @@
         <v>142</v>
       </c>
       <c r="C102" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D102">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E102" s="10" t="s">
         <v>33</v>
@@ -3294,6 +3292,9 @@
       <c r="F102" t="s">
         <v>105</v>
       </c>
+      <c r="G102" t="s">
+        <v>174</v>
+      </c>
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -3304,10 +3305,10 @@
         <v>142</v>
       </c>
       <c r="C103" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D103">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>33</v>
@@ -3325,14 +3326,17 @@
         <v>142</v>
       </c>
       <c r="C104" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
       <c r="D104">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F104" t="s">
+        <v>105</v>
+      </c>
       <c r="P104" s="2"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -3343,17 +3347,14 @@
         <v>142</v>
       </c>
       <c r="C105" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="D105">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E105" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F105" t="s">
-        <v>61</v>
-      </c>
       <c r="P105" s="2"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -3364,10 +3365,10 @@
         <v>142</v>
       </c>
       <c r="C106" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D106">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E106" s="10" t="s">
         <v>33</v>
@@ -3375,9 +3376,6 @@
       <c r="F106" t="s">
         <v>61</v>
       </c>
-      <c r="G106" t="s">
-        <v>174</v>
-      </c>
       <c r="P106" s="2"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
@@ -3388,10 +3386,10 @@
         <v>142</v>
       </c>
       <c r="C107" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D107">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>33</v>
@@ -3399,6 +3397,9 @@
       <c r="F107" t="s">
         <v>61</v>
       </c>
+      <c r="G107" t="s">
+        <v>174</v>
+      </c>
       <c r="P107" s="2"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -3409,10 +3410,10 @@
         <v>142</v>
       </c>
       <c r="C108" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D108">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E108" s="10" t="s">
         <v>33</v>
@@ -3430,14 +3431,17 @@
         <v>142</v>
       </c>
       <c r="C109" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="D109">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E109" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="F109" t="s">
+        <v>61</v>
+      </c>
       <c r="P109" s="2"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -3448,13 +3452,13 @@
         <v>142</v>
       </c>
       <c r="C110" t="s">
-        <v>235</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>239</v>
+        <v>227</v>
+      </c>
+      <c r="D110">
+        <v>68</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>236</v>
+        <v>33</v>
       </c>
       <c r="P110" s="2"/>
     </row>
@@ -3466,10 +3470,10 @@
         <v>142</v>
       </c>
       <c r="C111" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E111" s="10" t="s">
         <v>236</v>
@@ -3484,10 +3488,10 @@
         <v>142</v>
       </c>
       <c r="C112" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E112" s="10" t="s">
         <v>236</v>
@@ -3502,10 +3506,10 @@
         <v>142</v>
       </c>
       <c r="C113" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E113" s="10" t="s">
         <v>236</v>
@@ -3520,10 +3524,10 @@
         <v>142</v>
       </c>
       <c r="C114" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E114" s="10" t="s">
         <v>236</v>
@@ -3538,18 +3542,14 @@
         <v>142</v>
       </c>
       <c r="C115" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
       <c r="P115" s="2"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -3560,14 +3560,18 @@
         <v>142</v>
       </c>
       <c r="C116" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E116" s="10" t="s">
         <v>236</v>
       </c>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
       <c r="P116" s="2"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -3578,10 +3582,10 @@
         <v>142</v>
       </c>
       <c r="C117" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E117" s="10" t="s">
         <v>236</v>
@@ -3596,48 +3600,52 @@
         <v>142</v>
       </c>
       <c r="C118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E118" s="10" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C120" s="7" t="s">
+      <c r="P118" s="2"/>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119" t="s">
+        <v>142</v>
+      </c>
+      <c r="C119" t="s">
+        <v>253</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C121" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+    <row r="122" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="B122" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C122" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D121" s="9" t="s">
+      <c r="D122" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E121" s="2"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>28</v>
-      </c>
-      <c r="B122" t="s">
-        <v>31</v>
-      </c>
-      <c r="C122" t="s">
-        <v>34</v>
-      </c>
-      <c r="D122" t="s">
-        <v>37</v>
-      </c>
+      <c r="E122" s="2"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3647,7 +3655,7 @@
         <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D123" t="s">
         <v>37</v>
@@ -3661,10 +3669,10 @@
         <v>31</v>
       </c>
       <c r="C124" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D124" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -3675,10 +3683,10 @@
         <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D125" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -3689,7 +3697,7 @@
         <v>31</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D126" t="s">
         <v>42</v>
@@ -3703,7 +3711,7 @@
         <v>31</v>
       </c>
       <c r="C127" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D127" t="s">
         <v>42</v>
@@ -3717,7 +3725,7 @@
         <v>31</v>
       </c>
       <c r="C128" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D128" t="s">
         <v>42</v>
@@ -3731,10 +3739,10 @@
         <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D129" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,10 +3753,10 @@
         <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D130" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3759,10 +3767,10 @@
         <v>31</v>
       </c>
       <c r="C131" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D131" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3773,10 +3781,10 @@
         <v>31</v>
       </c>
       <c r="C132" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="D132" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3787,10 +3795,10 @@
         <v>31</v>
       </c>
       <c r="C133" t="s">
-        <v>52</v>
+        <v>211</v>
       </c>
       <c r="D133" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3801,10 +3809,10 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D134" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3815,7 +3823,7 @@
         <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D135" t="s">
         <v>79</v>
@@ -3829,7 +3837,7 @@
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D136" t="s">
         <v>79</v>
@@ -3843,10 +3851,10 @@
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D137" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,10 +3865,10 @@
         <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D138" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3871,10 +3879,10 @@
         <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D139" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3885,10 +3893,10 @@
         <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D140" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3899,10 +3907,10 @@
         <v>31</v>
       </c>
       <c r="C141" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="D141" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3910,13 +3918,13 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C142" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="D142" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,7 +3935,7 @@
         <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" t="s">
         <v>85</v>
@@ -3941,7 +3949,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D144" t="s">
         <v>85</v>
@@ -3952,10 +3960,10 @@
         <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C145" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="D145" t="s">
         <v>85</v>
@@ -3969,7 +3977,7 @@
         <v>31</v>
       </c>
       <c r="C146" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D146" t="s">
         <v>85</v>
@@ -3983,10 +3991,10 @@
         <v>31</v>
       </c>
       <c r="C147" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D147" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3994,13 +4002,13 @@
         <v>28</v>
       </c>
       <c r="B148" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C148" t="s">
-        <v>187</v>
+        <v>64</v>
       </c>
       <c r="D148" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4011,10 +4019,10 @@
         <v>142</v>
       </c>
       <c r="C149" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D149" t="s">
-        <v>208</v>
+        <v>85</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,13 +4030,13 @@
         <v>28</v>
       </c>
       <c r="B150" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C150" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
       <c r="D150" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4039,10 +4047,10 @@
         <v>31</v>
       </c>
       <c r="C151" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D151" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4053,10 +4061,10 @@
         <v>31</v>
       </c>
       <c r="C152" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D152" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4067,10 +4075,10 @@
         <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D153" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4081,10 +4089,10 @@
         <v>31</v>
       </c>
       <c r="C154" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D154" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4095,10 +4103,10 @@
         <v>31</v>
       </c>
       <c r="C155" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D155" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4106,13 +4114,13 @@
         <v>28</v>
       </c>
       <c r="B156" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C156" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="D156" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4123,7 +4131,7 @@
         <v>142</v>
       </c>
       <c r="C157" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D157" t="s">
         <v>85</v>
@@ -4137,7 +4145,7 @@
         <v>142</v>
       </c>
       <c r="C158" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D158" t="s">
         <v>85</v>
@@ -4148,10 +4156,10 @@
         <v>28</v>
       </c>
       <c r="B159" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C159" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="D159" t="s">
         <v>85</v>
@@ -4165,7 +4173,7 @@
         <v>31</v>
       </c>
       <c r="C160" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D160" t="s">
         <v>85</v>
@@ -4179,10 +4187,10 @@
         <v>31</v>
       </c>
       <c r="C161" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D161" t="s">
-        <v>203</v>
+        <v>85</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4190,13 +4198,13 @@
         <v>28</v>
       </c>
       <c r="B162" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C162" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="D162" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4207,10 +4215,10 @@
         <v>142</v>
       </c>
       <c r="C163" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D163" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,13 +4226,13 @@
         <v>28</v>
       </c>
       <c r="B164" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C164" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="D164" t="s">
-        <v>37</v>
+        <v>207</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4235,10 +4243,10 @@
         <v>31</v>
       </c>
       <c r="C165" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D165" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,7 +4257,7 @@
         <v>31</v>
       </c>
       <c r="C166" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D166" t="s">
         <v>149</v>
@@ -4263,10 +4271,10 @@
         <v>31</v>
       </c>
       <c r="C167" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D167" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4276,11 +4284,11 @@
       <c r="B168" t="s">
         <v>31</v>
       </c>
-      <c r="C168" s="5" t="s">
-        <v>110</v>
+      <c r="C168" t="s">
+        <v>104</v>
       </c>
       <c r="D168" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4290,8 +4298,8 @@
       <c r="B169" t="s">
         <v>31</v>
       </c>
-      <c r="C169" t="s">
-        <v>103</v>
+      <c r="C169" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D169" t="s">
         <v>109</v>
@@ -4302,13 +4310,13 @@
         <v>28</v>
       </c>
       <c r="B170" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C170" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D170" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4316,13 +4324,13 @@
         <v>28</v>
       </c>
       <c r="B171" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>120</v>
+        <v>257</v>
       </c>
       <c r="D171" t="s">
-        <v>123</v>
+        <v>259</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4333,10 +4341,10 @@
         <v>29</v>
       </c>
       <c r="C172" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D172" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4347,10 +4355,10 @@
         <v>29</v>
       </c>
       <c r="C173" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D173" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4361,10 +4369,10 @@
         <v>29</v>
       </c>
       <c r="C174" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D174" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4375,10 +4383,10 @@
         <v>29</v>
       </c>
       <c r="C175" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D175" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4389,10 +4397,10 @@
         <v>29</v>
       </c>
       <c r="C176" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D176" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4403,10 +4411,10 @@
         <v>29</v>
       </c>
       <c r="C177" t="s">
-        <v>220</v>
+        <v>127</v>
       </c>
       <c r="D177" t="s">
-        <v>224</v>
+        <v>51</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4414,13 +4422,13 @@
         <v>28</v>
       </c>
       <c r="B178" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C178" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D178" t="s">
-        <v>79</v>
+        <v>169</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4428,13 +4436,13 @@
         <v>28</v>
       </c>
       <c r="B179" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="C179" t="s">
-        <v>151</v>
+        <v>220</v>
       </c>
       <c r="D179" t="s">
-        <v>51</v>
+        <v>224</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4445,10 +4453,10 @@
         <v>142</v>
       </c>
       <c r="C180" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D180" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4459,10 +4467,10 @@
         <v>142</v>
       </c>
       <c r="C181" t="s">
-        <v>214</v>
+        <v>151</v>
       </c>
       <c r="D181" t="s">
-        <v>219</v>
+        <v>51</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4473,10 +4481,10 @@
         <v>142</v>
       </c>
       <c r="C182" t="s">
-        <v>217</v>
+        <v>152</v>
       </c>
       <c r="D182" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,10 +4495,10 @@
         <v>142</v>
       </c>
       <c r="C183" t="s">
-        <v>153</v>
+        <v>214</v>
       </c>
       <c r="D183" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4501,7 +4509,7 @@
         <v>142</v>
       </c>
       <c r="C184" t="s">
-        <v>154</v>
+        <v>217</v>
       </c>
       <c r="D184" t="s">
         <v>163</v>
@@ -4515,10 +4523,10 @@
         <v>142</v>
       </c>
       <c r="C185" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D185" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4529,7 +4537,7 @@
         <v>142</v>
       </c>
       <c r="C186" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D186" t="s">
         <v>163</v>
@@ -4543,10 +4551,10 @@
         <v>142</v>
       </c>
       <c r="C187" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D187" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4557,10 +4565,10 @@
         <v>142</v>
       </c>
       <c r="C188" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D188" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4571,10 +4579,10 @@
         <v>142</v>
       </c>
       <c r="C189" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D189" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4585,7 +4593,7 @@
         <v>142</v>
       </c>
       <c r="C190" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D190" t="s">
         <v>185</v>
@@ -4599,10 +4607,10 @@
         <v>142</v>
       </c>
       <c r="C191" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D191" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4613,10 +4621,10 @@
         <v>142</v>
       </c>
       <c r="C192" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="D192" t="s">
-        <v>79</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4627,10 +4635,10 @@
         <v>142</v>
       </c>
       <c r="C193" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D193" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4641,10 +4649,10 @@
         <v>142</v>
       </c>
       <c r="C194" t="s">
-        <v>171</v>
+        <v>225</v>
       </c>
       <c r="D194" t="s">
-        <v>179</v>
+        <v>79</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4655,7 +4663,7 @@
         <v>142</v>
       </c>
       <c r="C195" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D195" t="s">
         <v>179</v>
@@ -4669,10 +4677,10 @@
         <v>142</v>
       </c>
       <c r="C196" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D196" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4683,10 +4691,10 @@
         <v>142</v>
       </c>
       <c r="C197" t="s">
-        <v>226</v>
+        <v>172</v>
       </c>
       <c r="D197" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4697,10 +4705,10 @@
         <v>142</v>
       </c>
       <c r="C198" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D198" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4711,10 +4719,10 @@
         <v>142</v>
       </c>
       <c r="C199" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D199" t="s">
-        <v>186</v>
+        <v>79</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4725,7 +4733,7 @@
         <v>142</v>
       </c>
       <c r="C200" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D200" t="s">
         <v>186</v>
@@ -4739,10 +4747,10 @@
         <v>142</v>
       </c>
       <c r="C201" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D201" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4753,10 +4761,10 @@
         <v>142</v>
       </c>
       <c r="C202" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="D202" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4767,12 +4775,11 @@
         <v>142</v>
       </c>
       <c r="C203" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="D203" t="s">
-        <v>254</v>
-      </c>
-      <c r="E203" s="10"/>
+        <v>180</v>
+      </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
@@ -4782,12 +4789,11 @@
         <v>142</v>
       </c>
       <c r="C204" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D204" t="s">
-        <v>255</v>
-      </c>
-      <c r="E204" s="10"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
@@ -4797,10 +4803,10 @@
         <v>142</v>
       </c>
       <c r="C205" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D205" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E205" s="10"/>
     </row>
@@ -4812,10 +4818,10 @@
         <v>142</v>
       </c>
       <c r="C206" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D206" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E206" s="10"/>
     </row>
@@ -4827,10 +4833,10 @@
         <v>142</v>
       </c>
       <c r="C207" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D207" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E207" s="10"/>
     </row>
@@ -4842,10 +4848,10 @@
         <v>142</v>
       </c>
       <c r="C208" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D208" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E208" s="10"/>
     </row>
@@ -4857,10 +4863,10 @@
         <v>142</v>
       </c>
       <c r="C209" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D209" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E209" s="10"/>
     </row>
@@ -4872,10 +4878,10 @@
         <v>142</v>
       </c>
       <c r="C210" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D210" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E210" s="10"/>
     </row>
@@ -4887,15 +4893,45 @@
         <v>142</v>
       </c>
       <c r="C211" t="s">
+        <v>251</v>
+      </c>
+      <c r="D211" t="s">
+        <v>254</v>
+      </c>
+      <c r="E211" s="10"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>28</v>
+      </c>
+      <c r="B212" t="s">
+        <v>142</v>
+      </c>
+      <c r="C212" t="s">
+        <v>252</v>
+      </c>
+      <c r="D212" t="s">
+        <v>255</v>
+      </c>
+      <c r="E212" s="10"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>28</v>
+      </c>
+      <c r="B213" t="s">
+        <v>142</v>
+      </c>
+      <c r="C213" t="s">
         <v>253</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D213" t="s">
         <v>256</v>
       </c>
-      <c r="E211" s="10"/>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C213" t="s">
+      <c r="E213" s="10"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C215" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>